<commit_message>
Additions to msy.hpp, still not working yet
</commit_message>
<xml_diff>
--- a/examples/MSF.xlsx
+++ b/examples/MSF.xlsx
@@ -626,7 +626,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="335">
+  <cellStyleXfs count="347">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -682,6 +682,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -976,7 +988,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="52"/>
     <xf numFmtId="2" fontId="7" fillId="4" borderId="1" xfId="51" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="335">
+  <cellStyles count="347">
     <cellStyle name="20% - Accent1" xfId="52" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="53" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="54" builtinId="50"/>
@@ -1144,6 +1156,12 @@
     <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="49" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1309,6 +1327,12 @@
     <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="51" builtinId="20"/>
     <cellStyle name="Neutral" xfId="50" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1351,64 +1375,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.0003493161923391</c:v>
+                  <c:v>0.00127101626308136</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0026823732796317</c:v>
+                  <c:v>0.0344451956662112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0202816018270946</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.137437932448154</c:v>
+                  <c:v>0.965554804333789</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.550844062184243</c:v>
+                  <c:v>0.998728983736919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.904209534038349</c:v>
+                  <c:v>0.999954602131298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.986423083056256</c:v>
+                  <c:v>0.999998380405831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.998214964975444</c:v>
+                  <c:v>0.999999942222518</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.999767722839711</c:v>
+                  <c:v>0.999999997938846</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.999969815845295</c:v>
+                  <c:v>0.99999999992647</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.999996078292897</c:v>
+                  <c:v>0.999999999997377</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.999999490479845</c:v>
+                  <c:v>0.999999999999906</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.999999933801783</c:v>
+                  <c:v>0.999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.999999991399355</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.999999998882582</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.999999999854822</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.999999999981138</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.999999999997549</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.999999999999682</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.999999999999959</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,64 +1452,152 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.000335350130466478</c:v>
+                  <c:v>0.00247262315663477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00247262315663477</c:v>
+                  <c:v>0.119202922022118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0179862099620916</c:v>
+                  <c:v>0.880797077977882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.119202922022118</c:v>
+                  <c:v>0.997527376843365</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.999954602131298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.880797077977882</c:v>
+                  <c:v>0.999999168471972</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.982013790037908</c:v>
+                  <c:v>0.99999998477002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.997527376843365</c:v>
+                  <c:v>0.999999999721053</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.999664649869534</c:v>
+                  <c:v>0.999999999994891</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.999954602131298</c:v>
+                  <c:v>0.999999999999906</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.999993855825398</c:v>
+                  <c:v>0.999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.999999168471972</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.999999887464838</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.99999998477002</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.999999997938846</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.999999999721053</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.999999999962249</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.999999999994891</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.999999999999309</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.999999999999906</c:v>
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$G$3:$Z$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.252580457827647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.341247501684339</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.427643719230357</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.508367310902113</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.581557921734505</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.646462314779698</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.703062176584656</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.751788795470446</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.793319223640301</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.828438535949616</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85795164162232</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.882630331147932</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.903184345243872</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.920248190579841</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.934377843246983</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.946053327005152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1502,11 +1614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088701512"/>
-        <c:axId val="2088703304"/>
+        <c:axId val="2124285880"/>
+        <c:axId val="2124288008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2088701512"/>
+        <c:axId val="2124285880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088703304"/>
+        <c:crossAx val="2124288008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1523,7 +1635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088703304"/>
+        <c:axId val="2124288008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088701512"/>
+        <c:crossAx val="2124285880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1740,11 +1852,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2087880184"/>
-        <c:axId val="2087877192"/>
+        <c:axId val="2124376200"/>
+        <c:axId val="2124379176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2087880184"/>
+        <c:axId val="2124376200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,7 +1865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087877192"/>
+        <c:crossAx val="2124379176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1761,7 +1873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087877192"/>
+        <c:axId val="2124379176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,14 +1884,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087880184"/>
+        <c:crossAx val="2124376200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2072,8 +2183,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087829352"/>
-        <c:axId val="2087826360"/>
+        <c:axId val="2123852968"/>
+        <c:axId val="2123849976"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2336,11 +2447,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087820024"/>
-        <c:axId val="2087823320"/>
+        <c:axId val="2123843640"/>
+        <c:axId val="2123846936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087829352"/>
+        <c:axId val="2123852968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,12 +2461,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087826360"/>
+        <c:crossAx val="2123849976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087826360"/>
+        <c:axId val="2123849976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2366,12 +2477,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087829352"/>
+        <c:crossAx val="2123852968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087823320"/>
+        <c:axId val="2123846936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -2383,12 +2494,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087820024"/>
+        <c:crossAx val="2123843640"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087820024"/>
+        <c:axId val="2123843640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,7 +2509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087823320"/>
+        <c:crossAx val="2123846936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2697,8 +2808,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087768984"/>
-        <c:axId val="2087765992"/>
+        <c:axId val="2104782328"/>
+        <c:axId val="2104785320"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2961,11 +3072,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087759656"/>
-        <c:axId val="2087762952"/>
+        <c:axId val="2104791656"/>
+        <c:axId val="2104788360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087768984"/>
+        <c:axId val="2104782328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2975,12 +3086,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087765992"/>
+        <c:crossAx val="2104785320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087765992"/>
+        <c:axId val="2104785320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2991,12 +3102,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087768984"/>
+        <c:crossAx val="2104782328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087762952"/>
+        <c:axId val="2104788360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3008,12 +3119,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087759656"/>
+        <c:crossAx val="2104791656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087759656"/>
+        <c:axId val="2104791656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3023,7 +3134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087762952"/>
+        <c:crossAx val="2104788360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3712,8 +3823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3802,7 +3913,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -4170,101 +4281,101 @@
         <v>27</v>
       </c>
       <c r="B6" s="6">
-        <v>0.83668503118770632</v>
+        <v>6.6918965439920666E-2</v>
       </c>
       <c r="C6">
         <f>B6+dh</f>
-        <v>0.83678503118770631</v>
+        <v>6.7018965439920669E-2</v>
       </c>
       <c r="D6">
         <f>B6-dh</f>
-        <v>0.83658503118770633</v>
+        <v>6.6818965439920663E-2</v>
       </c>
       <c r="E6">
-        <v>4.9000000000000004</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:Z6" si="4">1/(1+EXP(-(G1-ah)/(0.1*ah)))</f>
-        <v>3.4931619233910023E-4</v>
+        <v>1.2710162630813592E-3</v>
       </c>
       <c r="H6">
         <f t="shared" si="4"/>
-        <v>2.6823732796317037E-3</v>
+        <v>3.4445195666211181E-2</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
-        <v>2.0281601827094563E-2</v>
+        <v>0.5</v>
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>0.13743793244815439</v>
+        <v>0.96555480433378871</v>
       </c>
       <c r="K6">
         <f t="shared" si="4"/>
-        <v>0.55084406218424253</v>
+        <v>0.99872898373691865</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>0.90420953403834892</v>
+        <v>0.99995460213129761</v>
       </c>
       <c r="M6">
         <f t="shared" si="4"/>
-        <v>0.98642308305625559</v>
+        <v>0.99999838040583089</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>0.99821496497544382</v>
+        <v>0.99999994222251809</v>
       </c>
       <c r="O6">
         <f t="shared" si="4"/>
-        <v>0.99976772283971149</v>
+        <v>0.99999999793884631</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
-        <v>0.99996981584529498</v>
+        <v>0.99999999992647037</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
-        <v>0.99999607829289727</v>
+        <v>0.99999999999737699</v>
       </c>
       <c r="R6">
         <f t="shared" si="4"/>
-        <v>0.99999949047984549</v>
+        <v>0.99999999999990652</v>
       </c>
       <c r="S6">
         <f t="shared" si="4"/>
-        <v>0.9999999338017832</v>
+        <v>0.99999999999999667</v>
       </c>
       <c r="T6">
         <f t="shared" si="4"/>
-        <v>0.99999999139935458</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="U6">
         <f t="shared" si="4"/>
-        <v>0.99999999888258162</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="4"/>
-        <v>0.99999999985482213</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="4"/>
-        <v>0.9999999999811382</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="4"/>
-        <v>0.99999999999754952</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="4"/>
-        <v>0.99999999999968159</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="4"/>
-        <v>0.9999999999999587</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -4272,98 +4383,98 @@
         <v>28</v>
       </c>
       <c r="B7" s="6">
-        <v>0.8807381382082371</v>
+        <v>6.066076068585366E-2</v>
       </c>
       <c r="C7">
         <f>B7</f>
-        <v>0.8807381382082371</v>
+        <v>6.066076068585366E-2</v>
       </c>
       <c r="D7">
         <f>C7</f>
-        <v>0.8807381382082371</v>
+        <v>6.066076068585366E-2</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G7">
         <f t="shared" ref="G7:Z7" si="5">1/(1+EXP(-(G1-ah)/(0.1*ah)))</f>
-        <v>3.3535013046647811E-4</v>
+        <v>2.4726231566347743E-3</v>
       </c>
       <c r="H7">
         <f t="shared" si="5"/>
-        <v>2.4726231566347743E-3</v>
+        <v>0.11920292202211755</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>1.7986209962091559E-2</v>
+        <v>0.88079707797788231</v>
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>0.11920292202211755</v>
+        <v>0.99752737684336534</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>0.99995460213129761</v>
       </c>
       <c r="L7">
         <f t="shared" si="5"/>
-        <v>0.88079707797788231</v>
+        <v>0.99999916847197223</v>
       </c>
       <c r="M7">
         <f t="shared" si="5"/>
-        <v>0.98201379003790845</v>
+        <v>0.9999999847700205</v>
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
-        <v>0.99752737684336534</v>
+        <v>0.99999999972105313</v>
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
-        <v>0.99966464986953363</v>
+        <v>0.99999999999489098</v>
       </c>
       <c r="P7">
         <f t="shared" si="5"/>
-        <v>0.99995460213129761</v>
+        <v>0.99999999999990652</v>
       </c>
       <c r="Q7">
         <f t="shared" si="5"/>
-        <v>0.99999385582539779</v>
+        <v>0.99999999999999822</v>
       </c>
       <c r="R7">
         <f t="shared" si="5"/>
-        <v>0.99999916847197223</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="5"/>
-        <v>0.99999988746483792</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="5"/>
-        <v>0.9999999847700205</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="5"/>
-        <v>0.99999999793884631</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="5"/>
-        <v>0.99999999972105313</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="5"/>
-        <v>0.99999999996224864</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="5"/>
-        <v>0.99999999999489098</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="5"/>
-        <v>0.99999999999930855</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="5"/>
-        <v>0.99999999999990652</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -4372,7 +4483,7 @@
       </c>
       <c r="B8">
         <f>4*h/(1-h)</f>
-        <v>12</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -4382,83 +4493,83 @@
       </c>
       <c r="G8">
         <f t="shared" ref="G8:Z8" si="6">m+SUMPRODUCT(fe,G6:G7)</f>
-        <v>0.30058762327883659</v>
+        <v>0.30023504629495368</v>
       </c>
       <c r="H8">
         <f t="shared" si="6"/>
-        <v>0.30442203508659083</v>
+        <v>0.3095359767841967</v>
       </c>
       <c r="I8">
         <f t="shared" si="6"/>
-        <v>0.33281045373267426</v>
+        <v>0.38688930347997585</v>
       </c>
       <c r="J8">
         <f t="shared" si="6"/>
-        <v>0.51997882040749943</v>
+        <v>0.42512469806584496</v>
       </c>
       <c r="K8">
         <f t="shared" si="6"/>
-        <v>1.2012520504523043</v>
+        <v>0.42749191716314267</v>
       </c>
       <c r="L8">
         <f t="shared" si="6"/>
-        <v>1.8322901607845929</v>
+        <v>0.42757663770624493</v>
       </c>
       <c r="M8">
         <f t="shared" si="6"/>
-        <v>1.9902224251439988</v>
+        <v>0.42757961682034601</v>
       </c>
       <c r="N8">
         <f t="shared" si="6"/>
-        <v>2.0137519237952866</v>
+        <v>0.42757972224244389</v>
       </c>
       <c r="O8">
         <f t="shared" si="6"/>
-        <v>2.0169334709232887</v>
+        <v>0.42757972598753419</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
-        <v>2.0173579311311629</v>
+        <v>0.42757972612084816</v>
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
-        <v>2.0174144767534141</v>
+        <v>0.42757972612559875</v>
       </c>
       <c r="R8">
         <f t="shared" si="6"/>
-        <v>2.0174220107296099</v>
+        <v>0.42757972612576811</v>
       </c>
       <c r="S8">
         <f t="shared" si="6"/>
-        <v>2.0174230148948773</v>
+        <v>0.42757972612577416</v>
       </c>
       <c r="T8">
         <f t="shared" si="6"/>
-        <v>2.0174231487862881</v>
+        <v>0.42757972612577433</v>
       </c>
       <c r="U8">
         <f t="shared" si="6"/>
-        <v>2.0174231666456794</v>
+        <v>0.42757972612577438</v>
       </c>
       <c r="V8">
         <f t="shared" si="6"/>
-        <v>2.0174231690287963</v>
+        <v>0.42757972612577438</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>2.0174231693469133</v>
+        <v>0.42757972612577438</v>
       </c>
       <c r="X8">
         <f t="shared" si="6"/>
-        <v>2.0174231693893931</v>
+        <v>0.42757972612577438</v>
       </c>
       <c r="Y8">
         <f t="shared" si="6"/>
-        <v>2.0174231693950677</v>
+        <v>0.42757972612577438</v>
       </c>
       <c r="Z8">
         <f t="shared" si="6"/>
-        <v>2.0174231693958262</v>
+        <v>0.42757972612577438</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -4467,83 +4578,83 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" ref="G9:Z9" si="7">EXP(-za)</f>
-        <v>0.74038302652748966</v>
+        <v>0.74064411456601276</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="7"/>
-        <v>0.73754952897821635</v>
+        <v>0.73378737161375129</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="7"/>
-        <v>0.71690606814732871</v>
+        <v>0.67916627210847402</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="7"/>
-        <v>0.59453313980647804</v>
+        <v>0.65368826638485422</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="7"/>
-        <v>0.3008173375450402</v>
+        <v>0.65214267313767105</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="7"/>
-        <v>0.16004661526344732</v>
+        <v>0.65208742559655652</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13666502432694708</v>
+        <v>0.6520854829566054</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13348690126841559</v>
+        <v>0.65208541421238941</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13306288127851906</v>
+        <v>0.65208541177027068</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13300641336531011</v>
+        <v>0.65208541168333867</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299889264753681</v>
+        <v>0.65208541168024081</v>
       </c>
       <c r="R9" s="7">
         <f t="shared" si="7"/>
-        <v>0.1329978906408201</v>
+        <v>0.65208541168013034</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299775708902473</v>
+        <v>0.65208541168012646</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773928176858</v>
+        <v>0.65208541168012635</v>
       </c>
       <c r="U9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773690650993</v>
+        <v>0.65208541168012635</v>
       </c>
       <c r="V9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773658956079</v>
+        <v>0.65208541168012635</v>
       </c>
       <c r="W9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773654725194</v>
+        <v>0.65208541168012635</v>
       </c>
       <c r="X9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773654160221</v>
+        <v>0.65208541168012635</v>
       </c>
       <c r="Y9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773654084751</v>
+        <v>0.65208541168012635</v>
       </c>
       <c r="Z9" s="7">
         <f t="shared" si="7"/>
-        <v>0.13299773654074665</v>
+        <v>0.65208541168012635</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -4552,83 +4663,83 @@
       </c>
       <c r="G10">
         <f t="shared" ref="G10:Z10" si="8">1-sa</f>
-        <v>0.25961697347251034</v>
+        <v>0.25935588543398724</v>
       </c>
       <c r="H10">
         <f t="shared" si="8"/>
-        <v>0.26245047102178365</v>
+        <v>0.26621262838624871</v>
       </c>
       <c r="I10">
         <f t="shared" si="8"/>
-        <v>0.28309393185267129</v>
+        <v>0.32083372789152598</v>
       </c>
       <c r="J10">
         <f t="shared" si="8"/>
-        <v>0.40546686019352196</v>
+        <v>0.34631173361514578</v>
       </c>
       <c r="K10">
         <f t="shared" si="8"/>
-        <v>0.69918266245495975</v>
+        <v>0.34785732686232895</v>
       </c>
       <c r="L10">
         <f t="shared" si="8"/>
-        <v>0.83995338473655268</v>
+        <v>0.34791257440344348</v>
       </c>
       <c r="M10">
         <f t="shared" si="8"/>
-        <v>0.86333497567305295</v>
+        <v>0.3479145170433946</v>
       </c>
       <c r="N10">
         <f t="shared" si="8"/>
-        <v>0.86651309873158444</v>
+        <v>0.34791458578761059</v>
       </c>
       <c r="O10">
         <f t="shared" si="8"/>
-        <v>0.86693711872148094</v>
+        <v>0.34791458822972932</v>
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>0.86699358663468984</v>
+        <v>0.34791458831666133</v>
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
-        <v>0.86700110735246316</v>
+        <v>0.34791458831975919</v>
       </c>
       <c r="R10">
         <f t="shared" si="8"/>
-        <v>0.86700210935917987</v>
+        <v>0.34791458831986966</v>
       </c>
       <c r="S10">
         <f t="shared" si="8"/>
-        <v>0.86700224291097527</v>
+        <v>0.34791458831987354</v>
       </c>
       <c r="T10">
         <f t="shared" si="8"/>
-        <v>0.86700226071823139</v>
+        <v>0.34791458831987365</v>
       </c>
       <c r="U10">
         <f t="shared" si="8"/>
-        <v>0.86700226309349004</v>
+        <v>0.34791458831987365</v>
       </c>
       <c r="V10">
         <f t="shared" si="8"/>
-        <v>0.86700226341043918</v>
+        <v>0.34791458831987365</v>
       </c>
       <c r="W10">
         <f t="shared" si="8"/>
-        <v>0.86700226345274811</v>
+        <v>0.34791458831987365</v>
       </c>
       <c r="X10">
         <f t="shared" si="8"/>
-        <v>0.86700226345839781</v>
+        <v>0.34791458831987365</v>
       </c>
       <c r="Y10">
         <f t="shared" si="8"/>
-        <v>0.86700226345915254</v>
+        <v>0.34791458831987365</v>
       </c>
       <c r="Z10">
         <f t="shared" si="8"/>
-        <v>0.86700226345925335</v>
+        <v>0.34791458831987365</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -4637,165 +4748,165 @@
       </c>
       <c r="G11">
         <f t="shared" ref="G11:Z11" si="9">wa*G6/za*(1-EXP(-za))</f>
-        <v>1.7970207722761125E-6</v>
+        <v>6.5397059436521005E-6</v>
       </c>
       <c r="H11">
         <f t="shared" si="9"/>
-        <v>8.2864422585796242E-5</v>
+        <v>1.0615092881088386E-3</v>
       </c>
       <c r="I11">
         <f t="shared" si="9"/>
-        <v>1.5845630537516199E-3</v>
+        <v>3.8083510229611359E-2</v>
       </c>
       <c r="J11">
         <f t="shared" si="9"/>
-        <v>1.7895878607042046E-2</v>
+        <v>0.13134226499213886</v>
       </c>
       <c r="K11">
         <f t="shared" si="9"/>
-        <v>8.0981334087791249E-2</v>
+        <v>0.2052677147118479</v>
       </c>
       <c r="L11">
         <f t="shared" si="9"/>
-        <v>0.14144887493689123</v>
+        <v>0.27765527047168931</v>
       </c>
       <c r="M11">
         <f t="shared" si="9"/>
-        <v>0.18298818292344909</v>
+        <v>0.34796611255761295</v>
       </c>
       <c r="N11">
         <f t="shared" si="9"/>
-        <v>0.21835887944399396</v>
+        <v>0.41365009372725131</v>
       </c>
       <c r="O11">
         <f t="shared" si="9"/>
-        <v>0.24991257677319109</v>
+        <v>0.47320411178910321</v>
       </c>
       <c r="P11">
         <f t="shared" si="9"/>
-        <v>0.27781969411126828</v>
+        <v>0.52601574946682272</v>
       </c>
       <c r="Q11">
         <f t="shared" si="9"/>
-        <v>0.30214579213221959</v>
+        <v>0.57207012583461792</v>
       </c>
       <c r="R11">
         <f t="shared" si="9"/>
-        <v>0.32308666005049214</v>
+        <v>0.61171817394034211</v>
       </c>
       <c r="S11">
         <f t="shared" si="9"/>
-        <v>0.34093469521790348</v>
+        <v>0.64551080005572448</v>
       </c>
       <c r="T11">
         <f t="shared" si="9"/>
-        <v>0.3560274788108041</v>
+        <v>0.67408680667531617</v>
       </c>
       <c r="U11">
         <f t="shared" si="9"/>
-        <v>0.36871095086952649</v>
+        <v>0.69810113519177053</v>
       </c>
       <c r="V11">
         <f t="shared" si="9"/>
-        <v>0.37931679703929472</v>
+        <v>0.71818177882839518</v>
       </c>
       <c r="W11">
         <f t="shared" si="9"/>
-        <v>0.38815003392681913</v>
+        <v>0.73490624192982434</v>
       </c>
       <c r="X11">
         <f t="shared" si="9"/>
-        <v>0.39548334542809238</v>
+        <v>0.74879081213386489</v>
       </c>
       <c r="Y11">
         <f t="shared" si="9"/>
-        <v>0.40155566631262152</v>
+        <v>0.76028787803858755</v>
       </c>
       <c r="Z11">
         <f t="shared" si="9"/>
-        <v>0.40657329027911904</v>
+        <v>0.7697880270797135</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="G12">
         <f t="shared" ref="G12:Z12" si="10">wa*G7/za*(1-EXP(-za))</f>
-        <v>1.7251738214550291E-6</v>
+        <v>1.2722282809076202E-5</v>
       </c>
       <c r="H12">
         <f t="shared" si="10"/>
-        <v>7.6384778995018047E-5</v>
+        <v>3.6735169142997561E-3</v>
       </c>
       <c r="I12">
         <f t="shared" si="10"/>
-        <v>1.4052284442777866E-3</v>
+        <v>6.7087689058764943E-2</v>
       </c>
       <c r="J12">
         <f t="shared" si="10"/>
-        <v>1.5521486565706564E-2</v>
+        <v>0.13569142267038234</v>
       </c>
       <c r="K12">
         <f t="shared" si="10"/>
-        <v>7.3506587115307026E-2</v>
+        <v>0.20551961476783867</v>
       </c>
       <c r="L12">
         <f t="shared" si="10"/>
-        <v>0.13778637698194049</v>
+        <v>0.27766764511284553</v>
       </c>
       <c r="M12">
         <f t="shared" si="10"/>
-        <v>0.18217022911512532</v>
+        <v>0.34796667082288718</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
-        <v>0.21820846998379981</v>
+        <v>0.41365011751152714</v>
       </c>
       <c r="O12">
         <f t="shared" si="10"/>
-        <v>0.249886811556947</v>
+        <v>0.47320411276203206</v>
       </c>
       <c r="P12">
         <f t="shared" si="10"/>
-        <v>0.27781546731431694</v>
+        <v>0.52601574950545138</v>
       </c>
       <c r="Q12">
         <f t="shared" si="10"/>
-        <v>0.30214512062038301</v>
+        <v>0.57207012583611749</v>
       </c>
       <c r="R12">
         <f t="shared" si="10"/>
-        <v>0.32308655601399078</v>
+        <v>0.61171817394039929</v>
       </c>
       <c r="S12">
         <f t="shared" si="10"/>
-        <v>0.34093467942003008</v>
+        <v>0.64551080005572659</v>
       </c>
       <c r="T12">
         <f t="shared" si="10"/>
-        <v>0.35602747645057903</v>
+        <v>0.6740868066753164</v>
       </c>
       <c r="U12">
         <f t="shared" si="10"/>
-        <v>0.36871095052156089</v>
+        <v>0.69810113519177053</v>
       </c>
       <c r="V12">
         <f t="shared" si="10"/>
-        <v>0.37931679698855386</v>
+        <v>0.71818177882839518</v>
       </c>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>0.38815003391948716</v>
+        <v>0.73490624192982434</v>
       </c>
       <c r="X12">
         <f t="shared" si="10"/>
-        <v>0.395483345427041</v>
+        <v>0.74879081213386489</v>
       </c>
       <c r="Y12">
         <f t="shared" si="10"/>
-        <v>0.40155566631247175</v>
+        <v>0.76028787803858755</v>
       </c>
       <c r="Z12">
         <f t="shared" si="10"/>
-        <v>0.40657329027909783</v>
+        <v>0.7697880270797135</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -4816,79 +4927,79 @@
       </c>
       <c r="H14">
         <f>G14*EXP(-m-SUMPRODUCT(G$6:G$7,$B$6:$B$7))</f>
-        <v>0.74038302652748966</v>
+        <v>0.74064411456601276</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="H14:Y14" si="11">H14*EXP(-m-SUMPRODUCT(H$6:H$7,$B$6:$B$7))</f>
-        <v>0.54606915247881627</v>
+        <f t="shared" ref="I14:Y14" si="11">H14*EXP(-m-SUMPRODUCT(H$6:H$7,$B$6:$B$7))</f>
+        <v>0.54347529812858864</v>
       </c>
       <c r="J14">
         <f t="shared" si="11"/>
-        <v>0.39148028904013227</v>
+        <v>0.36911009221303509</v>
       </c>
       <c r="K14">
         <f t="shared" si="11"/>
-        <v>0.23274800541537738</v>
+        <v>0.24128293628389258</v>
       </c>
       <c r="L14">
         <f t="shared" si="11"/>
-        <v>7.0014635307972417E-2</v>
+        <v>0.15735089905068406</v>
       </c>
       <c r="M14">
         <f t="shared" si="11"/>
-        <v>1.1205605399945636E-2</v>
+        <v>0.10260654267726421</v>
       </c>
       <c r="N14">
         <f t="shared" si="11"/>
-        <v>1.53141433458174E-3</v>
+        <v>6.6908236936211382E-2</v>
       </c>
       <c r="O14">
         <f t="shared" si="11"/>
-        <v>2.0442375408134909E-4</v>
+        <v>4.3629885396770089E-2</v>
       </c>
       <c r="P14">
         <f t="shared" si="11"/>
-        <v>2.7201213719835729E-5</v>
+        <v>2.8450411784442544E-2</v>
       </c>
       <c r="Q14">
         <f t="shared" si="11"/>
-        <v>3.6179358760586158E-6</v>
+        <v>1.8552098481018728E-2</v>
       </c>
       <c r="R14">
         <f t="shared" si="11"/>
-        <v>4.8118146518559185E-7</v>
+        <v>1.2097552775527468E-2</v>
       </c>
       <c r="S14">
         <f t="shared" si="11"/>
-        <v>6.3996119885142926E-8</v>
+        <v>7.8886376819519329E-3</v>
       </c>
       <c r="T14">
         <f t="shared" si="11"/>
-        <v>8.5113404071243431E-9</v>
+        <v>5.1440655504309844E-3</v>
       </c>
       <c r="U14">
         <f t="shared" si="11"/>
-        <v>1.1319890324051055E-9</v>
+        <v>3.3543701021623443E-3</v>
       </c>
       <c r="V14">
         <f t="shared" si="11"/>
-        <v>1.5055197951286896E-10</v>
+        <v>2.1873358089960398E-3</v>
       </c>
       <c r="W14">
         <f t="shared" si="11"/>
-        <v>2.0023072514289499E-11</v>
+        <v>1.4263297714918648E-3</v>
       </c>
       <c r="X14">
         <f t="shared" si="11"/>
-        <v>2.6630233231219963E-12</v>
+        <v>9.3008883623489321E-4</v>
       </c>
       <c r="Y14">
         <f t="shared" si="11"/>
-        <v>3.5417607433272128E-13</v>
+        <v>6.0649736167531991E-4</v>
       </c>
       <c r="Z14">
         <f>Y14*EXP(-m-SUMPRODUCT(Y$6:Y$7,$B$6:$B$7))/(1-EXP(-m-SUMPRODUCT(B$6:B$7,Z6:Z7)))</f>
-        <v>5.4330442039715243E-14</v>
+        <v>1.136739001606189E-3</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -4897,7 +5008,7 @@
       </c>
       <c r="B15">
         <f>phif/phie</f>
-        <v>0.16531088332217048</v>
+        <v>0.51908694922317566</v>
       </c>
       <c r="F15" t="s">
         <v>26</v>
@@ -4908,79 +5019,79 @@
       </c>
       <c r="H15">
         <f>G15*EXP(-m-SUMPRODUCT(G$6:G$7,$C$6:$C$7))</f>
-        <v>0.74038300066471219</v>
+        <v>0.74064402042894717</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="H15:Y15" si="12">H15*EXP(-m-SUMPRODUCT(H$6:H$7,$C$6:$C$7))</f>
-        <v>0.54606898692763139</v>
+        <f t="shared" ref="I15:Y15" si="12">H15*EXP(-m-SUMPRODUCT(H$6:H$7,$C$6:$C$7))</f>
+        <v>0.54347335704416233</v>
       </c>
       <c r="J15">
         <f t="shared" si="12"/>
-        <v>0.39147937637179459</v>
+        <v>0.36909031891664501</v>
       </c>
       <c r="K15">
         <f t="shared" si="12"/>
-        <v>0.23274426399277992</v>
+        <v>0.24124671589489541</v>
       </c>
       <c r="L15">
         <f t="shared" si="12"/>
-        <v>7.0009653276790901E-2</v>
+        <v>0.15731156624272721</v>
       </c>
       <c r="M15">
         <f t="shared" si="12"/>
-        <v>1.1203794939095554E-2</v>
+        <v>0.10257063713689357</v>
       </c>
       <c r="N15">
         <f t="shared" si="12"/>
-        <v>1.5310158775165392E-3</v>
+        <v>6.6878135317477036E-2</v>
       </c>
       <c r="O15">
         <f t="shared" si="12"/>
-        <v>2.0435016572493457E-4</v>
+        <v>4.3605895762888182E-2</v>
       </c>
       <c r="P15">
         <f t="shared" si="12"/>
-        <v>2.7188703466402603E-5</v>
+        <v>2.8431925159479992E-2</v>
       </c>
       <c r="Q15">
         <f t="shared" si="12"/>
-        <v>3.615910333921048E-6</v>
+        <v>1.8538189710904391E-2</v>
       </c>
       <c r="R15">
         <f t="shared" si="12"/>
-        <v>4.8086398171031317E-7</v>
+        <v>1.2087274281574955E-2</v>
       </c>
       <c r="S15">
         <f t="shared" si="12"/>
-        <v>6.3947500186109322E-8</v>
+        <v>7.8811470718772193E-3</v>
       </c>
       <c r="T15">
         <f t="shared" si="12"/>
-        <v>8.50402365137216E-9</v>
+        <v>5.1386671404684411E-3</v>
       </c>
       <c r="U15">
         <f t="shared" si="12"/>
-        <v>1.1309028244950087E-9</v>
+        <v>3.350514809545414E-3</v>
       </c>
       <c r="V15">
         <f t="shared" si="12"/>
-        <v>1.5039247631941348E-10</v>
+        <v>2.1846033576636342E-3</v>
       </c>
       <c r="W15">
         <f t="shared" si="12"/>
-        <v>1.9999858864692304E-11</v>
+        <v>1.4244055321643958E-3</v>
       </c>
       <c r="X15">
         <f t="shared" si="12"/>
-        <v>2.6596699799717833E-12</v>
+        <v>9.287411890781009E-4</v>
       </c>
       <c r="Y15">
         <f t="shared" si="12"/>
-        <v>3.5369471604375885E-13</v>
+        <v>6.0555802179421299E-4</v>
       </c>
       <c r="Z15">
         <f>Y15*EXP(-m-SUMPRODUCT(Y$6:Y$7,$C$6:$C$7))/(1-EXP(-m-SUMPRODUCT(C$6:C$7,Z6:Z7)))</f>
-        <v>5.425034436117285E-14</v>
+        <v>1.1346522804425844E-3</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -4993,79 +5104,79 @@
       </c>
       <c r="H16">
         <f>G16*EXP(-m-SUMPRODUCT(G$6:G$7,$D$6:$D$7))</f>
-        <v>0.74038305239026803</v>
+        <v>0.74064420870309022</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="H16:Y16" si="13">H16*EXP(-m-SUMPRODUCT(H$6:H$7,$D$6:$D$7))</f>
-        <v>0.54606931803005143</v>
+        <f t="shared" ref="I16:Y16" si="13">H16*EXP(-m-SUMPRODUCT(H$6:H$7,$D$6:$D$7))</f>
+        <v>0.54347723921994773</v>
       </c>
       <c r="J16">
         <f t="shared" si="13"/>
-        <v>0.3914812017105978</v>
+        <v>0.36912986656874103</v>
       </c>
       <c r="K16">
         <f t="shared" si="13"/>
-        <v>0.23275174689811928</v>
+        <v>0.24131916211095997</v>
       </c>
       <c r="L16">
         <f t="shared" si="13"/>
-        <v>7.0019617693685587E-2</v>
+        <v>0.15739024169307214</v>
       </c>
       <c r="M16">
         <f t="shared" si="13"/>
-        <v>1.1207416153354495E-2</v>
+        <v>0.10264246078661039</v>
       </c>
       <c r="N16">
         <f t="shared" si="13"/>
-        <v>1.5318128953480431E-3</v>
+        <v>6.6938352103580817E-2</v>
       </c>
       <c r="O16">
         <f t="shared" si="13"/>
-        <v>2.0449736893760138E-4</v>
+        <v>4.3653888228466754E-2</v>
       </c>
       <c r="P16">
         <f t="shared" si="13"/>
-        <v>2.7213729729572821E-5</v>
+        <v>2.8468910429530394E-2</v>
       </c>
       <c r="Q16">
         <f t="shared" si="13"/>
-        <v>3.6199625528540072E-6</v>
+        <v>1.8566017686557947E-2</v>
       </c>
       <c r="R16">
         <f t="shared" si="13"/>
-        <v>4.8149915827473448E-7</v>
+        <v>1.2107840009865572E-2</v>
       </c>
       <c r="S16">
         <f t="shared" si="13"/>
-        <v>6.4044776550048952E-8</v>
+        <v>7.8961354114521296E-3</v>
       </c>
       <c r="T16">
         <f t="shared" si="13"/>
-        <v>8.5186634581218063E-9</v>
+        <v>5.1494696316754648E-3</v>
       </c>
       <c r="U16">
         <f t="shared" si="13"/>
-        <v>1.1330762835946055E-9</v>
+        <v>3.3582298308979042E-3</v>
       </c>
       <c r="V16">
         <f t="shared" si="13"/>
-        <v>1.5071165187215855E-10</v>
+        <v>2.1900716780153488E-3</v>
       </c>
       <c r="W16">
         <f t="shared" si="13"/>
-        <v>2.0046313107753189E-11</v>
+        <v>1.4282566102876075E-3</v>
       </c>
       <c r="X16">
         <f t="shared" si="13"/>
-        <v>2.6663808942066385E-12</v>
+        <v>9.3143843889110839E-4</v>
       </c>
       <c r="Y16">
         <f t="shared" si="13"/>
-        <v>3.5465808772279712E-13</v>
+        <v>6.0743815865777883E-4</v>
       </c>
       <c r="Z16">
         <f>Y16*EXP(-m-SUMPRODUCT(Y$6:Y$7,$D$6:$D$7))/(1-EXP(-m-SUMPRODUCT(D$6:D$7,Z6:Z7)))</f>
-        <v>5.441065807438646E-14</v>
+        <v>1.138829621776346E-3</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -5074,7 +5185,7 @@
       </c>
       <c r="B17">
         <f>ro*(reck-phie/phif)/(reck-1)</f>
-        <v>0.54098104574874695</v>
+        <v>0.4441242822654039</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>31</v>
@@ -5084,80 +5195,80 @@
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" ref="H17:Z17" si="14">(H15-H14)/dh</f>
-        <v>-2.5862777475182952E-4</v>
+        <f t="shared" ref="H17:Y17" si="14">(H15-H14)/dh</f>
+        <v>-9.4137065587140967E-4</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.655511848719371E-3</v>
+        <v>-1.9410844263045846E-2</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="14"/>
-        <v>-9.1266833768255395E-3</v>
+        <v>-0.19773296390079853</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.7414225974585769E-2</v>
+        <v>-0.36220388997171282</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="14"/>
-        <v>-4.9820311815162999E-2</v>
+        <v>-0.39332807956843352</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.8104608500817132E-2</v>
+        <v>-0.35905540370639866</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.9845706520076976E-3</v>
+        <v>-0.30101618734346136</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="14"/>
-        <v>-7.3588356414516038E-4</v>
+        <v>-0.23989633881907335</v>
       </c>
       <c r="P17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.2510253433126184E-4</v>
+        <v>-0.18486624962552045</v>
       </c>
       <c r="Q17" s="3">
         <f t="shared" si="14"/>
-        <v>-2.0255421375677333E-5</v>
+        <v>-0.1390877011433686</v>
       </c>
       <c r="R17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.1748347527867745E-6</v>
+        <v>-0.1027849395251329</v>
       </c>
       <c r="S17" s="3">
         <f t="shared" si="14"/>
-        <v>-4.8619699033603744E-7</v>
+        <v>-7.4906100747135912E-2</v>
       </c>
       <c r="T17" s="3">
         <f t="shared" si="14"/>
-        <v>-7.3167557521830944E-8</v>
+        <v>-5.398409962543288E-2</v>
       </c>
       <c r="U17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.0862079100968683E-8</v>
+        <v>-3.8552926169303434E-2</v>
       </c>
       <c r="V17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.5950319345547635E-9</v>
+        <v>-2.7324513324055583E-2</v>
       </c>
       <c r="W17" s="3">
         <f t="shared" si="14"/>
-        <v>-2.3213649597194491E-10</v>
+        <v>-1.9242393274690201E-2</v>
       </c>
       <c r="X17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.353343150212966E-11</v>
+        <v>-1.3476471567923061E-2</v>
       </c>
       <c r="Y17" s="3">
         <f t="shared" si="14"/>
-        <v>-4.8135828896243483E-12</v>
+        <v>-9.3933988110691397E-3</v>
       </c>
       <c r="Z17" s="3">
         <f>(Z15-Z14)/dh</f>
-        <v>-8.0097678542392797E-13</v>
+        <v>-2.0867211636046296E-2</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -5177,79 +5288,79 @@
       </c>
       <c r="H18">
         <f t="shared" ref="H18:Y18" si="15">G18*EXP(-G8) - G14*G6*EXP(-G8)</f>
-        <v>-2.5862777969908171E-4</v>
+        <v>-9.4137071476889562E-4</v>
       </c>
       <c r="I18">
         <f t="shared" si="15"/>
-        <v>-1.6555121005380469E-3</v>
+        <v>-1.9410878926296116E-2</v>
       </c>
       <c r="J18">
         <f t="shared" si="15"/>
-        <v>-9.1266940162349122E-3</v>
+        <v>-0.19773826038523901</v>
       </c>
       <c r="K18">
         <f t="shared" si="15"/>
-        <v>-3.7414526695246447E-2</v>
+        <v>-0.36223107896185969</v>
       </c>
       <c r="L18">
         <f t="shared" si="15"/>
-        <v>-4.9822084431363697E-2</v>
+        <v>-0.39337724762671011</v>
       </c>
       <c r="M18">
         <f t="shared" si="15"/>
-        <v>-1.8106071215911901E-2</v>
+        <v>-0.35911824125207226</v>
       </c>
       <c r="N18">
         <f t="shared" si="15"/>
-        <v>-3.9850891125426998E-3</v>
+        <v>-0.30108392035740528</v>
       </c>
       <c r="O18">
         <f t="shared" si="15"/>
-        <v>-7.3601604743228784E-4</v>
+        <v>-0.23996231579489385</v>
       </c>
       <c r="P18">
         <f t="shared" si="15"/>
-        <v>-1.2513131143772387E-4</v>
+        <v>-0.18492633723026297</v>
       </c>
       <c r="Q18">
         <f t="shared" si="15"/>
-        <v>-2.0261093605751674E-5</v>
+        <v>-0.13913986522354255</v>
       </c>
       <c r="R18">
         <f t="shared" si="15"/>
-        <v>-3.1758825915258834E-6</v>
+        <v>-0.1028286290709227</v>
       </c>
       <c r="S18">
         <f t="shared" si="15"/>
-        <v>-4.8638177287367379E-7</v>
+        <v>-7.494168660216724E-2</v>
       </c>
       <c r="T18">
         <f t="shared" si="15"/>
-        <v>-7.3199024724870852E-8</v>
+        <v>-5.4012446110408209E-2</v>
       </c>
       <c r="U18">
         <f t="shared" si="15"/>
-        <v>-1.0867293828707376E-8</v>
+        <v>-3.8575098259918519E-2</v>
       </c>
       <c r="V18">
         <f t="shared" si="15"/>
-        <v>-1.5958774648608021E-9</v>
+        <v>-2.7341594638416331E-2</v>
       </c>
       <c r="W18">
         <f t="shared" si="15"/>
-        <v>-2.3227116321215562E-10</v>
+        <v>-1.9255384767274713E-2</v>
       </c>
       <c r="X18">
         <f t="shared" si="15"/>
-        <v>-3.3554562295485794E-11</v>
+        <v>-1.3486244339262458E-2</v>
       </c>
       <c r="Y18">
         <f t="shared" si="15"/>
-        <v>-4.8168569102756519E-12</v>
+        <v>-9.4006805536620535E-3</v>
       </c>
       <c r="Z18">
         <f>(Y18-Y14*Y6)*Y$9/oa-Y14*Y$9*Z6*sa/oa^2</f>
-        <v>-8.015682745448369E-13</v>
+        <v>-2.0886694305078016E-2</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -5258,7 +5369,7 @@
       </c>
       <c r="B19">
         <f>SUMPRODUCT(lz,fa)</f>
-        <v>8.8389878042416548E-2</v>
+        <v>0.27754997864132247</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
@@ -5268,79 +5379,79 @@
       </c>
       <c r="H19">
         <f t="shared" ref="H19:Y19" si="16">G19*EXP(-G8) - G14*G7*EXP(-G8)</f>
-        <v>-2.4828754454115959E-4</v>
+        <v>-1.831333788501182E-3</v>
       </c>
       <c r="I19">
         <f t="shared" si="16"/>
-        <v>-1.5333475930705369E-3</v>
+        <v>-6.6127653190980976E-2</v>
       </c>
       <c r="J19">
         <f t="shared" si="16"/>
-        <v>-8.1405128687474793E-3</v>
+        <v>-0.37002276237438858</v>
       </c>
       <c r="K19">
         <f t="shared" si="16"/>
-        <v>-3.2584047015824097E-2</v>
+        <v>-0.48256587256778516</v>
       </c>
       <c r="L19">
         <f t="shared" si="16"/>
-        <v>-4.4809163923728829E-2</v>
+        <v>-0.47204555375659685</v>
       </c>
       <c r="M19">
         <f t="shared" si="16"/>
-        <v>-1.7041419512023068E-2</v>
+        <v>-0.4104214272704883</v>
       </c>
       <c r="N19">
         <f t="shared" si="16"/>
-        <v>-3.8328360069973394E-3</v>
+        <v>-0.33453809053461597</v>
       </c>
       <c r="O19">
         <f t="shared" si="16"/>
-        <v>-7.155516928173234E-4</v>
+        <v>-0.26177729472068656</v>
       </c>
       <c r="P19">
         <f t="shared" si="16"/>
-        <v>-1.2240546173926078E-4</v>
+        <v>-0.19915156680434359</v>
       </c>
       <c r="Q19">
         <f t="shared" si="16"/>
-        <v>-1.989848307174451E-5</v>
+        <v>-0.14841592990800931</v>
       </c>
       <c r="R19">
         <f t="shared" si="16"/>
-        <v>-3.127654722630431E-6</v>
+        <v>-0.10887741552949746</v>
       </c>
       <c r="S19">
         <f t="shared" si="16"/>
-        <v>-4.7996754743322217E-7</v>
+        <v>-7.8886012010172896E-2</v>
       </c>
       <c r="T19">
         <f t="shared" si="16"/>
-        <v>-7.2345946733437909E-8</v>
+        <v>-5.6584483167887972E-2</v>
       </c>
       <c r="U19">
         <f t="shared" si="16"/>
-        <v>-1.0753836376911428E-8</v>
+        <v>-4.0252286103401751E-2</v>
       </c>
       <c r="V19">
         <f t="shared" si="16"/>
-        <v>-1.5807878803946801E-9</v>
+        <v>-2.8435264363799E-2</v>
       </c>
       <c r="W19">
         <f t="shared" si="16"/>
-        <v>-2.3026428262940591E-10</v>
+        <v>-1.9968550840392962E-2</v>
       </c>
       <c r="X19">
         <f t="shared" si="16"/>
-        <v>-3.328765172040915E-11</v>
+        <v>-1.395128953164807E-2</v>
       </c>
       <c r="Y19">
         <f t="shared" si="16"/>
-        <v>-4.7813584079304996E-12</v>
+        <v>-9.7039297393886875E-3</v>
       </c>
       <c r="Z19">
         <f>Y19*EXP(-Y8)/(1-EXP(-za))-Y14*Y7*EXP(-Y8)/(1-EXP(-za))-Y14*EXP(-Y8)*Z7*EXP(-za)/(1-EXP(-za))^2</f>
-        <v>-7.9612282109967989E-13</v>
+        <v>-2.1455064752178697E-2</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -5349,11 +5460,11 @@
       </c>
       <c r="B20">
         <f>B6</f>
-        <v>0.83668503118770632</v>
+        <v>6.6918965439920666E-2</v>
       </c>
       <c r="C20">
         <f>B7</f>
-        <v>0.8807381382082371</v>
+        <v>6.066076068585366E-2</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>58</v>
@@ -5363,79 +5474,79 @@
       </c>
       <c r="H20" s="4">
         <f t="shared" ref="H20:Y20" si="17">G20*EXP(-G$8)+G$14*G6^2*EXP(-G$8)</f>
-        <v>9.0342871237598882E-8</v>
+        <v>1.1964974880597898E-6</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="17"/>
-        <v>3.9956689235146171E-6</v>
+        <v>6.4569592936719101E-4</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="17"/>
-        <v>1.6389734172626811E-4</v>
+        <v>9.2716057950522707E-2</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="17"/>
-        <v>4.4938625980053262E-3</v>
+        <v>0.28555453489759308</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="17"/>
-        <v>2.2596315220589306E-2</v>
+        <v>0.34317345985957581</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="17"/>
-        <v>1.2778109386978742E-2</v>
+        <v>0.32637632462492194</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="17"/>
-        <v>3.2364334840502603E-3</v>
+        <v>0.27973328347665011</v>
       </c>
       <c r="O20" s="4">
         <f t="shared" si="17"/>
-        <v>6.3571607527242429E-4</v>
+        <v>0.22603987437998355</v>
       </c>
       <c r="P20" s="4">
         <f t="shared" si="17"/>
-        <v>1.1177879139687629E-4</v>
+        <v>0.17584771622873302</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="17"/>
-        <v>1.8485013604690162E-5</v>
+        <v>0.13321982890887876</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="17"/>
-        <v>2.9396640310858973E-6</v>
+        <v>9.8968259753481447E-2</v>
       </c>
       <c r="S20" s="4">
         <f t="shared" si="17"/>
-        <v>4.5496516999764827E-7</v>
+        <v>7.2424396086565479E-2</v>
       </c>
       <c r="T20" s="4">
         <f t="shared" si="17"/>
-        <v>6.9020686443567337E-8</v>
+        <v>5.2370957688223543E-2</v>
       </c>
       <c r="U20" s="4">
         <f t="shared" si="17"/>
-        <v>1.0311584273603702E-8</v>
+        <v>3.750470760637007E-2</v>
       </c>
       <c r="V20" s="4">
         <f t="shared" si="17"/>
-        <v>1.5219693514864602E-9</v>
+        <v>2.6643608508438631E-2</v>
       </c>
       <c r="W20" s="4">
         <f t="shared" si="17"/>
-        <v>2.224415514148566E-10</v>
+        <v>1.8800238194361187E-2</v>
       </c>
       <c r="X20" s="4">
         <f t="shared" si="17"/>
-        <v>3.2247246175256635E-11</v>
+        <v>1.3189449898889342E-2</v>
       </c>
       <c r="Y20" s="4">
         <f t="shared" si="17"/>
-        <v>4.6429868253399575E-12</v>
+        <v>9.2071452288269764E-3</v>
       </c>
       <c r="Z20" s="4">
         <f>Y20*EXP(-Y$8)/oa+2*Y$14*(Y6)*Y$9*sa/oa^2 + 2*Y$14*Y$9*Z6^2*sa^2/oa^3 +Y$14*Y$9*Z6^2*sa/oa^2</f>
-        <v>7.3979171630401916E-13</v>
+        <v>3.1634789005136561E-2</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -5444,11 +5555,11 @@
       </c>
       <c r="B21">
         <f>SUMPRODUCT(fa,G18:Z18)</f>
-        <v>-3.6746695310946972E-2</v>
+        <v>-1.1863689897094409</v>
       </c>
       <c r="C21">
         <f>SUMPRODUCT(fa,G19:Z19)</f>
-        <v>-3.326931135686502E-2</v>
+        <v>-1.3250641418892495</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>59</v>
@@ -5458,79 +5569,79 @@
       </c>
       <c r="H21" s="4">
         <f t="shared" ref="H21:Y21" si="18">G21*EXP(-G$8)+G$14*G7^2*EXP(-G$8)</f>
-        <v>8.3263260455079369E-8</v>
+        <v>4.5281983329757121E-6</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="18"/>
-        <v>3.4000040074694073E-6</v>
+        <v>7.7257461897620042E-3</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="18"/>
-        <v>1.2908282459064328E-4</v>
+        <v>0.29160396492227947</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="18"/>
-        <v>3.383938773256366E-3</v>
+        <v>0.43070929820514015</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="18"/>
-        <v>1.8521606279179512E-2</v>
+        <v>0.43822052566081882</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="18"/>
-        <v>1.1657668199913002E-2</v>
+        <v>0.38836446645863609</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="18"/>
-        <v>3.070016581475044E-3</v>
+        <v>0.32015506557205337</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="18"/>
-        <v>6.1322107838818294E-4</v>
+        <v>0.25239833391817634</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="18"/>
-        <v>1.0877993646878897E-4</v>
+        <v>0.19303568328731613</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="18"/>
-        <v>1.8086036586179228E-5</v>
+        <v>0.14442785148699938</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="18"/>
-        <v>2.8865983906225564E-6</v>
+        <v>0.1062768477705201</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="18"/>
-        <v>4.4790751053603851E-7</v>
+        <v>7.7190219712458069E-2</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="18"/>
-        <v>6.8082032776096132E-8</v>
+        <v>5.5478681749308617E-2</v>
       </c>
       <c r="U21" s="4">
         <f t="shared" si="18"/>
-        <v>1.0186745442852822E-8</v>
+        <v>3.9531209130130966E-2</v>
       </c>
       <c r="V21" s="4">
         <f t="shared" si="18"/>
-        <v>1.5053660692343759E-9</v>
+        <v>2.7965060588830658E-2</v>
       </c>
       <c r="W21" s="4">
         <f t="shared" si="18"/>
-        <v>2.2023335245001484E-10</v>
+        <v>1.9661937818219181E-2</v>
       </c>
       <c r="X21" s="4">
         <f t="shared" si="18"/>
-        <v>3.195356071098609E-11</v>
+        <v>1.3751351652857393E-2</v>
       </c>
       <c r="Y21" s="4">
         <f t="shared" si="18"/>
-        <v>4.603927323334922E-12</v>
+        <v>9.5735531653870186E-3</v>
       </c>
       <c r="Z21" s="4">
         <f>Y21*EXP(-Y$8)/oa+2*Y$14*(Y7)*Y$9*sa/oa^2 + 2*Y$14*Y$9*Z7^2*sa^2/oa^3 +Y$14*Y$9*Z7^2*sa/oa^2</f>
-        <v>7.3380000719779153E-13</v>
+        <v>3.2321535919971153E-2</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -5539,94 +5650,94 @@
       </c>
       <c r="B22">
         <f>SUMPRODUCT(fa,G20:Z20)</f>
-        <v>1.6413374352863434E-2</v>
+        <v>1.1083961420918551</v>
       </c>
       <c r="C22">
         <f>SUMPRODUCT(fa,G21:Z21)</f>
-        <v>1.4163446798239344E-2</v>
+        <v>1.2759145170604245</v>
       </c>
       <c r="F22" t="s">
         <v>44</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22:Z22" si="19">G11*G18+lz*wa*G6/za*(EXP(-za)-(1-EXP(-za))/za)</f>
-        <v>-8.5356450877766674E-7</v>
+        <v>-3.1064775182257074E-6</v>
       </c>
       <c r="H22">
         <f t="shared" si="19"/>
-        <v>-2.9143142189788449E-5</v>
+        <v>-3.7385210667271156E-4</v>
       </c>
       <c r="I22">
         <f t="shared" si="19"/>
-        <v>-4.1131006962206697E-4</v>
+        <v>-1.0422315025492327E-2</v>
       </c>
       <c r="J22">
         <f t="shared" si="19"/>
-        <v>-3.3640553998272316E-3</v>
+        <v>-4.8498924894933348E-2</v>
       </c>
       <c r="K22">
         <f t="shared" si="19"/>
-        <v>-1.0611082044176096E-2</v>
+        <v>-9.7359107693992669E-2</v>
       </c>
       <c r="L22">
         <f t="shared" si="19"/>
-        <v>-1.0565224016429122E-2</v>
+        <v>-0.12951593153214858</v>
       </c>
       <c r="M22">
         <f t="shared" si="19"/>
-        <v>-4.0188896366712057E-3</v>
+        <v>-0.14154446024006248</v>
       </c>
       <c r="N22">
         <f t="shared" si="19"/>
-        <v>-9.8472253467679063E-4</v>
+        <v>-0.13739852031421615</v>
       </c>
       <c r="O22">
         <f t="shared" si="19"/>
-        <v>-2.014279285892466E-4</v>
+        <v>-0.12314066168509601</v>
       </c>
       <c r="P22">
         <f t="shared" si="19"/>
-        <v>-3.7350615161081227E-5</v>
+        <v>-0.10422522545149836</v>
       </c>
       <c r="Q22">
         <f t="shared" si="19"/>
-        <v>-6.4959687070321502E-6</v>
+        <v>-8.4527295912452047E-2</v>
       </c>
       <c r="R22">
         <f t="shared" si="19"/>
-        <v>-1.0792976516686426E-6</v>
+        <v>-6.6339403034712585E-2</v>
       </c>
       <c r="S22">
         <f t="shared" si="19"/>
-        <v>-1.7329250726503685E-7</v>
+        <v>-5.074087547674791E-2</v>
       </c>
       <c r="T22">
         <f t="shared" si="19"/>
-        <v>-2.7098072377119118E-8</v>
+        <v>-3.8019671137637739E-2</v>
       </c>
       <c r="U22">
         <f t="shared" si="19"/>
-        <v>-4.1497509156321501E-9</v>
+        <v>-2.8016979565320021E-2</v>
       </c>
       <c r="V22">
         <f t="shared" si="19"/>
-        <v>-6.2488980765790384E-10</v>
+        <v>-2.036588333455203E-2</v>
       </c>
       <c r="W22">
         <f t="shared" si="19"/>
-        <v>-9.2816262946428491E-11</v>
+        <v>-1.4637775342914305E-2</v>
       </c>
       <c r="X22">
         <f t="shared" si="19"/>
-        <v>-1.3630755893021168E-11</v>
+        <v>-1.0421856753160142E-2</v>
       </c>
       <c r="Y22">
         <f t="shared" si="19"/>
-        <v>-1.9829160572218311E-12</v>
+        <v>-7.3613994137731748E-3</v>
       </c>
       <c r="Z22">
         <f t="shared" si="19"/>
-        <v>-3.3345702941560832E-13</v>
+        <v>-1.6484766430960765E-2</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -5635,94 +5746,94 @@
       </c>
       <c r="B23">
         <f>SUMPRODUCT(lz*G11:Z11)</f>
-        <v>3.9130858872943895E-2</v>
+        <v>0.29574480773656181</v>
       </c>
       <c r="C23">
         <f>SUMPRODUCT(lz*G12:Z12)</f>
-        <v>3.6092970528264344E-2</v>
+        <v>0.31511671637946242</v>
       </c>
       <c r="F23" t="s">
         <v>45</v>
       </c>
       <c r="G23">
         <f t="shared" ref="G23:Z23" si="20">G12*G19+lz*wa*G7/za*(EXP(-za)-(1-EXP(-za))/za)</f>
-        <v>-8.1943802107597177E-7</v>
+        <v>-6.0433123243510609E-6</v>
       </c>
       <c r="H23">
         <f t="shared" si="20"/>
-        <v>-2.686348322442814E-5</v>
+        <v>-1.2970422766037334E-3</v>
       </c>
       <c r="I23">
         <f t="shared" si="20"/>
-        <v>-3.6458794584634893E-4</v>
+        <v>-2.1494009666134926E-2</v>
       </c>
       <c r="J23">
         <f t="shared" si="20"/>
-        <v>-2.9024117601238802E-3</v>
+        <v>-7.3482406823427313E-2</v>
       </c>
       <c r="K23">
         <f t="shared" si="20"/>
-        <v>-9.2765848422944643E-3</v>
+        <v>-0.12220974508947238</v>
       </c>
       <c r="L23">
         <f t="shared" si="20"/>
-        <v>-9.6009493368125389E-3</v>
+        <v>-0.15136534715342881</v>
       </c>
       <c r="M23">
         <f t="shared" si="20"/>
-        <v>-3.8069774291694808E-3</v>
+        <v>-0.15939648617072902</v>
       </c>
       <c r="N23">
         <f t="shared" si="20"/>
-        <v>-9.5082132315812593E-4</v>
+        <v>-0.15123684963948408</v>
       </c>
       <c r="O23">
         <f t="shared" si="20"/>
-        <v>-1.9629338966545946E-4</v>
+        <v>-0.13346359968578086</v>
       </c>
       <c r="P23">
         <f t="shared" si="20"/>
-        <v>-3.6592763694545026E-5</v>
+        <v>-0.1117079202554494</v>
       </c>
       <c r="Q23">
         <f t="shared" si="20"/>
-        <v>-6.3863932663603874E-6</v>
+        <v>-8.9833855403980492E-2</v>
       </c>
       <c r="R23">
         <f t="shared" si="20"/>
-        <v>-1.0637155280607978E-6</v>
+        <v>-7.0039555641713547E-2</v>
       </c>
       <c r="S23">
         <f t="shared" si="20"/>
-        <v>-1.7110566734092272E-7</v>
+        <v>-5.3286980126549935E-2</v>
       </c>
       <c r="T23">
         <f t="shared" si="20"/>
-        <v>-2.6794352992971547E-8</v>
+        <v>-3.9753447384364871E-2</v>
       </c>
       <c r="U23">
         <f t="shared" si="20"/>
-        <v>-4.1079179068204447E-9</v>
+        <v>-2.9187826302785502E-2</v>
       </c>
       <c r="V23">
         <f t="shared" si="20"/>
-        <v>-6.1916607472673523E-10</v>
+        <v>-2.1151337003378116E-2</v>
       </c>
       <c r="W23">
         <f t="shared" si="20"/>
-        <v>-9.203729217840859E-11</v>
+        <v>-1.5161885541581486E-2</v>
       </c>
       <c r="X23">
         <f t="shared" si="20"/>
-        <v>-1.3525197205823766E-11</v>
+        <v>-1.0770078320445515E-2</v>
       </c>
       <c r="Y23">
         <f t="shared" si="20"/>
-        <v>-1.9686614324587892E-12</v>
+        <v>-7.5919560937062064E-3</v>
       </c>
       <c r="Z23">
         <f t="shared" si="20"/>
-        <v>-3.3124305349133181E-13</v>
+        <v>-1.6922291196084814E-2</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -5731,94 +5842,94 @@
       </c>
       <c r="B24">
         <f>SUM(G22:Z22)</f>
-        <v>-3.0231839492193859E-2</v>
+        <v>-1.1293980118238618</v>
       </c>
       <c r="C24">
         <f>SUM(G23:Z23)</f>
-        <v>-2.7170554555771474E-2</v>
+        <v>-1.2793586630874252</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" ref="G24:Z24" si="21">G20*G11+2*G18*wa*G6^2*sa/za - 2*G18*wa*G6^2*oa/za^2-lz*wa*G6^3*sa/za -2*lz*wa*G6^3*sa/za^2+2*lz*wa*G6^3*oa/za^3</f>
-        <v>6.766244323356963E-14</v>
+        <v>3.260302666037354E-12</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="21"/>
-        <v>1.9813600528682218E-10</v>
+        <v>3.2107691103337816E-7</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" si="21"/>
-        <v>1.6548822803315331E-7</v>
+        <v>1.9309536473984673E-3</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="21"/>
-        <v>6.194610987647251E-5</v>
+        <v>4.8974883433694327E-2</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" si="21"/>
-        <v>3.0758707444317537E-3</v>
+        <v>0.14233775921794473</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="21"/>
-        <v>9.3200262914944453E-3</v>
+        <v>0.20977466282520546</v>
       </c>
       <c r="M24" s="4">
         <f t="shared" si="21"/>
-        <v>4.962000359710346E-3</v>
+        <v>0.24030148113398078</v>
       </c>
       <c r="N24" s="4">
         <f t="shared" si="21"/>
-        <v>1.3637980331215988E-3</v>
+        <v>0.23966299496639054</v>
       </c>
       <c r="O24" s="4">
         <f t="shared" si="21"/>
-        <v>2.942708756251006E-4</v>
+        <v>0.2186056469430267</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="21"/>
-        <v>5.6257106396979328E-5</v>
+        <v>0.18732618755907987</v>
       </c>
       <c r="Q24" s="4">
         <f t="shared" si="21"/>
-        <v>9.9791740337345133E-6</v>
+        <v>0.15331970767798969</v>
       </c>
       <c r="R24" s="4">
         <f t="shared" si="21"/>
-        <v>1.6810924729326668E-6</v>
+        <v>0.12118143222433941</v>
       </c>
       <c r="S24" s="4">
         <f t="shared" si="21"/>
-        <v>2.726875771813571E-7</v>
+        <v>9.3208529888211031E-2</v>
       </c>
       <c r="T24" s="4">
         <f t="shared" si="21"/>
-        <v>4.2977014271455491E-8</v>
+        <v>7.0159312883653652E-2</v>
       </c>
       <c r="U24" s="4">
         <f t="shared" si="21"/>
-        <v>6.6225707354721173E-9</v>
+        <v>5.189671133288945E-2</v>
       </c>
       <c r="V24" s="4">
         <f t="shared" si="21"/>
-        <v>1.0023227121933395E-9</v>
+        <v>3.7844717108989331E-2</v>
       </c>
       <c r="W24" s="4">
         <f t="shared" si="21"/>
-        <v>1.4950335691442935E-10</v>
+        <v>2.7274634302425962E-2</v>
       </c>
       <c r="X24" s="4">
         <f t="shared" si="21"/>
-        <v>2.2033420776880338E-11</v>
+        <v>1.9464813985889881E-2</v>
       </c>
       <c r="Y24" s="4">
         <f t="shared" si="21"/>
-        <v>3.21497004522146E-12</v>
+        <v>1.3777071996086434E-2</v>
       </c>
       <c r="Z24" s="4">
         <f t="shared" si="21"/>
-        <v>5.279835803802328E-13</v>
+        <v>3.9549131099301672E-2</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -5827,94 +5938,94 @@
       </c>
       <c r="B25">
         <f>SUM(G24:Z24)</f>
-        <v>1.9146318938359691E-2</v>
+        <v>1.916590953306669</v>
       </c>
       <c r="C25">
         <f>SUM(G25:Z25)</f>
-        <v>1.6414960953027753E-2</v>
+        <v>2.2208481311791965</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>63</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" ref="G25:Z25" si="22">G21*G12+2*G19*wa*G7^2*sa/za - 2*G19*wa*G7^2*oa/za^2-lz*wa*G7^3*sa/za -2*lz*wa*G7^3*sa/za^2+2*lz*wa*G7^3*oa/za^3</f>
-        <v>5.9866926422720834E-14</v>
+        <v>2.4003711208157156E-11</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="22"/>
-        <v>1.5746402629849699E-10</v>
+        <v>1.2678656726648556E-5</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="22"/>
-        <v>1.1733816986536485E-7</v>
+        <v>1.2705236883303439E-2</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="22"/>
-        <v>4.088596622934149E-5</v>
+        <v>0.10099202682621122</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="22"/>
-        <v>2.2362056003787608E-3</v>
+        <v>0.19543898211556571</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="22"/>
-        <v>7.8913611583684706E-3</v>
+        <v>0.25647290124791339</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="22"/>
-        <v>4.5912797439913635E-3</v>
+        <v>0.27845537508271928</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="22"/>
-        <v>1.303346339089185E-3</v>
+        <v>0.26923864030618838</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="22"/>
-        <v>2.8510451989814867E-4</v>
+        <v>0.24066810221542509</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="22"/>
-        <v>5.4904324864408088E-5</v>
+        <v>0.20331840010459595</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="22"/>
-        <v>9.783591424014364E-6</v>
+        <v>0.16466102647798647</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="22"/>
-        <v>1.653280165890839E-6</v>
+        <v>0.12908949589369417</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="22"/>
-        <v>2.6878433046722945E-7</v>
+        <v>9.8650131848457195E-2</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="22"/>
-        <v>4.2434911951203564E-8</v>
+        <v>7.3864785171900704E-2</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="22"/>
-        <v>6.5479038883640231E-9</v>
+        <v>5.4399075837912966E-2</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="22"/>
-        <v>9.9210654327727645E-10</v>
+        <v>3.9523409390667077E-2</v>
       </c>
       <c r="W25" s="4">
         <f t="shared" si="22"/>
-        <v>1.4811298859711184E-10</v>
+        <v>2.8394776431962563E-2</v>
       </c>
       <c r="X25" s="4">
         <f t="shared" si="22"/>
-        <v>2.1845011326544307E-11</v>
+        <v>2.0209042296885419E-2</v>
       </c>
       <c r="Y25" s="4">
         <f t="shared" si="22"/>
-        <v>3.1895272693830548E-12</v>
+        <v>1.4269823808769774E-2</v>
       </c>
       <c r="Z25" s="4">
         <f t="shared" si="22"/>
-        <v>5.240319019538591E-13</v>
+        <v>4.0484220558307346E-2</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -5923,15 +6034,15 @@
       </c>
       <c r="B26">
         <f>ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-0.22862389637820754</v>
+        <v>-4.9407141524251053</v>
       </c>
       <c r="C26">
         <f>ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-0.20698894221272543</v>
+        <v>-5.5183195241023961</v>
       </c>
       <c r="G26">
         <f>G20*G11+2*G18*wa*G6^2*sa/za-2*G18*wa*G6^2*oa/za^2-lz*wa*G6^3*sa/za-2*lz*wa*G6^3*sa/za^2+2*lz*wa*G6^3*oa/za^3</f>
-        <v>6.766244323356963E-14</v>
+        <v>3.260302666037354E-12</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -5940,11 +6051,11 @@
       </c>
       <c r="B27">
         <f>-2*ro*phie*dphif^2/(phif^3*(reck-1)) + ro*phie*ddphif/(phif^2*(reck-1))</f>
-        <v>-8.7975802454849747E-2</v>
+        <v>-37.621519481832607</v>
       </c>
       <c r="C27">
         <f>-2*ro*phie*dphif^2/(phif^3*(reck-1)) + ro*phie*ddphif/(phif^2*(reck-1))</f>
-        <v>-6.7698730373253427E-2</v>
+        <v>-47.376894445986203</v>
       </c>
       <c r="G27">
         <f t="shared" ref="G27:Z27" si="23">(G15-2*G14+G16)/dh^2</f>
@@ -5952,79 +6063,79 @@
       </c>
       <c r="H27">
         <f t="shared" si="23"/>
-        <v>8.8817841970012523E-8</v>
+        <v>1.1879386363489175E-6</v>
       </c>
       <c r="I27">
         <f t="shared" si="23"/>
-        <v>5.0293103015519591E-6</v>
+        <v>6.93278767727179E-4</v>
       </c>
       <c r="J27">
         <f t="shared" si="23"/>
-        <v>2.127853448996575E-4</v>
+        <v>0.10593158572547168</v>
       </c>
       <c r="K27">
         <f t="shared" si="23"/>
-        <v>6.0144444979925993E-3</v>
+        <v>0.54380702163570049</v>
       </c>
       <c r="L27">
         <f t="shared" si="23"/>
-        <v>3.5453165403431797E-2</v>
+        <v>0.98344312415843405</v>
       </c>
       <c r="M27">
         <f t="shared" si="23"/>
-        <v>2.9255877755096638E-2</v>
+        <v>1.2568975540916405</v>
       </c>
       <c r="N27">
         <f t="shared" si="23"/>
-        <v>1.0370110239271702E-2</v>
+        <v>1.354863508884474</v>
       </c>
       <c r="O27">
         <f t="shared" si="23"/>
-        <v>2.6499837778781385E-3</v>
+        <v>1.3197814757726078</v>
       </c>
       <c r="P27">
         <f t="shared" si="23"/>
-        <v>5.7563039655239654E-4</v>
+        <v>1.2020125297884654</v>
       </c>
       <c r="Q27">
         <f t="shared" si="23"/>
-        <v>1.134657823664701E-4</v>
+        <v>1.0435424881855004</v>
       </c>
       <c r="R27">
         <f t="shared" si="23"/>
-        <v>2.0961386395798798E-5</v>
+        <v>0.87403855906359462</v>
       </c>
       <c r="S27">
         <f t="shared" si="23"/>
-        <v>3.6965872422383673E-6</v>
+        <v>0.71194254831763448</v>
       </c>
       <c r="T27">
         <f t="shared" si="23"/>
-        <v>6.2952452801661593E-7</v>
+        <v>0.56712819371251832</v>
       </c>
       <c r="U27">
         <f t="shared" si="23"/>
-        <v>1.0432794031167681E-7</v>
+        <v>0.443611862955412</v>
       </c>
       <c r="V27">
         <f t="shared" si="23"/>
-        <v>1.6916583411333011E-8</v>
+        <v>0.34176869034494017</v>
       </c>
       <c r="W27">
         <f t="shared" si="23"/>
-        <v>2.6943866495549024E-9</v>
+        <v>0.25994682736635993</v>
       </c>
       <c r="X27">
         <f t="shared" si="23"/>
-        <v>4.2279344292970485E-10</v>
+        <v>0.19554994228716469</v>
       </c>
       <c r="Y27">
         <f t="shared" si="23"/>
-        <v>6.5510111340339891E-11</v>
+        <v>0.14571013520108325</v>
       </c>
       <c r="Z27">
         <f t="shared" si="23"/>
-        <v>1.1835612882365823E-11</v>
+        <v>0.38990065523002854</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -6044,18 +6155,18 @@
       </c>
       <c r="B29">
         <f>f*re*phiq</f>
-        <v>1.7711829731141989E-2</v>
+        <v>8.7896354986049096E-3</v>
       </c>
       <c r="C29">
         <f>f*re*phiq</f>
-        <v>1.7196951988642725E-2</v>
+        <v>8.489533238671073E-3</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
         <f>B29</f>
-        <v>1.7711829731141989E-2</v>
+        <v>8.7896354986049096E-3</v>
       </c>
       <c r="H29">
         <f>B30</f>
@@ -6079,14 +6190,14 @@
       </c>
       <c r="G30">
         <f t="dataTable" ref="G30:H56" dt2D="0" dtr="0" r1="B6"/>
-        <v>8.6019778280879821E-3</v>
+        <v>-1.2410657063575687E-2</v>
       </c>
       <c r="H30">
-        <v>3.0956414063514761E-2</v>
+        <v>-0.28067040911637747</v>
       </c>
       <c r="Z30" s="4">
         <f>Y30*EXP(-Y$8)/oa+Y$14*(Y16)^2*Y$9/oa + 2*Y$14*Y16*Y$9*Z16*sa/oa^2 + 2*Y$14*Y$9*Z16^2*sa/oa^3 + Y$14*Y$9*Z16^2*sa/oa^2</f>
-        <v>7.2370579058249841E-39</v>
+        <v>2.2014599919549701E-8</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -6097,10 +6208,10 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="G31">
-        <v>8.7617691891247462E-3</v>
+        <v>-1.3833745692980657E-2</v>
       </c>
       <c r="H31">
-        <v>3.0488580079952032E-2</v>
+        <v>-0.28775712485387883</v>
       </c>
     </row>
     <row r="32" spans="1:26">
@@ -6110,22 +6221,22 @@
       </c>
       <c r="C32">
         <f>f*phiq*B26+f*re*B24</f>
-        <v>-2.1671942621530244E-2</v>
+        <v>-0.12486985447140397</v>
       </c>
       <c r="F32">
         <v>0.21</v>
       </c>
       <c r="G32">
-        <v>8.9193648362413704E-3</v>
+        <v>-1.5292157315700194E-2</v>
       </c>
       <c r="H32">
-        <v>3.0026867119453082E-2</v>
+        <v>-0.29470427186923637</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="B33">
         <f>f*phiq*C26+f*re*C24</f>
-        <v>-1.9075088468176422E-2</v>
+        <v>-0.14723568290856329</v>
       </c>
       <c r="C33">
         <f>re*phiq+f*phiq*dre+f*re*dphiq</f>
@@ -6135,10 +6246,10 @@
         <v>0.215</v>
       </c>
       <c r="G33">
-        <v>9.0747940489639325E-3</v>
+        <v>-1.6785223428318247E-2</v>
       </c>
       <c r="H33">
-        <v>2.957117446688972E-2</v>
+        <v>-0.30151929018151807</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -6150,21 +6261,21 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>52.424396440851737</v>
+        <v>6.7918318456879962</v>
       </c>
       <c r="F34">
         <v>0.22</v>
       </c>
       <c r="G34">
-        <v>9.2280856152883398E-3</v>
+        <v>-1.8312311889668711E-2</v>
       </c>
       <c r="H34">
-        <v>2.9121403422145677E-2</v>
+        <v>-0.30820925036421792</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35">
-        <v>46.14261016945192</v>
+        <v>8.008337995052333</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -6173,10 +6284,10 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="G35">
-        <v>9.3792678415793203E-3</v>
+        <v>-1.9872825127943868E-2</v>
       </c>
       <c r="H35">
-        <v>2.8677457252874319E-2</v>
+        <v>-0.31478087482349798</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -6184,10 +6295,10 @@
         <v>0.23</v>
       </c>
       <c r="G36">
-        <v>9.528368562236952E-3</v>
+        <v>-2.1466198450753867E-2</v>
       </c>
       <c r="H36">
-        <v>2.823924114852322E-2</v>
+        <v>-0.32124055771350479</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -6205,10 +6316,10 @@
         <v>0.23499999999999999</v>
       </c>
       <c r="G37">
-        <v>9.6754151491369664E-3</v>
+        <v>-2.3091898451568477E-2</v>
       </c>
       <c r="H37">
-        <v>2.780666217558718E-2</v>
+        <v>-0.32759438358539661</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -6217,20 +6328,20 @@
       </c>
       <c r="B38">
         <f>f+delta</f>
-        <v>0.83668503118770632</v>
+        <v>6.6918965439920666E-2</v>
       </c>
       <c r="C38">
         <f>f+delta</f>
-        <v>0.8807381382082371</v>
+        <v>6.066076068585366E-2</v>
       </c>
       <c r="F38">
         <v>0.24</v>
       </c>
       <c r="G38">
-        <v>9.8204345208507873E-3</v>
+        <v>-2.4749421506435342E-2</v>
       </c>
       <c r="H38">
-        <v>2.737962923405303E-2</v>
+        <v>-0.33384814485918551</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -6238,10 +6349,10 @@
         <v>0.245</v>
       </c>
       <c r="G39">
-        <v>9.9634531516513431E-3</v>
+        <v>-2.6438292355296156E-2</v>
       </c>
       <c r="H39">
-        <v>2.6958053015000642E-2</v>
+        <v>-0.34000735820062922</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -6250,39 +6361,39 @@
       </c>
       <c r="B40">
         <f>2*dre*phiq+2*re*dphiq+f*ddre*phiq+2*f*dre*dphiq+f*re*ddphiq</f>
-        <v>-3.3250469374861646E-2</v>
+        <v>-3.8663506163859971</v>
       </c>
       <c r="C40">
         <f>f*B27*phiq+2*f*B26*B24+f*re*B25</f>
-        <v>1.8500723217216748E-2</v>
+        <v>9.4691677147146561E-3</v>
       </c>
       <c r="F40">
         <v>0.25</v>
       </c>
       <c r="G40">
-        <v>1.0104497080310157E-2</v>
+        <v>-2.8158062762619358E-2</v>
       </c>
       <c r="H40">
-        <v>2.6541845959325322E-2</v>
+        <v>-0.34607727987910963</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="B41">
         <f>f*C27*phiq+2*f*C26*C24+f*re*C25</f>
-        <v>1.4624486244745702E-2</v>
+        <v>7.3254974939620229E-2</v>
       </c>
       <c r="C41">
         <f>2*dre*phiq+2*re*dphiq+f*ddre*phiq+2*f*dre*dphiq+f*re*ddphiq</f>
-        <v>-2.8763573854503982E-2</v>
+        <v>-4.6034870065564508</v>
       </c>
       <c r="F41">
         <v>0.255</v>
       </c>
       <c r="G41">
-        <v>1.0243591918691314E-2</v>
+        <v>-2.9908310252431649E-2</v>
       </c>
       <c r="H41">
-        <v>2.6130922217548428E-2</v>
+        <v>-0.35206292017666346</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -6291,36 +6402,36 @@
       </c>
       <c r="B42">
         <f t="array" ref="B42:C43">-MINVERSE(B40:C41)</f>
-        <v>41.93926555222739</v>
+        <v>0.25865191066892274</v>
       </c>
       <c r="C42">
-        <v>26.975324688090367</v>
+        <v>5.3203545885263887E-4</v>
       </c>
       <c r="F42">
         <v>0.26</v>
       </c>
       <c r="G42">
-        <v>1.038076286014772E-2</v>
+        <v>-3.1688636913167798E-2</v>
       </c>
       <c r="H42">
-        <v>2.5725197610684029E-2</v>
+        <v>-0.35796905691302222</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="B43">
-        <v>21.323505044462546</v>
+        <v>4.1159102235220953E-3</v>
       </c>
       <c r="C43">
-        <v>48.481467285754796</v>
+        <v>0.2172351030468673</v>
       </c>
       <c r="F43">
         <v>0.26500000000000001</v>
       </c>
       <c r="G43">
-        <v>1.0516034687724721E-2</v>
+        <v>-3.3498668268071463E-2</v>
       </c>
       <c r="H43">
-        <v>2.5324589592130332E-2</v>
+        <v>-0.36380024814667555</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -6328,10 +6439,10 @@
         <v>0.27</v>
       </c>
       <c r="G44">
-        <v>1.0649431782176177E-2</v>
+        <v>-3.5338052207167091E-2</v>
       </c>
       <c r="H44">
-        <v>2.4929017210555415E-2</v>
+        <v>-0.36956084410749035</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -6349,10 +6460,10 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="G45">
-        <v>1.0780978129798001E-2</v>
+        <v>-3.7206457977091136E-2</v>
       </c>
       <c r="H45">
-        <v>2.4538401073748925E-2</v>
+        <v>-0.37525499841232801</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -6361,20 +6472,20 @@
       </c>
       <c r="B46" s="5">
         <f>f+dta</f>
-        <v>0.83668503118770632</v>
+        <v>6.6918965439920666E-2</v>
       </c>
       <c r="C46" s="5">
         <f>f+dta</f>
-        <v>0.8807381382082371</v>
+        <v>6.066076068585366E-2</v>
       </c>
       <c r="F46">
         <v>0.28000000000000003</v>
       </c>
       <c r="G46">
-        <v>1.0910697330083647E-2</v>
+        <v>-3.91035752253188E-2</v>
       </c>
       <c r="H46">
-        <v>2.4152663313410299E-2</v>
+        <v>-0.38088667861132164</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -6382,10 +6493,10 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="G47">
-        <v>1.1038612603206476E-2</v>
+        <v>-4.1029113095549699E-2</v>
       </c>
       <c r="H47">
-        <v>2.377172755084743E-2</v>
+        <v>-0.38645967610899984</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -6393,10 +6504,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G48">
-        <v>1.1164746797333239E-2</v>
+        <v>-4.2982799371232706E-2</v>
       </c>
       <c r="H48">
-        <v>2.3395518863558347E-2</v>
+        <v>-0.39197761550125709</v>
       </c>
     </row>
     <row r="49" spans="6:8">
@@ -6404,10 +6515,10 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="G49">
-        <v>1.1289122395773087E-2</v>
+        <v>-4.496437966440376E-2</v>
       </c>
       <c r="H49">
-        <v>2.3023963752670906E-2</v>
+        <v>-0.3974439633662179</v>
       </c>
     </row>
     <row r="50" spans="6:8">
@@ -6415,10 +6526,10 @@
         <v>0.29999999999999899</v>
       </c>
       <c r="G50">
-        <v>1.1411761523966425E-2</v>
+        <v>-4.6973616647195529E-2</v>
       </c>
       <c r="H50">
-        <v>2.2656990111215754E-2</v>
+        <v>-0.40286203654432179</v>
       </c>
     </row>
     <row r="51" spans="6:8">
@@ -6426,10 +6537,10 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="G51">
-        <v>1.1532685956317679E-2</v>
+        <v>-4.9010289323551323E-2</v>
       </c>
       <c r="H51">
-        <v>2.229452719320767E-2</v>
+        <v>-0.40823500994047074</v>
       </c>
     </row>
     <row r="52" spans="6:8">
@@ -6437,10 +6548,10 @@
         <v>0.309999999999999</v>
       </c>
       <c r="G52">
-        <v>1.1651917122875555E-2</v>
+        <v>-5.107419233882169E-2</v>
       </c>
       <c r="H52">
-        <v>2.1936505583514256E-2</v>
+        <v>-0.41356592387873292</v>
       </c>
     </row>
     <row r="53" spans="6:8">
@@ -6448,10 +6559,10 @@
         <v>0.314999999999999</v>
       </c>
       <c r="G53">
-        <v>1.1769476115865676E-2</v>
+        <v>-5.3165135325094239E-2</v>
       </c>
       <c r="H53">
-        <v>2.1582857168486146E-2</v>
+        <v>-0.41885769103802228</v>
       </c>
     </row>
     <row r="54" spans="6:8">
@@ -6459,10 +6570,10 @@
         <v>0.31999999999999901</v>
       </c>
       <c r="G54">
-        <v>1.1885383696078014E-2</v>
+        <v>-5.5282942280209101E-2</v>
       </c>
       <c r="H54">
-        <v>2.1233515107330739E-2</v>
+        <v>-0.42411310299512239</v>
       </c>
     </row>
     <row r="55" spans="6:8">
@@ -6470,10 +6581,10 @@
         <v>0.32499999999999901</v>
       </c>
       <c r="G55">
-        <v>1.1999660299113906E-2</v>
+        <v>-5.7427450978574948E-2</v>
       </c>
       <c r="H55">
-        <v>2.0888413804205488E-2</v>
+        <v>-0.42933483639967562</v>
       </c>
     </row>
     <row r="56" spans="6:8">
@@ -6481,10 +6592,10 @@
         <v>0.32999999999999902</v>
       </c>
       <c r="G56">
-        <v>1.2112326041495529E-2</v>
+        <v>-5.9598512411994417E-2</v>
       </c>
       <c r="H56">
-        <v>2.054748888101169E-2</v>
+        <v>-0.43452545880402149</v>
       </c>
     </row>
   </sheetData>
@@ -8107,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:Y19" si="16">G19*EXP(-G8) - G14*G7*EXP(-G8)</f>
+        <f t="shared" ref="H19:X19" si="16">G19*EXP(-G8) - G14*G7*EXP(-G8)</f>
         <v>-0.12430300293711437</v>
       </c>
       <c r="I19">

</xml_diff>

<commit_message>
About to work on MSY.hpp for multiple fleets with allocation; chaning dphiq to a matrix
</commit_message>
<xml_diff>
--- a/examples/MSF.xlsx
+++ b/examples/MSF.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Allocation(2)" sheetId="7" r:id="rId3"/>
+    <sheet name="Allocation Mar" sheetId="8" r:id="rId3"/>
     <sheet name="Allocation" sheetId="3" r:id="rId4"/>
     <sheet name="SingleFleet" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
@@ -20,30 +20,31 @@
     <definedName name="age" localSheetId="5">Sheet5!$G$1:$M$1</definedName>
     <definedName name="age">SingleFleet!$F$1:$L$1</definedName>
     <definedName name="ah" localSheetId="3">Allocation!$E$6:$E$7</definedName>
-    <definedName name="ah" localSheetId="2">'Allocation(2)'!$E$6:$E$7</definedName>
+    <definedName name="ah" localSheetId="2">'Allocation Mar'!$E$6:$E$7</definedName>
     <definedName name="ah">Sheet2!$E$6:$E$7</definedName>
-    <definedName name="ak" localSheetId="2">'Allocation(2)'!$B$12:$C$12</definedName>
+    <definedName name="ak" localSheetId="2">'Allocation Mar'!$B$10:$C$10</definedName>
     <definedName name="ak">Allocation!$B$9:$C$9</definedName>
+    <definedName name="akdYe">'Allocation Mar'!$B$31:$C$31</definedName>
     <definedName name="B">Sheet1!$B$1</definedName>
     <definedName name="beta">FlakLake!$B$15</definedName>
     <definedName name="ca">Sheet5!$G$6:$M$6</definedName>
     <definedName name="Ct">Sheet5!$B$2</definedName>
     <definedName name="ddphif" localSheetId="3">Allocation!$B$22:$C$22</definedName>
-    <definedName name="ddphif" localSheetId="2">'Allocation(2)'!$B$25:$C$25</definedName>
+    <definedName name="ddphif" localSheetId="2">'Allocation Mar'!$B$22:$C$22</definedName>
     <definedName name="ddphif">Sheet2!$B$22:$C$22</definedName>
     <definedName name="ddphiq" localSheetId="3">Allocation!$B$25:$C$25</definedName>
-    <definedName name="ddphiq" localSheetId="2">'Allocation(2)'!$B$28:$C$28</definedName>
+    <definedName name="ddphiq" localSheetId="2">'Allocation Mar'!$B$25:$C$25</definedName>
     <definedName name="ddphiq">Sheet2!$B$25:$C$25</definedName>
     <definedName name="ddre" localSheetId="3">Allocation!$B$27:$C$27</definedName>
-    <definedName name="ddre" localSheetId="2">'Allocation(2)'!$B$30:$C$30</definedName>
+    <definedName name="ddre" localSheetId="2">'Allocation Mar'!$B$27:$C$27</definedName>
     <definedName name="ddre">Sheet2!$B$27:$C$27</definedName>
     <definedName name="delta" localSheetId="3">Allocation!$B$39:$C$39</definedName>
-    <definedName name="delta" localSheetId="2">'Allocation(2)'!#REF!</definedName>
+    <definedName name="delta" localSheetId="2">'Allocation Mar'!$B$37:$C$37</definedName>
     <definedName name="delta">Sheet2!$B$37:$C$37</definedName>
     <definedName name="dfe" localSheetId="6">FlakLake!$B$22</definedName>
     <definedName name="dfe">SingleFleet!$B$19</definedName>
     <definedName name="dh" localSheetId="3">Allocation!$B$14</definedName>
-    <definedName name="dh" localSheetId="2">'Allocation(2)'!$B$17</definedName>
+    <definedName name="dh" localSheetId="2">'Allocation Mar'!$B$13</definedName>
     <definedName name="dh" localSheetId="6">FlakLake!$B$6</definedName>
     <definedName name="dh" localSheetId="4">SingleFleet!$B$6</definedName>
     <definedName name="dh">Sheet2!$B$13</definedName>
@@ -52,43 +53,43 @@
     <definedName name="dlz" localSheetId="6">FlakLake!$F$15:$L$15</definedName>
     <definedName name="dlz">SingleFleet!$F$13:$L$13</definedName>
     <definedName name="dphif" localSheetId="3">Allocation!$B$21:$C$21</definedName>
-    <definedName name="dphif" localSheetId="2">'Allocation(2)'!$B$24:$C$24</definedName>
+    <definedName name="dphif" localSheetId="2">'Allocation Mar'!$B$21:$C$21</definedName>
     <definedName name="dphif" localSheetId="6">FlakLake!$B$16</definedName>
     <definedName name="dphif" localSheetId="4">SingleFleet!$B$15</definedName>
     <definedName name="dphif">Sheet2!$B$21:$C$21</definedName>
     <definedName name="dphiq" localSheetId="3">Allocation!$B$24:$C$24</definedName>
-    <definedName name="dphiq" localSheetId="2">'Allocation(2)'!$B$27:$C$27</definedName>
+    <definedName name="dphiq" localSheetId="2">'Allocation Mar'!$B$24:$C$24</definedName>
     <definedName name="dphiq" localSheetId="6">FlakLake!$B$17</definedName>
     <definedName name="dphiq" localSheetId="4">SingleFleet!$B$16</definedName>
     <definedName name="dphiq">Sheet2!$B$24:$C$24</definedName>
     <definedName name="dqa" localSheetId="6">FlakLake!$F$20:$L$20</definedName>
     <definedName name="dqa">SingleFleet!$F$17:$L$17</definedName>
     <definedName name="dre" localSheetId="3">Allocation!$B$26:$C$26</definedName>
-    <definedName name="dre" localSheetId="2">'Allocation(2)'!$B$29:$C$29</definedName>
+    <definedName name="dre" localSheetId="2">'Allocation Mar'!$B$26:$C$26</definedName>
     <definedName name="dre" localSheetId="6">FlakLake!$B$18</definedName>
     <definedName name="dre" localSheetId="4">SingleFleet!$B$17</definedName>
     <definedName name="dre">Sheet2!$B$26:$C$26</definedName>
     <definedName name="dta" localSheetId="3">Allocation!$B$47:$C$47</definedName>
-    <definedName name="dta" localSheetId="2">'Allocation(2)'!$B$41:$C$41</definedName>
+    <definedName name="dta" localSheetId="2">'Allocation Mar'!$B$45:$C$45</definedName>
     <definedName name="dta">Sheet2!$B$45:$C$45</definedName>
-    <definedName name="dYe" localSheetId="2">'Allocation(2)'!$B$33:$C$33</definedName>
+    <definedName name="dYe" localSheetId="2">'Allocation Mar'!$B$30:$C$30</definedName>
     <definedName name="dye" localSheetId="6">FlakLake!$B$24</definedName>
     <definedName name="dye" localSheetId="4">SingleFleet!$B$21</definedName>
     <definedName name="dYe">Allocation!$B$30:$C$30</definedName>
     <definedName name="f" localSheetId="3">Allocation!$B$20:$C$20</definedName>
-    <definedName name="f" localSheetId="2">'Allocation(2)'!$B$23:$C$23</definedName>
+    <definedName name="f" localSheetId="2">'Allocation Mar'!$B$20:$C$20</definedName>
     <definedName name="f">Sheet2!$B$20:$C$20</definedName>
     <definedName name="f_1">Sheet1!$B$3</definedName>
     <definedName name="f_2">Sheet1!$B$4</definedName>
     <definedName name="fa" localSheetId="3">Allocation!$G$3:$Z$3</definedName>
-    <definedName name="fa" localSheetId="2">'Allocation(2)'!$G$3:$Z$3</definedName>
+    <definedName name="fa" localSheetId="2">'Allocation Mar'!$G$3:$Z$3</definedName>
     <definedName name="fa" localSheetId="6">FlakLake!$F$3:$L$3</definedName>
     <definedName name="fa" localSheetId="4">SingleFleet!$F$3:$L$3</definedName>
     <definedName name="fa">Sheet2!$G$3:$Z$3</definedName>
-    <definedName name="favg">'Allocation(2)'!$D$23</definedName>
-    <definedName name="fbar">'Allocation(2)'!$D$42</definedName>
+    <definedName name="favg">#REF!</definedName>
+    <definedName name="fbar">Allocation!$D$48</definedName>
     <definedName name="fe" localSheetId="3">Allocation!$B$6:$B$7</definedName>
-    <definedName name="fe" localSheetId="2">'Allocation(2)'!$B$6:$B$7</definedName>
+    <definedName name="fe" localSheetId="2">'Allocation Mar'!$B$6:$B$7</definedName>
     <definedName name="fe" localSheetId="6">FlakLake!$B$4</definedName>
     <definedName name="fe" localSheetId="4">SingleFleet!$B$4</definedName>
     <definedName name="fe">Sheet2!$B$6:$B$7</definedName>
@@ -97,32 +98,32 @@
     <definedName name="fem" localSheetId="6">FlakLake!$B$8</definedName>
     <definedName name="fem">SingleFleet!$B$8</definedName>
     <definedName name="fiter" localSheetId="3">Allocation!$B$40:$C$40</definedName>
-    <definedName name="fiter" localSheetId="2">'Allocation(2)'!#REF!</definedName>
+    <definedName name="fiter" localSheetId="2">'Allocation Mar'!$B$38:$C$38</definedName>
     <definedName name="fiter">Sheet2!$B$38:$C$38</definedName>
+    <definedName name="fstp">'Allocation Mar'!$B$36:$C$36</definedName>
     <definedName name="ft">Sheet5!$B$3</definedName>
     <definedName name="h" localSheetId="3">Allocation!$B$2</definedName>
-    <definedName name="h" localSheetId="2">'Allocation(2)'!$B$2</definedName>
+    <definedName name="h" localSheetId="2">'Allocation Mar'!$B$2</definedName>
     <definedName name="h" localSheetId="6">FlakLake!$B$2</definedName>
     <definedName name="h" localSheetId="4">SingleFleet!$B$2</definedName>
     <definedName name="h">Sheet2!$B$2</definedName>
     <definedName name="kappa" localSheetId="6">FlakLake!$B$5</definedName>
     <definedName name="kappa">SingleFleet!$B$5</definedName>
-    <definedName name="lambda" localSheetId="2">'Allocation(2)'!$B$14:$C$14</definedName>
     <definedName name="lambda">Allocation!$B$11:$C$11</definedName>
     <definedName name="lw">FlakLake!$F$10:$L$10</definedName>
     <definedName name="lx" localSheetId="3">Allocation!$G$4:$Z$4</definedName>
-    <definedName name="lx" localSheetId="2">'Allocation(2)'!$G$4:$Z$4</definedName>
+    <definedName name="lx" localSheetId="2">'Allocation Mar'!$G$4:$Z$4</definedName>
     <definedName name="lx" localSheetId="6">FlakLake!$F$8:$L$8</definedName>
     <definedName name="lx" localSheetId="4">SingleFleet!$F$8:$L$8</definedName>
     <definedName name="lx">Sheet2!$G$4:$Z$4</definedName>
     <definedName name="lYe">Allocation!$B$31:$C$31</definedName>
     <definedName name="lz" localSheetId="3">Allocation!$G$14:$Z$14</definedName>
-    <definedName name="lz" localSheetId="2">'Allocation(2)'!$G$14:$Z$14</definedName>
+    <definedName name="lz" localSheetId="2">'Allocation Mar'!$G$14:$Z$14</definedName>
     <definedName name="lz" localSheetId="6">FlakLake!$F$9:$L$9</definedName>
     <definedName name="lz" localSheetId="4">SingleFleet!$F$9:$L$9</definedName>
     <definedName name="lz">Sheet2!$G$14:$Z$14</definedName>
     <definedName name="m" localSheetId="3">Allocation!$B$3</definedName>
-    <definedName name="m" localSheetId="2">'Allocation(2)'!$B$3</definedName>
+    <definedName name="m" localSheetId="2">'Allocation Mar'!$B$3</definedName>
     <definedName name="m" localSheetId="6">FlakLake!$B$3</definedName>
     <definedName name="m" localSheetId="1">Sheet2!$B$3</definedName>
     <definedName name="m" localSheetId="5">Sheet5!$B$1</definedName>
@@ -130,7 +131,7 @@
     <definedName name="M">Sheet1!$B$2</definedName>
     <definedName name="na">Sheet5!$G$3:$M$3</definedName>
     <definedName name="oa" localSheetId="3">Allocation!$G$10:$Z$10</definedName>
-    <definedName name="oa" localSheetId="2">'Allocation(2)'!$G$10:$Z$10</definedName>
+    <definedName name="oa" localSheetId="2">'Allocation Mar'!$G$10:$Z$10</definedName>
     <definedName name="oa" localSheetId="6">FlakLake!$F$7:$L$7</definedName>
     <definedName name="oa" localSheetId="4">SingleFleet!$F$7:$L$7</definedName>
     <definedName name="oa">Sheet2!$G$10:$Z$10</definedName>
@@ -139,67 +140,66 @@
     <definedName name="phef" localSheetId="6">FlakLake!$B$11</definedName>
     <definedName name="phef">SingleFleet!$B$11</definedName>
     <definedName name="phie" localSheetId="3">Allocation!$B$18</definedName>
-    <definedName name="phie" localSheetId="2">'Allocation(2)'!$B$21</definedName>
+    <definedName name="phie" localSheetId="2">'Allocation Mar'!$B$18</definedName>
     <definedName name="phie" localSheetId="6">FlakLake!$B$10</definedName>
     <definedName name="phie" localSheetId="4">SingleFleet!$B$10</definedName>
     <definedName name="phie">Sheet2!$B$18</definedName>
     <definedName name="phif" localSheetId="3">Allocation!$B$19</definedName>
-    <definedName name="phif" localSheetId="2">'Allocation(2)'!$B$22</definedName>
+    <definedName name="phif" localSheetId="2">'Allocation Mar'!$B$19</definedName>
     <definedName name="phif" localSheetId="6">FlakLake!$B$11</definedName>
     <definedName name="phif" localSheetId="4">SingleFleet!$B$11</definedName>
     <definedName name="phif">Sheet2!$B$19</definedName>
     <definedName name="phiq" localSheetId="3">Allocation!$B$23:$C$23</definedName>
-    <definedName name="phiq" localSheetId="2">'Allocation(2)'!$B$26:$C$26</definedName>
+    <definedName name="phiq" localSheetId="2">'Allocation Mar'!$B$23:$C$23</definedName>
     <definedName name="phiq" localSheetId="6">FlakLake!$B$13</definedName>
     <definedName name="phiq" localSheetId="4">SingleFleet!$B$13</definedName>
     <definedName name="phiq">Sheet2!$B$23:$C$23</definedName>
-    <definedName name="pk" localSheetId="2">'Allocation(2)'!$B$13:$C$13</definedName>
     <definedName name="pk">Allocation!$B$10:$C$10</definedName>
-    <definedName name="plambda">'Allocation(2)'!$B$15:$C$15</definedName>
+    <definedName name="plambda">#REF!</definedName>
     <definedName name="qa" localSheetId="6">FlakLake!$F$19:$L$19</definedName>
     <definedName name="qa">SingleFleet!$F$16:$L$16</definedName>
     <definedName name="re" localSheetId="3">Allocation!$B$17</definedName>
-    <definedName name="re" localSheetId="2">'Allocation(2)'!$B$20</definedName>
+    <definedName name="re" localSheetId="2">'Allocation Mar'!$B$17</definedName>
     <definedName name="re" localSheetId="6">FlakLake!$B$12</definedName>
     <definedName name="re" localSheetId="4">SingleFleet!$B$12</definedName>
     <definedName name="re">Sheet2!$B$17</definedName>
     <definedName name="reck" localSheetId="3">Allocation!$B$8</definedName>
-    <definedName name="reck" localSheetId="2">'Allocation(2)'!$B$8</definedName>
+    <definedName name="reck" localSheetId="2">'Allocation Mar'!$B$8</definedName>
     <definedName name="reck">Sheet2!$B$8</definedName>
     <definedName name="ro" localSheetId="3">Allocation!$B$1</definedName>
-    <definedName name="ro" localSheetId="2">'Allocation(2)'!$B$1</definedName>
+    <definedName name="ro" localSheetId="2">'Allocation Mar'!$B$1</definedName>
     <definedName name="ro" localSheetId="6">FlakLake!$B$1</definedName>
     <definedName name="ro" localSheetId="4">SingleFleet!$B$1</definedName>
     <definedName name="ro">Sheet2!$B$1</definedName>
     <definedName name="sa" localSheetId="3">Allocation!$G$9:$Z$9</definedName>
-    <definedName name="sa" localSheetId="2">'Allocation(2)'!$G$9:$Z$9</definedName>
+    <definedName name="sa" localSheetId="2">'Allocation Mar'!$G$9:$Z$9</definedName>
     <definedName name="sa" localSheetId="6">FlakLake!$F$6:$L$6</definedName>
     <definedName name="sa" localSheetId="4">SingleFleet!$F$6:$L$6</definedName>
     <definedName name="sa">Sheet2!$G$9:$Z$9</definedName>
     <definedName name="so">FlakLake!$B$14</definedName>
     <definedName name="V" localSheetId="3">Allocation!$G$6:$Z$7</definedName>
-    <definedName name="V" localSheetId="2">'Allocation(2)'!$G$6:$Z$7</definedName>
+    <definedName name="V" localSheetId="2">'Allocation Mar'!$G$6:$Z$7</definedName>
     <definedName name="V">Sheet2!$G$6:$Z$7</definedName>
     <definedName name="va" localSheetId="6">FlakLake!$F$4:$L$4</definedName>
     <definedName name="va" localSheetId="5">Sheet5!$G$2:$M$2</definedName>
     <definedName name="va">SingleFleet!$F$4:$L$4</definedName>
     <definedName name="vbk" localSheetId="3">Allocation!$B$4</definedName>
-    <definedName name="vbk" localSheetId="2">'Allocation(2)'!$B$4</definedName>
+    <definedName name="vbk" localSheetId="2">'Allocation Mar'!$B$4</definedName>
     <definedName name="vbk">Sheet2!$B$4</definedName>
     <definedName name="wa" localSheetId="3">Allocation!$G$2:$Z$2</definedName>
-    <definedName name="wa" localSheetId="2">'Allocation(2)'!$G$2:$Z$2</definedName>
+    <definedName name="wa" localSheetId="2">'Allocation Mar'!$G$2:$Z$2</definedName>
     <definedName name="wa" localSheetId="6">FlakLake!$F$2:$L$2</definedName>
     <definedName name="wa" localSheetId="5">Sheet5!$G$4:$M$4</definedName>
     <definedName name="wa" localSheetId="4">SingleFleet!$F$2:$L$2</definedName>
     <definedName name="wa">Sheet2!$G$2:$Z$2</definedName>
-    <definedName name="Ye" localSheetId="2">'Allocation(2)'!$B$32:$C$32</definedName>
+    <definedName name="Ye" localSheetId="2">'Allocation Mar'!$B$29:$C$29</definedName>
     <definedName name="ye" localSheetId="6">FlakLake!$B$23</definedName>
     <definedName name="Ye" localSheetId="1">Sheet2!$B$29:$C$29</definedName>
     <definedName name="ye" localSheetId="4">SingleFleet!$B$20</definedName>
     <definedName name="Ye">Allocation!$B$29:$C$29</definedName>
     <definedName name="Z">Sheet1!$B$5</definedName>
     <definedName name="za" localSheetId="3">Allocation!$G$8:$Z$8</definedName>
-    <definedName name="za" localSheetId="2">'Allocation(2)'!$G$8:$Z$8</definedName>
+    <definedName name="za" localSheetId="2">'Allocation Mar'!$G$8:$Z$8</definedName>
     <definedName name="za" localSheetId="6">FlakLake!$F$5:$L$5</definedName>
     <definedName name="za" localSheetId="5">Sheet5!$G$5:$M$5</definedName>
     <definedName name="za" localSheetId="4">SingleFleet!$F$5:$L$5</definedName>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="109">
   <si>
     <t>B</t>
   </si>
@@ -537,27 +537,23 @@
     <t>spr</t>
   </si>
   <si>
-    <t>lfi</t>
+    <t>akdYe</t>
   </si>
   <si>
-    <t>plambda</t>
+    <t>invJacobian</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.4378 3.90</t>
-  </si>
-  <si>
-    <t>allocation</t>
+    <t>fstp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.000E+00;\驠"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -616,16 +612,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,13 +653,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -694,23 +677,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1904">
+  <cellStyleXfs count="1909">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2124,7 +2092,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2616,7 +2589,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2629,15 +2602,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="52"/>
     <xf numFmtId="2" fontId="7" fillId="4" borderId="1" xfId="51" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="51" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="1413"/>
   </cellXfs>
-  <cellStyles count="1904">
+  <cellStyles count="1909">
     <cellStyle name="20% - Accent1" xfId="52" builtinId="30"/>
     <cellStyle name="20% - Accent4" xfId="53" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="54" builtinId="50"/>
-    <cellStyle name="Check Cell" xfId="1413" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3341,251 +3310,254 @@
     <cellStyle name="Followed Hyperlink" xfId="1408" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1410" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1412" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1415" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1417" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1419" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1421" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1423" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1425" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1427" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1429" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1431" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1433" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1435" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1437" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1439" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1441" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1443" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1445" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1447" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1449" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1451" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1453" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1455" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1457" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1459" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1461" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1463" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1465" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1467" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1469" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1471" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1473" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1475" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1477" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1479" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1481" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1483" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1485" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1487" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1489" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1491" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1493" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1495" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1497" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1499" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1501" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1503" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1505" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1507" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1509" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1511" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1513" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1515" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1517" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1519" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1521" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1523" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1525" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1527" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1529" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1531" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1533" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1535" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1537" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1539" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1541" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1543" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1545" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1547" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1549" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1551" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1553" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1555" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1557" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1559" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1561" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1563" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1565" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1567" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1569" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1571" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1573" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1575" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1577" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1579" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1581" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1583" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1585" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1587" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1589" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1591" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1593" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1595" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1597" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1599" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1601" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1603" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1605" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1607" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1609" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1611" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1613" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1615" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1617" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1619" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1621" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1623" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1625" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1627" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1629" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1631" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1633" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1635" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1637" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1639" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1641" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1643" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1645" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1647" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1649" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1651" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1653" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1655" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1657" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1659" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1661" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1663" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1665" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1667" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1669" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1671" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1673" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1675" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1677" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1679" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1681" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1683" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1685" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1687" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1689" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1691" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1693" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1695" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1697" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1699" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1701" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1703" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1705" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1707" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1709" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1711" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1713" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1715" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1717" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1719" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1721" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1723" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1725" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1727" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1729" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1731" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1733" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1735" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1737" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1739" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1741" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1743" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1745" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1747" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1749" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1751" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1753" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1755" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1757" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1759" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1761" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1763" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1765" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1767" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1769" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1771" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1773" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1775" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1777" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1779" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1781" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1783" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1785" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1787" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1789" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1791" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1793" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1795" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1797" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1799" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1801" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1803" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1805" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1807" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1809" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1811" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1813" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1815" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1817" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1819" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1821" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1823" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1825" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1827" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1829" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1831" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1833" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1835" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1837" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1839" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1841" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1843" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1845" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1847" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1849" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1851" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1853" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1855" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1857" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1859" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1861" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1863" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1865" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1867" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1869" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1871" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1873" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1875" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1877" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1879" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1881" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1883" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1885" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1887" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1889" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1891" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1893" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1895" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1897" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1899" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1901" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="1903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1908" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="49" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -4290,251 +4262,254 @@
     <cellStyle name="Hyperlink" xfId="1407" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1409" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1411" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1414" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1416" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1418" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1420" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1422" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1424" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1426" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1428" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1430" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1432" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1434" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1436" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1438" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1440" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1442" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1444" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1446" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1448" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1450" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1452" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1454" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1456" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1458" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1460" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1462" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1464" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1466" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1468" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1470" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1472" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1474" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1476" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1478" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1480" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1482" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1484" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1486" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1488" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1490" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1492" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1494" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1496" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1498" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1500" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1502" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1504" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1506" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1508" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1510" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1512" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1514" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1516" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1518" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1520" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1522" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1524" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1526" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1528" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1530" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1532" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1534" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1536" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1538" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1540" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1542" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1544" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1546" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1548" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1550" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1552" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1554" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1556" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1558" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1560" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1562" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1564" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1566" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1568" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1570" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1572" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1574" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1576" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1578" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1580" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1582" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1584" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1586" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1588" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1590" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1592" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1594" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1596" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1598" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1600" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1602" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1604" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1606" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1608" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1610" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1612" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1614" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1616" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1618" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1620" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1622" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1624" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1626" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1628" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1630" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1632" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1634" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1636" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1638" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1640" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1642" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1644" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1646" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1648" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1650" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1652" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1654" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1656" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1658" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1660" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1662" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1664" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1666" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1668" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1670" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1672" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1674" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1676" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1678" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1680" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1682" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1684" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1686" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1688" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1690" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1692" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1694" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1696" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1698" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1700" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1702" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1704" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1706" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1708" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1710" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1712" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1714" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1716" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1718" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1720" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1722" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1724" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1726" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1728" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1730" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1732" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1734" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1736" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1738" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1740" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1742" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1744" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1746" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1748" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1750" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1752" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1754" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1756" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1758" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1760" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1762" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1764" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1766" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1768" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1770" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1772" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1774" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1776" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1778" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1780" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1782" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1784" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1786" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1788" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1790" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1792" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1794" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1796" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1798" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1800" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1802" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1804" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1806" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1808" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1810" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1812" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1814" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1816" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1818" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1820" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1822" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1824" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1826" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1828" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1830" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1832" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1834" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1836" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1838" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1840" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1842" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1844" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1846" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1848" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1850" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1852" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1854" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1856" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1858" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1860" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1862" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1864" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1866" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1868" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1870" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1872" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1874" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1876" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1878" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1880" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1882" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1884" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1886" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1888" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1890" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1892" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1894" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1896" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1898" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1900" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1907" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="51" builtinId="20"/>
     <cellStyle name="Neutral" xfId="50" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4816,11 +4791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2116479608"/>
-        <c:axId val="2116482136"/>
+        <c:axId val="2142774472"/>
+        <c:axId val="2142775880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2116479608"/>
+        <c:axId val="2142774472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4829,7 +4804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116482136"/>
+        <c:crossAx val="2142775880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4837,7 +4812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116482136"/>
+        <c:axId val="2142775880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4848,13 +4823,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116479608"/>
+        <c:crossAx val="2142774472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4897,7 +4873,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Allocation(2)'!$G$6:$Z$6</c:f>
+              <c:f>'Allocation Mar'!$G$6:$Z$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4974,7 +4950,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Allocation(2)'!$G$7:$Z$7</c:f>
+              <c:f>'Allocation Mar'!$G$7:$Z$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -5048,7 +5024,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Allocation(2)'!$F$3</c:f>
+              <c:f>'Allocation Mar'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5062,7 +5038,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Allocation(2)'!$G$3:$Z$3</c:f>
+              <c:f>'Allocation Mar'!$G$3:$Z$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -5141,11 +5117,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2116565592"/>
-        <c:axId val="2116568568"/>
+        <c:axId val="-2137736984"/>
+        <c:axId val="-2137734008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2116565592"/>
+        <c:axId val="-2137736984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5154,7 +5130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116568568"/>
+        <c:crossAx val="-2137734008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5162,7 +5138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116568568"/>
+        <c:axId val="-2137734008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5173,7 +5149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116565592"/>
+        <c:crossAx val="-2137736984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5379,11 +5355,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2116614856"/>
-        <c:axId val="2116617832"/>
+        <c:axId val="2142859016"/>
+        <c:axId val="2142861992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2116614856"/>
+        <c:axId val="2142859016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5392,7 +5368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116617832"/>
+        <c:crossAx val="2142861992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5400,7 +5376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116617832"/>
+        <c:axId val="2142861992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5411,13 +5387,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116614856"/>
+        <c:crossAx val="2142859016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5710,8 +5687,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116665784"/>
-        <c:axId val="2116668776"/>
+        <c:axId val="2142909752"/>
+        <c:axId val="2142912744"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -5974,11 +5951,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116675112"/>
-        <c:axId val="2116671816"/>
+        <c:axId val="2142919080"/>
+        <c:axId val="2142915784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116665784"/>
+        <c:axId val="2142909752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5988,12 +5965,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116668776"/>
+        <c:crossAx val="2142912744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116668776"/>
+        <c:axId val="2142912744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6004,12 +5981,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116665784"/>
+        <c:crossAx val="2142909752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116671816"/>
+        <c:axId val="2142915784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -6021,12 +5998,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116675112"/>
+        <c:crossAx val="2142919080"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116675112"/>
+        <c:axId val="2142919080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6036,7 +6013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116671816"/>
+        <c:crossAx val="2142915784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6335,8 +6312,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116727848"/>
-        <c:axId val="2116730840"/>
+        <c:axId val="2142971976"/>
+        <c:axId val="2142974968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -6599,11 +6576,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116737176"/>
-        <c:axId val="2116733880"/>
+        <c:axId val="2142981304"/>
+        <c:axId val="2142978008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116727848"/>
+        <c:axId val="2142971976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6613,12 +6590,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116730840"/>
+        <c:crossAx val="2142974968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116730840"/>
+        <c:axId val="2142974968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6629,12 +6606,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116727848"/>
+        <c:crossAx val="2142971976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116733880"/>
+        <c:axId val="2142978008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -6646,12 +6623,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116737176"/>
+        <c:crossAx val="2142981304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116737176"/>
+        <c:axId val="2142981304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6661,7 +6638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116733880"/>
+        <c:crossAx val="2142978008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7389,10 +7366,10 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="C10" sqref="C10"/>
+      <selection pane="topRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10137,18 +10114,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4"/>
+      <selection pane="topRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="7.1640625" customWidth="1"/>
     <col min="9" max="23" width="7.33203125" customWidth="1"/>
@@ -10601,15 +10576,15 @@
         <v>27</v>
       </c>
       <c r="B6" s="11">
-        <v>0.22797681823165919</v>
+        <v>0.22198504671239971</v>
       </c>
       <c r="C6">
         <f>B6+dh</f>
-        <v>0.22797781823165919</v>
+        <v>0.22198604671239971</v>
       </c>
       <c r="D6">
         <f>B6-dh</f>
-        <v>0.22797581823165919</v>
+        <v>0.22198404671239971</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -10703,15 +10678,15 @@
         <v>28</v>
       </c>
       <c r="B7" s="11">
-        <v>0.43854729534046094</v>
+        <v>0.22198504671239971</v>
       </c>
       <c r="C7">
         <f>B7</f>
-        <v>0.43854729534046094</v>
+        <v>0.22198504671239971</v>
       </c>
       <c r="D7">
         <f>C7</f>
-        <v>0.43854729534046094</v>
+        <v>0.22198504671239971</v>
       </c>
       <c r="E7">
         <v>7</v>
@@ -10805,88 +10780,91 @@
         <f>4*h/(1-h)</f>
         <v>12</v>
       </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" t="s">
         <v>35</v>
       </c>
       <c r="G8">
         <f t="shared" ref="G8:Z8" si="6">m+SUMPRODUCT(fe,G6:G7)</f>
-        <v>0.30020908417921827</v>
+        <v>0.3001647538788268</v>
       </c>
       <c r="H8">
         <f t="shared" si="6"/>
-        <v>0.3018722084310474</v>
+        <v>0.30166105125303944</v>
       </c>
       <c r="I8">
         <f t="shared" si="6"/>
-        <v>0.31873570152688419</v>
+        <v>0.31756919330186456</v>
       </c>
       <c r="J8">
         <f t="shared" si="6"/>
-        <v>0.4199425293205708</v>
+        <v>0.41400639589816735</v>
       </c>
       <c r="K8">
         <f t="shared" si="6"/>
-        <v>0.53450184767714792</v>
+        <v>0.51720239799642365</v>
       </c>
       <c r="L8">
         <f t="shared" si="6"/>
-        <v>0.61123156723135752</v>
+        <v>0.56341378719340385</v>
       </c>
       <c r="M8">
         <f t="shared" si="6"/>
-        <v>0.74712444518705745</v>
+        <v>0.63285486147706049</v>
       </c>
       <c r="N8">
         <f t="shared" si="6"/>
-        <v>0.8817332000521434</v>
+        <v>0.70104556247072436</v>
       </c>
       <c r="O8">
         <f t="shared" si="6"/>
-        <v>0.94270432802117732</v>
+        <v>0.73191253324704664</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
-        <v>0.96056992362876259</v>
+        <v>0.74095615297711181</v>
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
-        <v>0.96508231283882773</v>
+        <v>0.74324027618442579</v>
       </c>
       <c r="R8">
         <f t="shared" si="6"/>
-        <v>0.96617771952979492</v>
+        <v>0.74379475453928123</v>
       </c>
       <c r="S8">
         <f t="shared" si="6"/>
-        <v>0.96644105006916292</v>
+        <v>0.74392804809995428</v>
       </c>
       <c r="T8">
         <f t="shared" si="6"/>
-        <v>0.96650420445642038</v>
+        <v>0.74396001577371207</v>
       </c>
       <c r="U8">
         <f t="shared" si="6"/>
-        <v>0.96651934216770663</v>
+        <v>0.74396767822238874</v>
       </c>
       <c r="V8">
         <f t="shared" si="6"/>
-        <v>0.96652297009068855</v>
+        <v>0.74396951461429017</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>0.96652383953507004</v>
+        <v>0.74396995471198923</v>
       </c>
       <c r="X8">
         <f t="shared" si="6"/>
-        <v>0.96652404789882618</v>
+        <v>0.7439700601821152</v>
       </c>
       <c r="Y8">
         <f t="shared" si="6"/>
-        <v>0.96652409783344551</v>
+        <v>0.74397008545815491</v>
       </c>
       <c r="Z8">
         <f t="shared" si="6"/>
-        <v>0.96652410980033043</v>
+        <v>0.7439700915155848</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -10895,385 +10873,356 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" ref="G9:Z9" si="7">EXP(-za)</f>
-        <v>0.74066334350384477</v>
+        <v>0.74069617806012866</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="7"/>
-        <v>0.73943255209803616</v>
+        <v>0.73958870507489516</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="7"/>
-        <v>0.72706768679386902</v>
+        <v>0.72791631209862906</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="7"/>
-        <v>0.65708458182730223</v>
+        <v>0.66099672358465955</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="7"/>
-        <v>0.58596111534276785</v>
+        <v>0.59618610854786458</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="7"/>
-        <v>0.54268210784575455</v>
+        <v>0.56926240229655334</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="7"/>
-        <v>0.47372682348444495</v>
+        <v>0.53107349350122179</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="7"/>
-        <v>0.41406463255794207</v>
+        <v>0.49606636417342198</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38957287667761381</v>
+        <v>0.48098820392235364</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38267472844458045</v>
+        <v>0.47665793965636655</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38095184122124304</v>
+        <v>0.47557043666267168</v>
       </c>
       <c r="R9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38053477249707252</v>
+        <v>0.47530681624199572</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38043457926273078</v>
+        <v>0.47524346512628834</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38041055390864709</v>
+        <v>0.4752282729410704</v>
       </c>
       <c r="U9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38040479540709715</v>
+        <v>0.47522463154277034</v>
       </c>
       <c r="V9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38040341533030092</v>
+        <v>0.47522375884490692</v>
       </c>
       <c r="W9" s="7">
         <f t="shared" si="7"/>
-        <v>0.3804030845908325</v>
+        <v>0.47522354970007014</v>
       </c>
       <c r="X9" s="7">
         <f t="shared" si="7"/>
-        <v>0.3804030053286252</v>
+        <v>0.4752234995781851</v>
       </c>
       <c r="Y9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38040298633334646</v>
+        <v>0.47522348756641719</v>
       </c>
       <c r="Z9" s="7">
         <f t="shared" si="7"/>
-        <v>0.38040298178110771</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="16" thickBot="1">
+        <v>0.47522348468778425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10">
+        <v>0.4</v>
+      </c>
+      <c r="C10">
+        <f>1-B10</f>
+        <v>0.6</v>
+      </c>
       <c r="F10" t="s">
         <v>61</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:Z10" si="8">1-sa</f>
-        <v>0.25933665649615523</v>
+        <v>0.25930382193987134</v>
       </c>
       <c r="H10">
         <f t="shared" si="8"/>
-        <v>0.26056744790196384</v>
+        <v>0.26041129492510484</v>
       </c>
       <c r="I10">
         <f t="shared" si="8"/>
-        <v>0.27293231320613098</v>
+        <v>0.27208368790137094</v>
       </c>
       <c r="J10">
         <f t="shared" si="8"/>
-        <v>0.34291541817269777</v>
+        <v>0.33900327641534045</v>
       </c>
       <c r="K10">
         <f t="shared" si="8"/>
-        <v>0.41403888465723215</v>
+        <v>0.40381389145213542</v>
       </c>
       <c r="L10">
         <f t="shared" si="8"/>
-        <v>0.45731789215424545</v>
+        <v>0.43073759770344666</v>
       </c>
       <c r="M10">
         <f t="shared" si="8"/>
-        <v>0.52627317651555505</v>
+        <v>0.46892650649877821</v>
       </c>
       <c r="N10">
         <f t="shared" si="8"/>
-        <v>0.58593536744205799</v>
+        <v>0.50393363582657802</v>
       </c>
       <c r="O10">
         <f t="shared" si="8"/>
-        <v>0.61042712332238613</v>
+        <v>0.51901179607764636</v>
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>0.61732527155541961</v>
+        <v>0.5233420603436334</v>
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
-        <v>0.61904815877875696</v>
+        <v>0.52442956333732837</v>
       </c>
       <c r="R10">
         <f t="shared" si="8"/>
-        <v>0.61946522750292754</v>
+        <v>0.52469318375800422</v>
       </c>
       <c r="S10">
         <f t="shared" si="8"/>
-        <v>0.61956542073726917</v>
+        <v>0.52475653487371166</v>
       </c>
       <c r="T10">
         <f t="shared" si="8"/>
-        <v>0.61958944609135291</v>
+        <v>0.5247717270589296</v>
       </c>
       <c r="U10">
         <f t="shared" si="8"/>
-        <v>0.61959520459290285</v>
+        <v>0.52477536845722961</v>
       </c>
       <c r="V10">
         <f t="shared" si="8"/>
-        <v>0.61959658466969914</v>
+        <v>0.52477624115509314</v>
       </c>
       <c r="W10">
         <f t="shared" si="8"/>
-        <v>0.6195969154091675</v>
+        <v>0.52477645029992992</v>
       </c>
       <c r="X10">
         <f t="shared" si="8"/>
-        <v>0.61959699467137486</v>
+        <v>0.5247765004218149</v>
       </c>
       <c r="Y10">
         <f t="shared" si="8"/>
-        <v>0.61959701366665354</v>
+        <v>0.52477651243358281</v>
       </c>
       <c r="Z10">
         <f t="shared" si="8"/>
-        <v>0.61959701821889235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="17" thickTop="1" thickBot="1">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="14">
-        <f>Ye/SUM(Ye)</f>
-        <v>0.65806690320872352</v>
-      </c>
-      <c r="C11" s="14">
-        <f>Ye/SUM(Ye)</f>
-        <v>0.34193309679127654</v>
-      </c>
+        <v>0.5247765153122157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="F11" t="s">
         <v>40</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:Z11" si="9">wa*G6/za*(1-EXP(-za))</f>
-        <v>2.844223496420916E-6</v>
+        <v>2.8442833903233952E-6</v>
       </c>
       <c r="H11">
         <f t="shared" si="9"/>
-        <v>2.0700736711258333E-4</v>
+        <v>2.0702812615141169E-4</v>
       </c>
       <c r="I11">
-        <f t="shared" si="9"/>
-        <v>5.9662347280344486E-3</v>
+        <f>wa*I6/za*(1-EXP(-za))</f>
+        <v>5.9695312604443451E-3</v>
       </c>
       <c r="J11">
         <f t="shared" si="9"/>
-        <v>6.817793756504241E-2</v>
+        <v>6.8366532256935564E-2</v>
       </c>
       <c r="K11">
         <f t="shared" si="9"/>
-        <v>0.18081326523765018</v>
+        <v>0.1822464573414547</v>
       </c>
       <c r="L11">
         <f t="shared" si="9"/>
-        <v>0.25360946590052708</v>
+        <v>0.2591423262633164</v>
       </c>
       <c r="M11">
         <f t="shared" si="9"/>
-        <v>0.30106498730197689</v>
+        <v>0.31669603389935391</v>
       </c>
       <c r="N11">
         <f t="shared" si="9"/>
-        <v>0.33780838059701218</v>
+        <v>0.36541384875993488</v>
       </c>
       <c r="O11">
         <f t="shared" si="9"/>
-        <v>0.37657343422056988</v>
+        <v>0.41239121198241591</v>
       </c>
       <c r="P11">
         <f t="shared" si="9"/>
-        <v>0.4154589813049912</v>
+        <v>0.45660031959900554</v>
       </c>
       <c r="Q11">
         <f t="shared" si="9"/>
-        <v>0.45097638740561641</v>
+        <v>0.4960799257272403</v>
       </c>
       <c r="R11">
         <f t="shared" si="9"/>
-        <v>0.48200968294632307</v>
+        <v>0.53033239800175513</v>
       </c>
       <c r="S11">
         <f t="shared" si="9"/>
-        <v>0.5085805890129903</v>
+        <v>0.55959638548245694</v>
       </c>
       <c r="T11">
         <f t="shared" si="9"/>
-        <v>0.5310807456769524</v>
+        <v>0.58436086892961103</v>
       </c>
       <c r="U11">
         <f t="shared" si="9"/>
-        <v>0.54999698374267447</v>
+        <v>0.60517667908113149</v>
       </c>
       <c r="V11">
         <f t="shared" si="9"/>
-        <v>0.56581659787535143</v>
+        <v>0.62258388067067572</v>
       </c>
       <c r="W11">
         <f t="shared" si="9"/>
-        <v>0.57899268643817248</v>
+        <v>0.63708201072048454</v>
       </c>
       <c r="X11">
         <f t="shared" si="9"/>
-        <v>0.58993153297591361</v>
+        <v>0.64911835948583985</v>
       </c>
       <c r="Y11">
         <f t="shared" si="9"/>
-        <v>0.59898943296898877</v>
+        <v>0.65908502970573268</v>
       </c>
       <c r="Z11">
         <f t="shared" si="9"/>
-        <v>0.60647408020638927</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="16" thickTop="1">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12">
-        <v>0.5</v>
-      </c>
-      <c r="C12">
-        <v>0.5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>108</v>
-      </c>
+        <v>0.66732060052832298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="G12">
         <f t="shared" ref="G12:Z12" si="10">wa*G7/za*(1-EXP(-za))</f>
-        <v>9.7455436915488243E-7</v>
+        <v>9.7457489140442438E-7</v>
       </c>
       <c r="H12">
         <f t="shared" si="10"/>
-        <v>2.4430257123684155E-5</v>
+        <v>2.4432707030000494E-5</v>
       </c>
       <c r="I12">
         <f t="shared" si="10"/>
-        <v>2.5857408560664571E-4</v>
+        <v>2.5871695592476386E-4</v>
       </c>
       <c r="J12">
         <f t="shared" si="10"/>
-        <v>1.8512923914327398E-3</v>
+        <v>1.8564134603684685E-3</v>
       </c>
       <c r="K12">
         <f t="shared" si="10"/>
-        <v>1.0626679566768207E-2</v>
+        <v>1.0710910517549034E-2</v>
       </c>
       <c r="L12">
         <f t="shared" si="10"/>
-        <v>4.935847827969736E-2</v>
+        <v>5.043530546779787E-2</v>
       </c>
       <c r="M12">
         <f t="shared" si="10"/>
-        <v>0.15061575082042619</v>
+        <v>0.1584355967628957</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
-        <v>0.27251517333735675</v>
+        <v>0.29478492558027752</v>
       </c>
       <c r="O12">
         <f t="shared" si="10"/>
-        <v>0.35612182820686061</v>
+        <v>0.38999435170352448</v>
       </c>
       <c r="P12">
         <f t="shared" si="10"/>
-        <v>0.40981845458665866</v>
+        <v>0.45040123276206284</v>
       </c>
       <c r="Q12">
         <f t="shared" si="10"/>
-        <v>0.44949374103755874</v>
+        <v>0.49444899532669961</v>
       </c>
       <c r="R12">
         <f t="shared" si="10"/>
-        <v>0.48162896090688795</v>
+        <v>0.52991350759500733</v>
       </c>
       <c r="S12">
         <f t="shared" si="10"/>
-        <v>0.5084842609125475</v>
+        <v>0.55949039469556361</v>
       </c>
       <c r="T12">
         <f t="shared" si="10"/>
-        <v>0.5310566357503651</v>
+        <v>0.58433434019972386</v>
       </c>
       <c r="U12">
         <f t="shared" si="10"/>
-        <v>0.54999099976410326</v>
+        <v>0.60517009474633232</v>
       </c>
       <c r="V12">
         <f t="shared" si="10"/>
-        <v>0.565815122548186</v>
+        <v>0.62258225732679484</v>
       </c>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>0.57899232464037653</v>
+        <v>0.63708161262414797</v>
       </c>
       <c r="X12">
         <f t="shared" si="10"/>
-        <v>0.58993144463254177</v>
+        <v>0.64911826227912783</v>
       </c>
       <c r="Y12">
         <f t="shared" si="10"/>
-        <v>0.59898941147233398</v>
+        <v>0.65908500605235476</v>
       </c>
       <c r="Z12">
         <f t="shared" si="10"/>
-        <v>0.6064740749903208</v>
+        <v>0.66732059478893513</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13">
-        <f>(Ye/SUM(Ye))</f>
-        <v>0.65806690320872352</v>
-      </c>
-      <c r="C13">
-        <f>(Ye/SUM(Ye))</f>
-        <v>0.34193309679127654</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="1">
-        <f>ak/pk</f>
-        <v>0.75980116544686893</v>
-      </c>
-      <c r="C14" s="1">
-        <f>ak/pk</f>
-        <v>1.4622743592007736</v>
-      </c>
       <c r="F14" t="s">
         <v>25</v>
       </c>
@@ -11283,90 +11232,88 @@
       </c>
       <c r="H14">
         <f>G14*EXP(-m-SUMPRODUCT(G$6:G$7,$B$6:$B$7))</f>
-        <v>0.74066334350384477</v>
+        <v>0.74069617806012866</v>
       </c>
       <c r="I14">
         <f t="shared" ref="I14:Y14" si="11">H14*EXP(-m-SUMPRODUCT(H$6:H$7,$B$6:$B$7))</f>
-        <v>0.54767058633251231</v>
+        <v>0.54781052718541456</v>
       </c>
       <c r="J14">
         <f t="shared" si="11"/>
-        <v>0.39819358632982166</v>
+        <v>0.39876021867761274</v>
       </c>
       <c r="K14">
         <f t="shared" si="11"/>
-        <v>0.26164686615984462</v>
+        <v>0.26357919804180441</v>
       </c>
       <c r="L14">
         <f t="shared" si="11"/>
-        <v>0.15331488952096245</v>
+        <v>0.1571422563747103</v>
       </c>
       <c r="M14">
-        <f>L14*EXP(-m-SUMPRODUCT(L$6:L$7,$B$6:$B$7))</f>
-        <v>8.3201247409374887E-2</v>
+        <f t="shared" si="11"/>
+        <v>8.9455178366168453E-2</v>
       </c>
       <c r="N14">
         <f t="shared" si="11"/>
-        <v>3.9414662645186567E-2</v>
+        <v>4.7507274086696E-2</v>
       </c>
       <c r="O14">
         <f t="shared" si="11"/>
-        <v>1.6320217805574421E-2</v>
+        <v>2.3566760727977511E-2</v>
       </c>
       <c r="P14">
         <f t="shared" si="11"/>
-        <v>6.3579141985228406E-3</v>
+        <v>1.1335333914817763E-2</v>
       </c>
       <c r="Q14">
         <f t="shared" si="11"/>
-        <v>2.4330130893936703E-3</v>
+        <v>5.4030769091539706E-3</v>
       </c>
       <c r="R14">
         <f t="shared" si="11"/>
-        <v>9.2686081611990348E-4</v>
+        <v>2.5695436450083524E-3</v>
       </c>
       <c r="S14">
         <f t="shared" si="11"/>
-        <v>3.5270276979863845E-4</v>
+        <v>1.2213216091037729E-3</v>
       </c>
       <c r="T14">
         <f t="shared" si="11"/>
-        <v>1.3418032983314481E-4</v>
+        <v>5.804251135440912E-4</v>
       </c>
       <c r="U14">
         <f t="shared" si="11"/>
-        <v>5.1043613595471585E-5</v>
+        <v>2.7583442428118313E-4</v>
       </c>
       <c r="V14">
         <f t="shared" si="11"/>
-        <v>1.9417235386624289E-5</v>
+        <v>1.3108331264583743E-4</v>
       </c>
       <c r="W14">
         <f t="shared" si="11"/>
-        <v>7.3863826573442556E-6</v>
+        <v>6.2293904557396984E-5</v>
       </c>
       <c r="X14">
         <f t="shared" si="11"/>
-        <v>2.8098027468219851E-6</v>
+        <v>2.960353044844357E-5</v>
       </c>
       <c r="Y14">
         <f t="shared" si="11"/>
-        <v>1.0688574092717094E-6</v>
+        <v>1.4068293339578713E-5</v>
       </c>
       <c r="Z14">
         <f>Y14*EXP(-m-SUMPRODUCT(Y$6:Y$7,$B$6:$B$7))/(1-EXP(-m-SUMPRODUCT(B$6:B$7,Z6:Z7)))</f>
-        <v>6.5622741636216036E-7</v>
+        <v>1.273986779108133E-5</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B15">
-        <v>0.75992272743886402</v>
-      </c>
-      <c r="C15">
-        <v>1.4618243178015364</v>
+        <f>phif/phie</f>
+        <v>0.39514573861617147</v>
       </c>
       <c r="F15" t="s">
         <v>26</v>
@@ -11377,93 +11324,82 @@
       </c>
       <c r="H15">
         <f>G15*EXP(-m-SUMPRODUCT(G$6:G$7,$C$6:$C$7))</f>
-        <v>0.74066334309442183</v>
+        <v>0.74069617765068774</v>
       </c>
       <c r="I15">
         <f t="shared" ref="I15:Y15" si="12">H15*EXP(-m-SUMPRODUCT(H$6:H$7,$C$6:$C$7))</f>
-        <v>0.54767058236429411</v>
+        <v>0.54781052321618251</v>
       </c>
       <c r="J15">
         <f t="shared" si="12"/>
-        <v>0.39819355323841898</v>
+        <v>0.39876018553912085</v>
       </c>
       <c r="K15">
         <f t="shared" si="12"/>
-        <v>0.26164671359260466</v>
+        <v>0.26357904434781471</v>
       </c>
       <c r="L15">
         <f t="shared" si="12"/>
-        <v>0.15331465843793943</v>
+        <v>0.15714201952290968</v>
       </c>
       <c r="M15">
         <f t="shared" si="12"/>
-        <v>8.3201039360524601E-2</v>
+        <v>8.9454954679053303E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="12"/>
-        <v>3.9414524694108721E-2</v>
+        <v>4.7507107811527685E-2</v>
       </c>
       <c r="O15">
         <f t="shared" si="12"/>
-        <v>1.6320144365500437E-2</v>
+        <v>2.3566654678862726E-2</v>
       </c>
       <c r="P15">
         <f t="shared" si="12"/>
-        <v>6.3578792304032393E-3</v>
+        <v>1.1335271571209518E-2</v>
       </c>
       <c r="Q15">
         <f t="shared" si="12"/>
-        <v>2.4329972749802505E-3</v>
+        <v>5.4030417895352756E-3</v>
       </c>
       <c r="R15">
         <f t="shared" si="12"/>
-        <v>9.268538647356886E-4</v>
+        <v>2.5695243736303603E-3</v>
       </c>
       <c r="S15">
         <f t="shared" si="12"/>
-        <v>3.526997718552802E-4</v>
+        <v>1.2213112279746187E-3</v>
       </c>
       <c r="T15">
         <f t="shared" si="12"/>
-        <v>1.3417905513270244E-4</v>
+        <v>5.8041959956041042E-4</v>
       </c>
       <c r="U15">
         <f t="shared" si="12"/>
-        <v>5.104307764286707E-5</v>
+        <v>2.7583152804857555E-4</v>
       </c>
       <c r="V15">
         <f t="shared" si="12"/>
-        <v>1.9417012090661623E-5</v>
+        <v>1.310818052028929E-4</v>
       </c>
       <c r="W15">
         <f t="shared" si="12"/>
-        <v>7.3862903285034056E-6</v>
+        <v>6.2293125891537613E-5</v>
       </c>
       <c r="X15">
         <f t="shared" si="12"/>
-        <v>2.8097648148799091E-6</v>
+        <v>2.9603130804944239E-5</v>
       </c>
       <c r="Y15">
         <f t="shared" si="12"/>
-        <v>1.0688419110045004E-6</v>
+        <v>1.4068089351499991E-5</v>
       </c>
       <c r="Z15">
         <f>Y15*EXP(-m-SUMPRODUCT(Y$6:Y$7,$C$6:$C$7))/(1-EXP(-m-SUMPRODUCT(C$6:C$7,Z6:Z7)))</f>
-        <v>6.5621684206288718E-7</v>
+        <v>1.2739658788604744E-5</v>
       </c>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="1">
-        <f>fbar*plambda</f>
-        <v>0.22797681823165919</v>
-      </c>
-      <c r="C16" s="1">
-        <f>fbar*plambda</f>
-        <v>0.43854729534046094</v>
-      </c>
       <c r="F16" t="s">
         <v>66</v>
       </c>
@@ -11473,87 +11409,88 @@
       </c>
       <c r="H16">
         <f>G16*EXP(-m-SUMPRODUCT(G$6:G$7,$D$6:$D$7))</f>
-        <v>0.7406633439132676</v>
+        <v>0.7406961784695697</v>
       </c>
       <c r="I16">
         <f t="shared" ref="I16:Y16" si="13">H16*EXP(-m-SUMPRODUCT(H$6:H$7,$D$6:$D$7))</f>
-        <v>0.54767059030073062</v>
+        <v>0.54781053115464673</v>
       </c>
       <c r="J16">
         <f t="shared" si="13"/>
-        <v>0.39819361942122711</v>
+        <v>0.39876025181610741</v>
       </c>
       <c r="K16">
         <f t="shared" si="13"/>
-        <v>0.26164701872717361</v>
+        <v>0.2635793517358837</v>
       </c>
       <c r="L16">
         <f t="shared" si="13"/>
-        <v>0.15331512060433383</v>
+        <v>0.15714249322686794</v>
       </c>
       <c r="M16">
         <f t="shared" si="13"/>
-        <v>8.3201455458745424E-2</v>
+        <v>8.9455402053842947E-2</v>
       </c>
       <c r="N16">
         <f t="shared" si="13"/>
-        <v>3.9414800596747256E-2</v>
+        <v>4.7507440362446286E-2</v>
       </c>
       <c r="O16">
         <f t="shared" si="13"/>
-        <v>1.6320291245978891E-2</v>
+        <v>2.3566866777569518E-2</v>
       </c>
       <c r="P16">
         <f t="shared" si="13"/>
-        <v>6.3579491668347681E-3</v>
+        <v>1.1335396258768896E-2</v>
       </c>
       <c r="Q16">
         <f t="shared" si="13"/>
-        <v>2.4330289039098847E-3</v>
+        <v>5.4031120290009421E-3</v>
       </c>
       <c r="R16">
         <f t="shared" si="13"/>
-        <v>9.2686776755625429E-4</v>
+        <v>2.569562916530879E-3</v>
       </c>
       <c r="S16">
         <f t="shared" si="13"/>
-        <v>3.527057677674794E-4</v>
+        <v>1.2213319903211664E-3</v>
       </c>
       <c r="T16">
         <f t="shared" si="13"/>
-        <v>1.3418160454569688E-4</v>
+        <v>5.8043062758015489E-4</v>
       </c>
       <c r="U16">
         <f t="shared" si="13"/>
-        <v>5.1044149553703617E-5</v>
+        <v>2.7583732054420123E-4</v>
       </c>
       <c r="V16">
         <f t="shared" si="13"/>
-        <v>1.9417458685154871E-5</v>
+        <v>1.310848201061176E-4</v>
       </c>
       <c r="W16">
         <f t="shared" si="13"/>
-        <v>7.386474987339221E-6</v>
+        <v>6.2294683232989712E-5</v>
       </c>
       <c r="X16">
         <f t="shared" si="13"/>
-        <v>2.8098406792761446E-6</v>
+        <v>2.9603930097338107E-5</v>
       </c>
       <c r="Y16">
         <f t="shared" si="13"/>
-        <v>1.0688729077636446E-6</v>
-      </c>
-      <c r="Z16" s="13">
+        <v>1.4068497330615273E-5</v>
+      </c>
+      <c r="Z16">
         <f>Y16*EXP(-m-SUMPRODUCT(Y$6:Y$7,$D$6:$D$7))/(1-EXP(-m-SUMPRODUCT(D$6:D$7,Z6:Z7)))</f>
-        <v>6.5623799083247893E-7</v>
+        <v>1.2740076797008714E-5</v>
       </c>
     </row>
     <row r="17" spans="1:26">
       <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <f>ro*(reck-phie/phif)/(reck-1)</f>
+        <v>0.86084437800731195</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>31</v>
@@ -11563,89 +11500,89 @@
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" ref="H17:X17" si="14">(H15-H14)/dh</f>
-        <v>-4.0942293999535195E-4</v>
+        <f t="shared" ref="H17:Y17" si="14">(H15-H14)/dh</f>
+        <v>-4.0944092560835088E-4</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.9682181984801446E-3</v>
+        <v>-3.9692320541462323E-3</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.3091402673601777E-2</v>
+        <v>-3.3138491895012834E-2</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="14"/>
-        <v>-0.1525672399527167</v>
+        <v>-0.15369398970177528</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="14"/>
-        <v>-0.23108302302232708</v>
+        <v>-0.23685180061683297</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="14"/>
-        <v>-0.20804885028646858</v>
+        <v>-0.2236871151500841</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="14"/>
-        <v>-0.13795107784569938</v>
+        <v>-0.166275168314578</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="14"/>
-        <v>-7.3440073983938037E-2</v>
+        <v>-0.106049114784873</v>
       </c>
       <c r="P17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.496811960129742E-2</v>
+        <v>-6.2343608244613824E-2</v>
       </c>
       <c r="Q17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.5814413419860257E-2</v>
+        <v>-3.5119618694949561E-2</v>
       </c>
       <c r="R17" s="3">
         <f t="shared" si="14"/>
-        <v>-6.9513842148845664E-3</v>
+        <v>-1.9271377992100686E-2</v>
       </c>
       <c r="S17" s="3">
         <f t="shared" si="14"/>
-        <v>-2.9979433582437605E-3</v>
+        <v>-1.0381129154218849E-2</v>
       </c>
       <c r="T17" s="3">
         <f t="shared" si="14"/>
-        <v>-1.2747004423676288E-3</v>
+        <v>-5.5139836807821876E-3</v>
       </c>
       <c r="U17" s="3">
         <f t="shared" si="14"/>
-        <v>-5.3595260451493086E-4</v>
+        <v>-2.896232607582129E-3</v>
       </c>
       <c r="V17" s="3">
         <f t="shared" si="14"/>
-        <v>-2.2329596266641716E-4</v>
+        <v>-1.5074429445319486E-3</v>
       </c>
       <c r="W17" s="3">
         <f t="shared" si="14"/>
-        <v>-9.2328840849947966E-5</v>
+        <v>-7.7866585937089432E-4</v>
       </c>
       <c r="X17" s="3">
         <f t="shared" si="14"/>
-        <v>-3.7931942076030657E-5</v>
+        <v>-3.9964349933069255E-4</v>
       </c>
       <c r="Y17" s="3">
-        <f>(Y15-Y14)/dh</f>
-        <v>-1.5498267208928154E-5</v>
+        <f t="shared" si="14"/>
+        <v>-2.03988078722477E-4</v>
       </c>
       <c r="Z17" s="3">
         <f>(Z15-Z14)/dh</f>
-        <v>-1.0574299273180406E-5</v>
+        <v>-2.0900247658547607E-4</v>
       </c>
     </row>
     <row r="18" spans="1:26">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="B18">
-        <f>phif/phie</f>
-        <v>0.35627128424474719</v>
+        <f>SUMPRODUCT(lx,fa)</f>
+        <v>0.53468880128210072</v>
       </c>
       <c r="F18" t="s">
         <v>33</v>
@@ -11656,85 +11593,88 @@
       </c>
       <c r="H18">
         <f t="shared" ref="H18:Y18" si="15">G18*EXP(-G8) - G14*G6*EXP(-G8)</f>
-        <v>-4.0942287344133109E-4</v>
+        <v>-4.0944102368259768E-4</v>
       </c>
       <c r="I18">
         <f t="shared" si="15"/>
-        <v>-3.9682181901352183E-3</v>
+        <v>-3.9692321497158279E-3</v>
       </c>
       <c r="J18">
         <f t="shared" si="15"/>
-        <v>-3.309140397530716E-2</v>
+        <v>-3.3138493282041256E-2</v>
       </c>
       <c r="K18">
         <f t="shared" si="15"/>
-        <v>-0.15256728442311535</v>
+        <v>-0.15369403450486374</v>
       </c>
       <c r="L18">
         <f t="shared" si="15"/>
-        <v>-0.23108319717713016</v>
+        <v>-0.23685197914016906</v>
       </c>
       <c r="M18">
         <f t="shared" si="15"/>
-        <v>-0.2080491103955705</v>
+        <v>-0.22368739482698413</v>
       </c>
       <c r="N18">
         <f t="shared" si="15"/>
-        <v>-0.13795131925815299</v>
+        <v>-0.16627545930343599</v>
       </c>
       <c r="O18">
         <f t="shared" si="15"/>
-        <v>-7.3440239221979758E-2</v>
+        <v>-0.10604935339518952</v>
       </c>
       <c r="P18">
         <f t="shared" si="15"/>
-        <v>-3.49682157624688E-2</v>
+        <v>-6.2343779688796258E-2</v>
       </c>
       <c r="Q18">
         <f t="shared" si="15"/>
-        <v>-1.5814464816223794E-2</v>
+        <v>-3.5119732833192766E-2</v>
       </c>
       <c r="R18">
         <f t="shared" si="15"/>
-        <v>-6.951410282515458E-3</v>
+        <v>-1.9271450259444985E-2</v>
       </c>
       <c r="S18">
         <f t="shared" si="15"/>
-        <v>-2.9979560994624942E-3</v>
+        <v>-1.038117327376922E-2</v>
       </c>
       <c r="T18">
         <f t="shared" si="15"/>
-        <v>-1.2747064971575944E-3</v>
+        <v>-5.5140098721483885E-3</v>
       </c>
       <c r="U18">
         <f t="shared" si="15"/>
-        <v>-5.359554182494344E-4</v>
+        <v>-2.8962478127984434E-3</v>
       </c>
       <c r="V18">
         <f t="shared" si="15"/>
-        <v>-2.2329724661310341E-4</v>
+        <v>-1.5074516123393827E-3</v>
       </c>
       <c r="W18">
         <f t="shared" si="15"/>
-        <v>-9.2329417902820574E-5</v>
+        <v>-7.7867072605012808E-4</v>
       </c>
       <c r="X18">
         <f t="shared" si="15"/>
-        <v>-3.7932198115530941E-5</v>
+        <v>-3.9964619692951607E-4</v>
       </c>
       <c r="Y18">
         <f t="shared" si="15"/>
-        <v>-1.5498379571140493E-5</v>
+        <v>-2.0398955763753585E-4</v>
       </c>
       <c r="Z18">
         <f>(Y18-Y14*Y6)*Y$9/oa-Y14*Y$9*Z6*sa/oa^2</f>
-        <v>-1.0574384795113847E-5</v>
+        <v>-2.0900420197627822E-4</v>
       </c>
     </row>
     <row r="19" spans="1:26">
-      <c r="D19">
-        <f>B15/SUM(plambda)*favg</f>
-        <v>0.11398840911582959</v>
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <f>SUMPRODUCT(lz,fa)</f>
+        <v>0.21128000131241101</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
@@ -11744,88 +11684,92 @@
       </c>
       <c r="H19">
         <f t="shared" ref="H19:Y19" si="16">G19*EXP(-G8) - G14*G7*EXP(-G8)</f>
-        <v>-1.402860396330637E-4</v>
+        <v>-1.4029225869318672E-4</v>
       </c>
       <c r="I19">
         <f t="shared" si="16"/>
-        <v>-5.3631840774449283E-4</v>
+        <v>-5.364554478873814E-4</v>
       </c>
       <c r="J19">
         <f t="shared" si="16"/>
-        <v>-1.6990654620068959E-3</v>
+        <v>-1.7014832444243913E-3</v>
       </c>
       <c r="K19">
         <f t="shared" si="16"/>
-        <v>-4.6687874890432223E-3</v>
+        <v>-4.7032677297110456E-3</v>
       </c>
       <c r="L19">
         <f t="shared" si="16"/>
-        <v>-1.1062760321026557E-2</v>
+        <v>-1.1338932076398465E-2</v>
       </c>
       <c r="M19">
         <f t="shared" si="16"/>
-        <v>-2.2088141208048213E-2</v>
+        <v>-2.3748425330945577E-2</v>
       </c>
       <c r="N19">
         <f t="shared" si="16"/>
-        <v>-3.0171076293757836E-2</v>
+        <v>-3.6365796249006176E-2</v>
       </c>
       <c r="O19">
         <f t="shared" si="16"/>
-        <v>-2.5657946563381218E-2</v>
+        <v>-3.7050650587757611E-2</v>
       </c>
       <c r="P19">
         <f t="shared" si="16"/>
-        <v>-1.6008235164946892E-2</v>
+        <v>-2.8540600787560148E-2</v>
       </c>
       <c r="Q19">
         <f t="shared" si="16"/>
-        <v>-8.525927317378966E-3</v>
+        <v>-1.8933823750671017E-2</v>
       </c>
       <c r="R19">
         <f t="shared" si="16"/>
-        <v>-4.1717813212786212E-3</v>
+        <v>-1.1565462684387866E-2</v>
       </c>
       <c r="S19">
         <f t="shared" si="16"/>
-        <v>-1.939932037893515E-3</v>
+        <v>-6.7175001756428366E-3</v>
       </c>
       <c r="T19">
         <f t="shared" si="16"/>
-        <v>-8.7217214391544136E-4</v>
+        <v>-3.7727632380365928E-3</v>
       </c>
       <c r="U19">
         <f t="shared" si="16"/>
-        <v>-3.8282478469476883E-4</v>
+        <v>-2.0687456598138965E-3</v>
       </c>
       <c r="V19">
         <f t="shared" si="16"/>
-        <v>-1.6504540802525866E-4</v>
+        <v>-1.1142007803972966E-3</v>
       </c>
       <c r="W19">
         <f t="shared" si="16"/>
-        <v>-7.0170200295259369E-5</v>
+        <v>-5.9178842509872835E-4</v>
       </c>
       <c r="X19">
         <f t="shared" si="16"/>
-        <v>-2.9502761629720941E-5</v>
+        <v>-3.1083530799678224E-4</v>
       </c>
       <c r="Y19">
         <f t="shared" si="16"/>
-        <v>-1.2291796438648167E-5</v>
+        <v>-1.6178453409151881E-4</v>
       </c>
       <c r="Z19">
         <f>Y19*EXP(-Y8)/(1-EXP(-za))-Y14*Y7*EXP(-Y8)/(1-EXP(-za))-Y14*EXP(-Y8)*Z7*EXP(-za)/(1-EXP(-za))^2</f>
-        <v>-8.6056958240602576E-6</v>
+        <v>-1.707844680721562E-4</v>
       </c>
     </row>
     <row r="20" spans="1:26">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20">
-        <f>ro*(reck-phie/phif)/(reck-1)</f>
-        <v>0.83574092291652491</v>
+        <f>B6</f>
+        <v>0.22198504671239971</v>
+      </c>
+      <c r="C20">
+        <f>B7</f>
+        <v>0.22198504671239971</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>58</v>
@@ -11835,88 +11779,92 @@
       </c>
       <c r="H20" s="4">
         <f t="shared" ref="H20:Y21" si="17">G20*EXP(-G$8)+G$14*G6^2*EXP(-G$8)</f>
-        <v>2.263202179062424E-7</v>
+        <v>2.2633025097186959E-7</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="17"/>
-        <v>2.4699843612087686E-5</v>
+        <v>2.470615491904462E-5</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="17"/>
-        <v>2.3093489071255354E-3</v>
+        <v>2.3126351272908935E-3</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="17"/>
-        <v>6.6929154100893076E-2</v>
+        <v>6.7423443752437168E-2</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="17"/>
-        <v>0.17015463926052943</v>
+        <v>0.17440239515920308</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="17"/>
-        <v>0.17443114554952954</v>
+        <v>0.18754249153228519</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="17"/>
-        <v>0.12200381201984517</v>
+        <v>0.14705361274876602</v>
       </c>
       <c r="O20" s="4">
         <f t="shared" si="17"/>
-        <v>6.6836199627665002E-2</v>
+        <v>9.6512972029975996E-2</v>
       </c>
       <c r="P20" s="4">
         <f t="shared" si="17"/>
-        <v>3.239543736645422E-2</v>
+        <v>5.7756850501480363E-2</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="17"/>
-        <v>1.4829926797916936E-2</v>
+        <v>3.293333496460437E-2</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="17"/>
-        <v>6.5763486884156813E-3</v>
+        <v>1.823166400584085E-2</v>
       </c>
       <c r="S20" s="4">
         <f t="shared" si="17"/>
-        <v>2.8552321203523714E-3</v>
+        <v>9.8869557774791152E-3</v>
       </c>
       <c r="T20" s="4">
         <f t="shared" si="17"/>
-        <v>1.2204093601914301E-3</v>
+        <v>5.2791362365872379E-3</v>
       </c>
       <c r="U20" s="4">
         <f t="shared" si="17"/>
-        <v>5.1530021429977335E-4</v>
+        <v>2.784629220607497E-3</v>
       </c>
       <c r="V20" s="4">
         <f t="shared" si="17"/>
-        <v>2.1543990798051862E-4</v>
+        <v>1.454407707991968E-3</v>
       </c>
       <c r="W20" s="4">
         <f t="shared" si="17"/>
-        <v>8.934045945157792E-5</v>
+        <v>7.534630024423341E-4</v>
       </c>
       <c r="X20" s="4">
         <f t="shared" si="17"/>
-        <v>3.6795189100964382E-5</v>
+        <v>3.8766689303676173E-4</v>
       </c>
       <c r="Y20" s="4">
         <f t="shared" si="17"/>
-        <v>1.5065857924913632E-5</v>
+        <v>1.9829671091911057E-4</v>
       </c>
       <c r="Z20" s="4">
         <f>Y20*Y9/oa+2*Y$14*(Y6)*Y$9*sa/oa^2 + 2*Y$14*Y$9*Z6^2*sa^2/oa^3 +Y$14*Y$9*Z6^2*sa/oa^2</f>
-        <v>1.0953107595344321E-5</v>
+        <v>2.3507778626202615E-4</v>
       </c>
     </row>
     <row r="21" spans="1:26">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B21">
-        <f>SUMPRODUCT(lx,fa)</f>
-        <v>0.53468880128210072</v>
+        <f>SUMPRODUCT(fa,G18:Z18)</f>
+        <v>-0.45906729022292792</v>
+      </c>
+      <c r="C21">
+        <f>SUMPRODUCT(fa,G19:Z19)</f>
+        <v>-0.10805055992994111</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>59</v>
@@ -11926,493 +11874,493 @@
       </c>
       <c r="H21" s="4">
         <f t="shared" si="17"/>
-        <v>2.6571009742197889E-8</v>
+        <v>2.6572187669150196E-8</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="17"/>
-        <v>3.6133268908502742E-7</v>
+        <v>3.614250168564176E-7</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="17"/>
-        <v>4.5666752629928879E-6</v>
+        <v>4.5731736748576282E-6</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="17"/>
-        <v>5.1230758309297139E-5</v>
+        <v>5.1609111121509116E-5</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="17"/>
-        <v>4.8228755893305823E-4</v>
+        <v>4.9432742944271915E-4</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="17"/>
-        <v>3.3712216969402293E-3</v>
+        <v>3.6246240002611408E-3</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="17"/>
-        <v>1.1450703807049977E-2</v>
+        <v>1.3801760252121058E-2</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="17"/>
-        <v>1.5361393527762862E-2</v>
+        <v>2.2182196955327207E-2</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="17"/>
-        <v>1.1670413700498431E-2</v>
+        <v>2.0806829423704515E-2</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="17"/>
-        <v>6.8333683336002458E-3</v>
+        <v>1.5175099063778792E-2</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="17"/>
-        <v>3.5239606736938893E-3</v>
+        <v>9.7695043277976762E-3</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="17"/>
-        <v>1.6931353872876313E-3</v>
+        <v>5.8629050086939569E-3</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="17"/>
-        <v>7.7825675424039319E-4</v>
+        <v>3.3665125544717033E-3</v>
       </c>
       <c r="U21" s="4">
         <f t="shared" si="17"/>
-        <v>3.4709606212186838E-4</v>
+        <v>1.8756713273557332E-3</v>
       </c>
       <c r="V21" s="4">
         <f t="shared" si="17"/>
-        <v>1.5145381936711085E-4</v>
+        <v>1.0224456757207112E-3</v>
       </c>
       <c r="W21" s="4">
         <f t="shared" si="17"/>
-        <v>6.4999894290509232E-5</v>
+        <v>5.4818405693453636E-4</v>
       </c>
       <c r="X21" s="4">
         <f t="shared" si="17"/>
-        <v>2.7535959521462325E-5</v>
+        <v>2.9011346687688469E-4</v>
       </c>
       <c r="Y21" s="4">
         <f t="shared" si="17"/>
-        <v>1.1543618845716504E-5</v>
+        <v>1.5193702613006452E-4</v>
       </c>
       <c r="Z21" s="4">
         <f>Y21*EXP(-Y$8)/oa+2*Y$14*(Y7)*Y$9*sa/oa^2 + 2*Y$14*Y$9*Z7^2*sa^2/oa^3 +Y$14*Y$9*Z7^2*sa/oa^2</f>
-        <v>8.7906209267635164E-6</v>
+        <v>1.9309570213210932E-4</v>
       </c>
     </row>
     <row r="22" spans="1:26">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B22">
-        <f>SUMPRODUCT(lz,fa)</f>
-        <v>0.19049426590405846</v>
+        <f>SUMPRODUCT(fa,G20:Z20)</f>
+        <v>0.37916357724459171</v>
+      </c>
+      <c r="C22">
+        <f>SUMPRODUCT(fa,G21:Z21)</f>
+        <v>6.4151354343679051E-2</v>
       </c>
       <c r="F22" t="s">
         <v>44</v>
       </c>
       <c r="G22">
         <f>G11*G18+lz*wa*G6/za*(EXP(-za)-(1-EXP(-za))/za)</f>
-        <v>-1.351063256662056E-6</v>
+        <v>-1.3511021676229991E-6</v>
       </c>
       <c r="H22">
         <f>H11*H18+lz*wa*H6/za*(EXP(-za)-(1-EXP(-za))/za)</f>
-        <v>-7.2894992888035268E-5</v>
+        <v>-7.2908220852422288E-5</v>
       </c>
       <c r="I22">
         <f t="shared" ref="I22:Z22" si="18">I11*I18+lz*wa*I6/za*(EXP(-za)-(1-EXP(-za))/za)</f>
-        <v>-1.5707976497681302E-3</v>
+        <v>-1.5723834448617747E-3</v>
       </c>
       <c r="J22">
         <f t="shared" si="18"/>
-        <v>-1.4882842525571413E-2</v>
+        <v>-1.4958618010957206E-2</v>
       </c>
       <c r="K22">
         <f t="shared" si="18"/>
-        <v>-4.9143527919776026E-2</v>
+        <v>-4.9967175450824283E-2</v>
       </c>
       <c r="L22">
         <f t="shared" si="18"/>
-        <v>-7.6077665574167869E-2</v>
+        <v>-7.9837562757625088E-2</v>
       </c>
       <c r="M22">
         <f t="shared" si="18"/>
-        <v>-7.3615553886919122E-2</v>
+        <v>-8.3521769629464782E-2</v>
       </c>
       <c r="N22">
         <f t="shared" si="18"/>
-        <v>-5.2292532669696266E-2</v>
+        <v>-6.8433306092444343E-2</v>
       </c>
       <c r="O22">
         <f t="shared" si="18"/>
-        <v>-3.0252723434764706E-2</v>
+        <v>-4.8005638308254411E-2</v>
       </c>
       <c r="P22">
         <f t="shared" si="18"/>
-        <v>-1.5640325697411753E-2</v>
+        <v>-3.0737353205787746E-2</v>
       </c>
       <c r="Q22">
         <f t="shared" si="18"/>
-        <v>-7.5936628356970716E-3</v>
+        <v>-1.8597869559807526E-2</v>
       </c>
       <c r="R22">
         <f t="shared" si="18"/>
-        <v>-3.5386020299966784E-3</v>
+        <v>-1.0817934389444351E-2</v>
       </c>
       <c r="S22">
         <f t="shared" si="18"/>
-        <v>-1.6001646646628947E-3</v>
+        <v>-6.1090067244360825E-3</v>
       </c>
       <c r="T22">
         <f t="shared" si="18"/>
-        <v>-7.0695031506876711E-4</v>
+        <v>-3.3709240260312878E-3</v>
       </c>
       <c r="U22">
         <f t="shared" si="18"/>
-        <v>-3.0658406118800507E-4</v>
+        <v>-1.8259510200359498E-3</v>
       </c>
       <c r="V22">
         <f t="shared" si="18"/>
-        <v>-1.3096716374883327E-4</v>
+        <v>-9.7430668628097734E-4</v>
       </c>
       <c r="W22">
         <f t="shared" si="18"/>
-        <v>-5.5257176998548301E-5</v>
+        <v>-5.1348222427088322E-4</v>
       </c>
       <c r="X22">
         <f t="shared" si="18"/>
-        <v>-2.3074720399920117E-5</v>
+        <v>-2.6784527236792493E-4</v>
       </c>
       <c r="Y22">
         <f t="shared" si="18"/>
-        <v>-9.5527013338463728E-6</v>
+        <v>-1.3851294505184516E-4</v>
       </c>
       <c r="Z22">
         <f t="shared" si="18"/>
-        <v>-6.5805158184183618E-6</v>
+        <v>-1.4320132015623009E-4</v>
       </c>
     </row>
     <row r="23" spans="1:26">
       <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="12">
-        <f>B6</f>
-        <v>0.22797681823165919</v>
-      </c>
-      <c r="C23" s="12">
-        <f>B7</f>
-        <v>0.43854729534046094</v>
-      </c>
-      <c r="D23" s="12">
-        <f>AVERAGE(f)</f>
-        <v>0.33326205678606008</v>
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <f>SUMPRODUCT(lz*G11:Z11)</f>
+        <v>0.18542206809774034</v>
+      </c>
+      <c r="C23">
+        <f>SUMPRODUCT(lz*G12:Z12)</f>
+        <v>5.9504294198978319E-2</v>
       </c>
       <c r="F23" t="s">
         <v>45</v>
       </c>
       <c r="G23">
         <f t="shared" ref="G23:Z23" si="19">G12*G19+lz*wa*G7/za*(EXP(-za)-(1-EXP(-za))/za)</f>
-        <v>-4.6293288886808878E-7</v>
+        <v>-4.6294622145149615E-7</v>
       </c>
       <c r="H23">
         <f t="shared" si="19"/>
-        <v>-8.5962270506635169E-6</v>
+        <v>-8.5977872160739734E-6</v>
       </c>
       <c r="I23">
         <f t="shared" si="19"/>
-        <v>-6.7190304347826616E-5</v>
+        <v>-6.7258314844845574E-5</v>
       </c>
       <c r="J23">
         <f t="shared" si="19"/>
-        <v>-3.4600983627406572E-4</v>
+        <v>-3.4782374006835841E-4</v>
       </c>
       <c r="K23">
         <f t="shared" si="19"/>
-        <v>-1.3165723808435028E-3</v>
+        <v>-1.3408226042439292E-3</v>
       </c>
       <c r="L23">
         <f t="shared" si="19"/>
-        <v>-3.9466625077497113E-3</v>
+        <v>-4.1644831208397862E-3</v>
       </c>
       <c r="M23">
         <f t="shared" si="19"/>
-        <v>-8.8194837521140615E-3</v>
+        <v>-1.0106532159143686E-2</v>
       </c>
       <c r="N23">
         <f t="shared" si="19"/>
-        <v>-1.2813432147206696E-2</v>
+        <v>-1.6910781506343009E-2</v>
       </c>
       <c r="O23">
         <f t="shared" si="19"/>
-        <v>-1.1593388416173462E-2</v>
+        <v>-1.8489360112883525E-2</v>
       </c>
       <c r="P23">
         <f t="shared" si="19"/>
-        <v>-7.6578330664297855E-3</v>
+        <v>-1.509505054081791E-2</v>
       </c>
       <c r="Q23">
         <f t="shared" si="19"/>
-        <v>-4.2925456466159839E-3</v>
+        <v>-1.0533620043349963E-2</v>
       </c>
       <c r="R23">
         <f t="shared" si="19"/>
-        <v>-2.1970572077524763E-3</v>
+        <v>-6.7258827884079395E-3</v>
       </c>
       <c r="S23">
         <f t="shared" si="19"/>
-        <v>-1.0618730012603949E-3</v>
+        <v>-4.0580597355787448E-3</v>
       </c>
       <c r="T23">
         <f t="shared" si="19"/>
-        <v>-4.931496816342753E-4</v>
+        <v>-2.3533007902430559E-3</v>
       </c>
       <c r="U23">
         <f t="shared" si="19"/>
-        <v>-2.2236025530383025E-4</v>
+        <v>-1.3251515973265917E-3</v>
       </c>
       <c r="V23">
         <f t="shared" si="19"/>
-        <v>-9.8007051071884432E-5</v>
+        <v>-7.2947315519836134E-4</v>
       </c>
       <c r="W23">
         <f t="shared" si="19"/>
-        <v>-4.2427125554930716E-5</v>
+        <v>-3.9442262574787882E-4</v>
       </c>
       <c r="X23">
         <f t="shared" si="19"/>
-        <v>-1.8101927300924593E-5</v>
+        <v>-2.1019646236210388E-4</v>
       </c>
       <c r="Y23">
         <f t="shared" si="19"/>
-        <v>-7.6319916476483891E-6</v>
+        <v>-1.1069624188159793E-4</v>
       </c>
       <c r="Z23">
         <f t="shared" si="19"/>
-        <v>-5.3865569391583071E-6</v>
+        <v>-1.1769650336303277E-4</v>
       </c>
     </row>
     <row r="24" spans="1:26">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B24">
-        <f>SUMPRODUCT(fa,G18:Z18)</f>
-        <v>-0.362386893582481</v>
+        <f>SUM(G22:Z22)</f>
+        <v>-0.41986710039112274</v>
       </c>
       <c r="C24">
-        <f>SUMPRODUCT(fa,G19:Z19)</f>
-        <v>-6.6984884640302195E-2</v>
+        <f>SUM(G23:Z23)</f>
+        <v>-9.3089672776081822E-2</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" ref="G24:Z24" si="20">G20*G11+2*G18*wa*G6^2*sa/za - 2*G18*wa*G6^2*oa/za^2-lz*wa*G6^3*sa/za -2*lz*wa*G6^3*sa/za^2+2*lz*wa*G6^3*oa/za^3</f>
-        <v>2.6820487945064326E-13</v>
+        <v>2.6821365960263372E-13</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="20"/>
-        <v>2.7041488278855059E-9</v>
+        <v>2.7046776699178183E-9</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" si="20"/>
-        <v>7.6224239744949866E-6</v>
+        <v>7.6307135048239694E-6</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="20"/>
-        <v>3.2356048884670391E-3</v>
+        <v>3.2535327335717068E-3</v>
       </c>
       <c r="K24" s="4">
         <f t="shared" si="20"/>
-        <v>4.7043568514133466E-2</v>
+        <v>4.7896536419774149E-2</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="20"/>
-        <v>0.1063570864726664</v>
+        <v>0.11201928533910005</v>
       </c>
       <c r="M24" s="4">
         <f t="shared" si="20"/>
-        <v>0.11422834028992671</v>
+        <v>0.13075878482792214</v>
       </c>
       <c r="N24" s="4">
         <f t="shared" si="20"/>
-        <v>8.4552282414369684E-2</v>
+        <v>0.11225427887452208</v>
       </c>
       <c r="O24" s="4">
         <f t="shared" si="20"/>
-        <v>5.0129769787905266E-2</v>
+        <v>8.0913212185490982E-2</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" si="20"/>
-        <v>2.6374841411077449E-2</v>
+        <v>5.2770698350747255E-2</v>
       </c>
       <c r="Q24" s="4">
         <f t="shared" si="20"/>
-        <v>1.2971783044834621E-2</v>
+        <v>3.2354234391018748E-2</v>
       </c>
       <c r="R24" s="4">
         <f t="shared" si="20"/>
-        <v>6.1037985544762589E-3</v>
+        <v>1.9006290557755514E-2</v>
       </c>
       <c r="S24" s="4">
         <f t="shared" si="20"/>
-        <v>2.7809900920466339E-3</v>
+        <v>1.0815118517258596E-2</v>
       </c>
       <c r="T24" s="4">
         <f t="shared" si="20"/>
-        <v>1.2360018322783166E-3</v>
+        <v>6.003939506489901E-3</v>
       </c>
       <c r="U24" s="4">
         <f t="shared" si="20"/>
-        <v>5.3862903831874444E-4</v>
+        <v>3.2682238184766968E-3</v>
       </c>
       <c r="V24" s="4">
         <f t="shared" si="20"/>
-        <v>2.31020817678577E-4</v>
+        <v>1.7510080482952503E-3</v>
       </c>
       <c r="W24" s="4">
         <f t="shared" si="20"/>
-        <v>9.7802475633587173E-5</v>
+        <v>9.2599476211197506E-4</v>
       </c>
       <c r="X24" s="4">
         <f t="shared" si="20"/>
-        <v>4.0959493209083775E-5</v>
+        <v>4.8443980722222572E-4</v>
       </c>
       <c r="Y24" s="4">
         <f t="shared" si="20"/>
-        <v>1.6999254859949907E-5</v>
+        <v>2.511571368320585E-4</v>
       </c>
       <c r="Z24" s="4">
         <f t="shared" si="20"/>
-        <v>1.2140638153461183E-5</v>
+        <v>2.8153306857718933E-4</v>
       </c>
     </row>
     <row r="25" spans="1:26">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B25">
-        <f>SUMPRODUCT(fa,G20:Z20)</f>
-        <v>0.29081630442677187</v>
+        <f>SUM(G24:Z24)</f>
+        <v>0.61501590176361709</v>
       </c>
       <c r="C25">
-        <f>SUMPRODUCT(fa,G21:Z21)</f>
-        <v>3.3894497724346107E-2</v>
+        <f>SUM(G25:Z25)</f>
+        <v>0.10561386177572663</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>63</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" ref="G25:Z25" si="21">G21*G12+2*G19*wa*G7^2*sa/za - 2*G19*wa*G7^2*oa/za^2-lz*wa*G7^3*sa/za -2*lz*wa*G7^3*sa/za^2+2*lz*wa*G7^3*oa/za^3</f>
-        <v>1.0789311546921533E-14</v>
+        <v>1.0789664753751024E-14</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="21"/>
-        <v>6.7024905010085787E-12</v>
+        <v>6.7037484417897258E-12</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="21"/>
-        <v>9.9524170097530477E-10</v>
+        <v>9.9627933308531121E-10</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="21"/>
-        <v>8.8799639248318258E-8</v>
+        <v>8.9279109423762603E-8</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="21"/>
-        <v>5.3770678602778078E-6</v>
+        <v>5.4789216992315494E-6</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="21"/>
-        <v>1.989256658720762E-4</v>
+        <v>2.1032071075924178E-4</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="21"/>
-        <v>2.8217595850226537E-3</v>
+        <v>3.2577999171205449E-3</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="21"/>
-        <v>1.0628400095037991E-2</v>
+        <v>1.423591464491402E-2</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="21"/>
-        <v>1.4116387197515567E-2</v>
+        <v>2.2918508741264533E-2</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="21"/>
-        <v>1.0885274835816068E-2</v>
+        <v>2.1859275399896901E-2</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="21"/>
-        <v>6.5650921053046381E-3</v>
+        <v>1.6414783895545553E-2</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="21"/>
-        <v>3.5008900604810546E-3</v>
+        <v>1.0920332690341697E-2</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="21"/>
-        <v>1.7367283179704901E-3</v>
+        <v>6.7630028518707239E-3</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="21"/>
-        <v>8.2125999631027947E-4</v>
+        <v>3.9934997144097893E-3</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="21"/>
-        <v>3.7525000456853851E-4</v>
+        <v>2.2788502372354507E-3</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="21"/>
-        <v>1.6708445630240359E-4</v>
+        <v>1.2673202851302611E-3</v>
       </c>
       <c r="W25" s="4">
         <f t="shared" si="21"/>
-        <v>7.2914648466755174E-5</v>
+        <v>6.9078358413859507E-4</v>
       </c>
       <c r="X25" s="4">
         <f t="shared" si="21"/>
-        <v>3.1313236981166085E-5</v>
+        <v>3.7055030241484944E-4</v>
       </c>
       <c r="Y25" s="4">
         <f t="shared" si="21"/>
-        <v>1.3273450209485325E-5</v>
+        <v>1.9620318067193693E-4</v>
       </c>
       <c r="Z25" s="4">
         <f t="shared" si="21"/>
-        <v>9.8245893298376492E-6</v>
+        <v>2.3114641620998089E-4</v>
       </c>
     </row>
     <row r="26" spans="1:26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B26">
-        <f>SUMPRODUCT(lz*G11:Z11)</f>
-        <v>0.16575450467747987</v>
+        <f>ro/(reck-1)*phie/phif^2*dphif</f>
+        <v>-0.49988254293678641</v>
       </c>
       <c r="C26">
-        <f>SUMPRODUCT(lz*G12:Z12)</f>
-        <v>4.4772431613819379E-2</v>
+        <f>ro/(reck-1)*phie/phif^2*dphif</f>
+        <v>-0.11765723634392143</v>
       </c>
       <c r="G26">
         <f>G20*G11+2*G18*wa*G6^2*sa/za-2*G18*wa*G6^2*oa/za^2-lz*wa*G6^3*sa/za-2*lz*wa*G6^3*sa/za^2+2*lz*wa*G6^3*oa/za^3</f>
-        <v>2.6820487945064326E-13</v>
+        <v>2.6821365960263372E-13</v>
       </c>
     </row>
     <row r="27" spans="1:26">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B27">
-        <f>SUM(G22:Z22)</f>
-        <v>-0.32752161159913296</v>
+        <f>-2*ro*phie*dphif^2/(phif^3*(reck-1)) + ro*phie*ddphif/(phif^2*(reck-1))</f>
+        <v>-1.7594059398940818</v>
       </c>
       <c r="C27">
-        <f>SUM(G23:Z23)</f>
-        <v>-5.5008172016160151E-2</v>
+        <f>-2*ro*phie*dphif^2/(phif^3*(reck-1)) + ro*phie*ddphif/(phif^2*(reck-1))</f>
+        <v>-5.0487019821761264E-2</v>
       </c>
       <c r="G27">
         <f t="shared" ref="G27:Z27" si="22">(G15-2*G14+G16)/dh^2</f>
@@ -12420,7 +12368,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="22"/>
-        <v>-1.1102230246251565E-4</v>
+        <v>1.1102230246251565E-4</v>
       </c>
       <c r="I27">
         <f t="shared" si="22"/>
@@ -12432,81 +12380,70 @@
       </c>
       <c r="K27">
         <f t="shared" si="22"/>
-        <v>8.9039886574937555E-2</v>
+        <v>8.9594998087250133E-2</v>
       </c>
       <c r="L27">
         <f t="shared" si="22"/>
-        <v>0.34836022955175849</v>
+        <v>0.35701996914383471</v>
       </c>
       <c r="M27">
         <f t="shared" si="22"/>
-        <v>0.52025050933934835</v>
+        <v>0.55934423759396168</v>
       </c>
       <c r="N27">
         <f t="shared" si="22"/>
-        <v>0.48284293230338449</v>
+        <v>0.58197197061460315</v>
       </c>
       <c r="O27">
         <f t="shared" si="22"/>
-        <v>0.33048563885529347</v>
+        <v>0.47722242824121963</v>
       </c>
       <c r="P27">
         <f t="shared" si="22"/>
-        <v>0.19232618969633464</v>
+        <v>0.34288891170852764</v>
       </c>
       <c r="Q27">
         <f t="shared" si="22"/>
-        <v>0.10279450901595766</v>
+        <v>0.22827659901247799</v>
       </c>
       <c r="R27">
         <f t="shared" si="22"/>
-        <v>5.2135921448093203E-2</v>
+        <v>0.1445345579331736</v>
       </c>
       <c r="S27">
         <f t="shared" si="22"/>
-        <v>2.5482708391338926E-2</v>
+        <v>8.8239311690774258E-2</v>
       </c>
       <c r="T27">
         <f t="shared" si="22"/>
-        <v>1.2109698009979408E-2</v>
+        <v>5.2382902702985401E-2</v>
       </c>
       <c r="U27">
         <f t="shared" si="22"/>
-        <v>5.6275174949681206E-3</v>
+        <v>3.0410515685502792E-2</v>
       </c>
       <c r="V27">
         <f t="shared" si="22"/>
-        <v>2.5679159048729722E-3</v>
+        <v>1.7335633796522476E-2</v>
       </c>
       <c r="W27">
         <f t="shared" si="22"/>
-        <v>1.1541154249189271E-3</v>
+        <v>9.7333572408528357E-3</v>
       </c>
       <c r="X27">
         <f t="shared" si="22"/>
-        <v>5.1208350914148069E-4</v>
+        <v>5.3952068507223672E-3</v>
       </c>
       <c r="Y27">
         <f t="shared" si="22"/>
-        <v>2.2472631123603842E-4</v>
+        <v>2.9578373577461223E-3</v>
       </c>
       <c r="Z27">
         <f t="shared" si="22"/>
-        <v>1.7104538644556033E-4</v>
+        <v>3.4507986745868635E-3</v>
       </c>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28">
-        <f>SUM(G24:Z24)</f>
-        <v>0.4559592441484267</v>
-      </c>
-      <c r="C28">
-        <f>SUM(G25:Z25)</f>
-        <v>5.1949845114643525E-2</v>
-      </c>
       <c r="F28" t="s">
         <v>30</v>
       </c>
@@ -12519,293 +12456,298 @@
     </row>
     <row r="29" spans="1:26">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B29">
-        <f>ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-0.48541933428342954</v>
+        <f>f*re*phiq</f>
+        <v>3.5433152126493957E-2</v>
       </c>
       <c r="C29">
-        <f>ro/(reck-1)*phie/phif^2*dphif</f>
-        <v>-8.9726639359673954E-2</v>
+        <f>f*re*phiq</f>
+        <v>1.1370948076259458E-2</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <f>B32</f>
-        <v>3.1581132259519119E-2</v>
+        <f>B29</f>
+        <v>3.5433152126493957E-2</v>
       </c>
       <c r="H29">
-        <f>B33</f>
-        <v>5.7782159919073532E-2</v>
+        <f>B30</f>
+        <v>5.8809589317839361E-2</v>
       </c>
     </row>
     <row r="30" spans="1:26">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B30">
-        <f>-2*ro*phie*dphif^2/(phif^3*(reck-1)) + ro*phie*ddphif/(phif^2*(reck-1))</f>
-        <v>-1.4573254703034795</v>
+        <f>re*phiq+f*phiq*dre+f*re*dphiq</f>
+        <v>5.8809589317839361E-2</v>
       </c>
       <c r="C30">
-        <f>-2*ro*phie*dphif^2/(phif^3*(reck-1)) + ro*phie*ddphif/(phif^2*(reck-1))</f>
-        <v>-1.7700586776129748E-2</v>
+        <f>re*phiq+f*phiq*dre+f*re*dphiq</f>
+        <v>3.1880863347572175E-2</v>
       </c>
       <c r="F30">
         <v>0.2</v>
       </c>
       <c r="G30">
         <f t="dataTable" ref="G30:H56" dt2D="0" dtr="0" r1="B6"/>
-        <v>2.9728945043416319E-2</v>
+        <v>3.396599399742567E-2</v>
       </c>
       <c r="H30">
-        <v>7.1462787155911506E-2</v>
+        <v>7.1383047929654275E-2</v>
       </c>
       <c r="Z30" s="4">
         <f>Y30*EXP(-Y$8)/oa+Y$14*(Y16)^2*Y$9/oa + 2*Y$14*Y16*Y$9*Z16*sa/oa^2 + 2*Y$14*Y$9*Z16^2*sa/oa^3 + Y$14*Y$9*Z16^2*sa/oa^2</f>
-        <v>2.0485003961974628E-18</v>
+        <v>1.5666197587887692E-14</v>
       </c>
     </row>
     <row r="31" spans="1:26">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31">
+        <f>ak*SUM(dYe)</f>
+        <v>3.6276181066164613E-2</v>
+      </c>
+      <c r="C31">
+        <f>ak*SUM(dYe)</f>
+        <v>5.4414271599246923E-2</v>
+      </c>
       <c r="F31">
         <v>0.20499999999999999</v>
       </c>
       <c r="G31">
-        <v>3.0088097988063205E-2</v>
+        <v>3.4323950787470199E-2</v>
       </c>
       <c r="H31">
-        <v>6.8877970021831769E-2</v>
+        <v>6.8379210345511768E-2</v>
       </c>
     </row>
     <row r="32" spans="1:26">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B32">
-        <f>f*re*phiq</f>
-        <v>3.1581132259519119E-2</v>
+        <f>ak*SUM(B40,C41)</f>
+        <v>-0.36794595232515442</v>
       </c>
       <c r="C32">
-        <f>f*re*phiq</f>
-        <v>1.6409629934309552E-2</v>
-      </c>
-      <c r="D32">
-        <f>SUM(Ye)</f>
-        <v>4.7990762193828668E-2</v>
+        <f>ak*SUM(C40,B41)</f>
+        <v>0.12626113602840591</v>
       </c>
       <c r="F32">
         <v>0.21</v>
       </c>
       <c r="G32">
-        <v>3.0434645064195558E-2</v>
+        <v>3.4667272742697236E-2</v>
       </c>
       <c r="H32">
-        <v>6.6356092205559297E-2</v>
+        <v>6.5462682818601667E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>53</v>
-      </c>
       <c r="B33">
-        <f>re*phiq+f*phiq*dre+f*re*dphiq</f>
-        <v>5.7782159919073532E-2</v>
+        <f>ak*SUM(B41,C40)</f>
+        <v>8.4174090685603956E-2</v>
       </c>
       <c r="C33">
-        <f>re*phiq+f*phiq*dre+f*re*dphiq</f>
-        <v>1.5495235300800877E-2</v>
-      </c>
-      <c r="D33">
-        <f>SUM(dYe)</f>
-        <v>7.3277395219874406E-2</v>
+        <f>ak*SUM(B40,C41)</f>
+        <v>-0.55191892848773161</v>
       </c>
       <c r="F33">
         <v>0.215</v>
       </c>
       <c r="G33">
-        <v>3.0768894423796635E-2</v>
+        <v>3.4996386723931183E-2</v>
       </c>
       <c r="H33">
-        <v>6.3895377632580366E-2</v>
+        <v>6.2630471888328279E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34">
+        <f t="array" ref="B34:C35">-MINVERSE(B32:C33)</f>
+        <v>2.8678797680402006</v>
+      </c>
+      <c r="C34">
+        <v>0.65607780203843102</v>
+      </c>
       <c r="F34">
         <v>0.22</v>
       </c>
       <c r="G34">
-        <v>3.1091145488381478E-2</v>
+        <v>3.5311704929879839E-2</v>
       </c>
       <c r="H34">
-        <v>6.1494106794718249E-2</v>
+        <v>5.9879701928461246E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8">
+      <c r="B35">
+        <v>0.43738520135895415</v>
+      </c>
+      <c r="C35">
+        <v>1.9119198453601338</v>
+      </c>
       <c r="F35">
         <v>0.22500000000000001</v>
       </c>
       <c r="G35">
-        <v>3.1401689226700294E-2</v>
+        <v>3.5613625472981032E-2</v>
       </c>
       <c r="H35">
-        <v>5.9150614724936372E-2</v>
+        <v>5.7207609873364235E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="B36">
-        <f>2*dre*phiq+2*re*dphiq+f*ddre*phiq+2*f*dre*dphiq+f*re*ddphiq</f>
-        <v>-0.60407334583573657</v>
+        <f t="array" ref="B36:C36">MMULT(B31:C31,B34:C35)</f>
+        <v>0.12783572288165393</v>
       </c>
       <c r="C36">
-        <f>f*B30*phiq+2*f*B29*B27+f*re*B28</f>
-        <v>0.27794532903742164</v>
-      </c>
-      <c r="D36">
-        <f>B38+C39</f>
-        <v>15.729091608614045</v>
+        <v>0.12783572288165393</v>
       </c>
       <c r="F36">
         <v>0.23</v>
       </c>
       <c r="G36">
-        <v>3.1700808422519294E-2</v>
+        <v>3.5902532929549182E-2</v>
       </c>
       <c r="H36">
-        <v>5.6863289053074514E-2</v>
+        <v>5.46115402095253E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="B37">
-        <f>f*C30*phiq+2*f*C29*C27+f*re*C28</f>
-        <v>1.1479557547755303E-2</v>
-      </c>
-      <c r="C37">
-        <f>2*dre*phiq+2*re*dphiq+f*ddre*phiq+2*f*dre*dphiq+f*re*ddphiq</f>
-        <v>-7.695795661213492E-2</v>
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="7">
+        <f>f+fstp</f>
+        <v>0.34982076959405362</v>
+      </c>
+      <c r="C37" s="7">
+        <f>f+fstp</f>
+        <v>0.34982076959405362</v>
       </c>
       <c r="F37">
         <v>0.23499999999999999</v>
       </c>
       <c r="G37">
-        <v>3.1988777932875356E-2</v>
+        <v>3.6178798865511438E-2</v>
       </c>
       <c r="H37">
-        <v>5.4630568138937297E-2</v>
+        <v>5.2088940217553781E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38">
-        <f t="array" ref="B38:C39">-MINVERSE(B36:C37)</f>
-        <v>1.7774201350409577</v>
-      </c>
-      <c r="C38">
-        <v>6.4194223186247932</v>
-      </c>
       <c r="F38">
         <v>0.24</v>
       </c>
       <c r="G38">
-        <v>3.2265864937181622E-2</v>
+        <v>3.6442782338949993E-2</v>
       </c>
       <c r="H38">
-        <v>5.2450939279322262E-2</v>
+        <v>4.9637355450713225E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39">
-        <v>0.26513173718446059</v>
-      </c>
-      <c r="C39">
-        <v>13.951671473573088</v>
-      </c>
       <c r="F39">
         <v>0.245</v>
       </c>
       <c r="G39">
-        <v>3.2532329177546865E-2</v>
+        <v>3.6694830380600771E-2</v>
       </c>
       <c r="H39">
-        <v>5.0322936985746705E-2</v>
+        <v>4.7254425436918768E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <f>2*dre*phiq+2*re*dphiq+f*ddre*phiq+2*f*dre*dphiq+f*re*ddphiq</f>
+        <v>-0.76996922606580975</v>
+      </c>
+      <c r="C40">
+        <f>f*B27*phiq+2*f*B26*B24+f*re*B25</f>
+        <v>0.18746842318667006</v>
+      </c>
       <c r="F40">
         <v>0.25</v>
       </c>
       <c r="G40">
-        <v>3.2788423190653067E-2</v>
+        <v>3.6935278453394414E-2</v>
       </c>
       <c r="H40">
-        <v>4.8245141329782623E-2</v>
+        <v>4.4937879591918667E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>65</v>
-      </c>
       <c r="B41">
-        <f t="array" ref="B41:C41">MMULT(B33:C33,B38:C39)</f>
-        <v>0.10681145313970121</v>
+        <f>f*C27*phiq+2*f*C26*C24+f*re*C25</f>
+        <v>2.2966803527339808E-2</v>
       </c>
       <c r="C41">
-        <v>0.58711251932533393</v>
-      </c>
-      <c r="D41">
-        <f>D33/D36</f>
-        <v>4.6587175561838548E-3</v>
+        <f>2*dre*phiq+2*re*dphiq+f*ddre*phiq+2*f*dre*dphiq+f*re*ddphiq</f>
+        <v>-0.14989565474707625</v>
       </c>
       <c r="F41">
         <v>0.255</v>
       </c>
       <c r="G41">
-        <v>3.3034392531522891E-2</v>
+        <v>3.7164450892066443E-2</v>
       </c>
       <c r="H41">
-        <v>4.6216176353063215E-2</v>
+        <v>4.268553333212545E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="5">
-        <f>(f+dta)/plambda</f>
-        <v>0.44055567662738998</v>
-      </c>
-      <c r="C42" s="5">
-        <f>(f+dta)/plambda</f>
-        <v>0.70163001270104941</v>
-      </c>
-      <c r="D42" s="12">
-        <v>0.3</v>
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <f t="array" ref="B42:C43">-MINVERSE(B40:C41)</f>
+        <v>1.3490805656911284</v>
+      </c>
+      <c r="C42">
+        <v>1.6872404128634673</v>
       </c>
       <c r="F42">
         <v>0.26</v>
       </c>
       <c r="G42">
-        <v>3.3270475989492503E-2</v>
+        <v>3.7382661323807589E-2</v>
       </c>
       <c r="H42">
-        <v>4.4234708539159104E-2</v>
+        <v>4.049528437625427E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8">
+      <c r="B43">
+        <v>0.20670424601074</v>
+      </c>
+      <c r="C43">
+        <v>6.9298240887525395</v>
+      </c>
       <c r="F43">
         <v>0.26500000000000001</v>
       </c>
       <c r="G43">
-        <v>3.349690579669299E-2</v>
+        <v>3.7590213070872514E-2</v>
       </c>
       <c r="H43">
-        <v>4.229944534466093E-2</v>
+        <v>3.8365109225574859E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -12813,32 +12755,53 @@
         <v>0.27</v>
       </c>
       <c r="G44">
-        <v>3.3713907829329766E-2</v>
+        <v>3.7787399536015807E-2</v>
       </c>
       <c r="H44">
-        <v>4.0409133786927579E-2</v>
+        <v>3.6293059813189837E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45">
+        <f t="array" ref="B45:C45">MMULT(B30:C30,B42:C43)</f>
+        <v>8.5928783845405005E-2</v>
+      </c>
+      <c r="C45">
+        <v>0.32015469055719581</v>
+      </c>
       <c r="F45">
         <v>0.27500000000000002</v>
       </c>
       <c r="G45">
-        <v>3.3921701802037033E-2</v>
+        <v>3.7974504571577639E-2</v>
       </c>
       <c r="H45">
-        <v>3.8562559086080445E-2</v>
+        <v>3.4277260313317195E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8">
+      <c r="A46" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="5">
+        <f>f+dta</f>
+        <v>0.30791383055780475</v>
+      </c>
+      <c r="C46" s="5">
+        <f>f+dta</f>
+        <v>0.54213973726959552</v>
+      </c>
       <c r="F46">
         <v>0.28000000000000003</v>
       </c>
       <c r="G46">
-        <v>3.4120501455573091E-2</v>
+        <v>3.8151802832997433E-2</v>
       </c>
       <c r="H46">
-        <v>3.6758543358937024E-2</v>
+        <v>3.231590410208561E-2</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -12846,10 +12809,10 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="G47">
-        <v>3.4310514738110358E-2</v>
+        <v>3.8319560117493628E-2</v>
       </c>
       <c r="H47">
-        <v>3.4995944362686993E-2</v>
+        <v>3.0407250861850033E-2</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -12857,10 +12820,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G48">
-        <v>3.4491943980363461E-2</v>
+        <v>3.8478033688606916E-2</v>
       </c>
       <c r="H48">
-        <v>3.327365428621161E-2</v>
+        <v>2.8549623821491871E-2</v>
       </c>
     </row>
     <row r="49" spans="6:8">
@@ -12868,10 +12831,10 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="G49">
-        <v>3.4664986064789204E-2</v>
+        <v>3.8627472587270451E-2</v>
       </c>
       <c r="H49">
-        <v>3.1590598587050794E-2</v>
+        <v>2.6741407125614014E-2</v>
       </c>
     </row>
     <row r="50" spans="6:8">
@@ -12879,10 +12842,10 @@
         <v>0.29999999999999899</v>
       </c>
       <c r="G50">
-        <v>3.4829832589080748E-2</v>
+        <v>3.8768117930033361E-2</v>
       </c>
       <c r="H50">
-        <v>2.9945734872107832E-2</v>
+        <v>2.4981043325937619E-2</v>
       </c>
     </row>
     <row r="51" spans="6:8">
@@ -12890,10 +12853,10 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="G51">
-        <v>3.4986670024171475E-2</v>
+        <v>3.890020319503365E-2</v>
       </c>
       <c r="H51">
-        <v>2.8338051820272395E-2</v>
+        <v>2.3267030988595186E-2</v>
       </c>
     </row>
     <row r="52" spans="6:8">
@@ -12901,10 +12864,10 @@
         <v>0.309999999999999</v>
       </c>
       <c r="G52">
-        <v>3.5135679866952117E-2</v>
+        <v>3.9023954496283736E-2</v>
       </c>
       <c r="H52">
-        <v>2.6766568145231151E-2</v>
+        <v>2.1597922411378256E-2</v>
       </c>
     </row>
     <row r="53" spans="6:8">
@@ -12912,10 +12875,10 @@
         <v>0.314999999999999</v>
       </c>
       <c r="G53">
-        <v>3.5277038787899902E-2</v>
+        <v>3.9139590846805981E-2</v>
       </c>
       <c r="H53">
-        <v>2.5230331596796343E-2</v>
+        <v>1.9972321445313468E-2</v>
       </c>
     </row>
     <row r="54" spans="6:8">
@@ -12923,10 +12886,10 @@
         <v>0.31999999999999901</v>
       </c>
       <c r="G54">
-        <v>3.5410918773806331E-2</v>
+        <v>3.9247324411124863E-2</v>
       </c>
       <c r="H54">
-        <v>2.372841799918525E-2</v>
+        <v>1.8388881415288605E-2</v>
       </c>
     </row>
     <row r="55" spans="6:8">
@@ -12934,10 +12897,10 @@
         <v>0.32499999999999901</v>
       </c>
       <c r="G55">
-        <v>3.5537487265785789E-2</v>
+        <v>3.9347360747599217E-2</v>
       </c>
       <c r="H55">
-        <v>2.2259930324726993E-2</v>
+        <v>1.6846303134711638E-2</v>
       </c>
     </row>
     <row r="56" spans="6:8">
@@ -12945,14 +12908,15 @@
         <v>0.32999999999999902</v>
       </c>
       <c r="G56">
-        <v>3.5656907292738405E-2</v>
+        <v>3.943989904105287E-2</v>
       </c>
       <c r="H56">
-        <v>2.0823997801561314E-2</v>
+        <v>1.5343333009489327E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -12967,8 +12931,8 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13429,7 +13393,7 @@
       </c>
       <c r="C6">
         <f>fbar*lambda</f>
-        <v>0.37946351321637939</v>
+        <v>0.2406542626817135</v>
       </c>
       <c r="D6">
         <f>B6-dh</f>
@@ -14099,11 +14063,11 @@
       </c>
       <c r="B13">
         <f>fbar*B12</f>
-        <v>0.23717695342339751</v>
+        <v>0.15041668793767735</v>
       </c>
       <c r="C13">
         <f>fbar*C12</f>
-        <v>0.36282304657660247</v>
+        <v>0.23010094440367487</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -14216,79 +14180,79 @@
       </c>
       <c r="H15">
         <f t="shared" ref="H15:Y15" si="12">G15*EXP(-m-SUMPRODUCT(G$6:G$7,$C$6:$C$7))</f>
-        <v>0.68080136505630007</v>
+        <v>0.69826098198545472</v>
       </c>
       <c r="I15">
         <f t="shared" si="12"/>
-        <v>0.44669899956876574</v>
+        <v>0.47558179975962273</v>
       </c>
       <c r="J15">
         <f t="shared" si="12"/>
-        <v>0.27990281760651814</v>
+        <v>0.31403439169594038</v>
       </c>
       <c r="K15">
         <f t="shared" si="12"/>
-        <v>0.16648696920521339</v>
+        <v>0.20021298266431431</v>
       </c>
       <c r="L15">
         <f t="shared" si="12"/>
-        <v>9.3937128541513343E-2</v>
+        <v>0.12316112979027531</v>
       </c>
       <c r="M15">
         <f t="shared" si="12"/>
-        <v>5.0517020356753622E-2</v>
+        <v>7.3306977315344218E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="12"/>
-        <v>2.6103532061830009E-2</v>
+        <v>4.2432009144946999E-2</v>
       </c>
       <c r="O15">
         <f t="shared" si="12"/>
-        <v>1.3075570212301551E-2</v>
+        <v>2.4018894201588266E-2</v>
       </c>
       <c r="P15">
         <f t="shared" si="12"/>
-        <v>6.3991056834971655E-3</v>
+        <v>1.3363576524415293E-2</v>
       </c>
       <c r="Q15">
         <f t="shared" si="12"/>
-        <v>3.0786302741873557E-3</v>
+        <v>7.3381405177668935E-3</v>
       </c>
       <c r="R15">
         <f t="shared" si="12"/>
-        <v>1.4627581655266369E-3</v>
+        <v>3.9894961427511108E-3</v>
       </c>
       <c r="S15">
         <f t="shared" si="12"/>
-        <v>6.8867731363111138E-4</v>
+        <v>2.1525889388133487E-3</v>
       </c>
       <c r="T15">
         <f t="shared" si="12"/>
-        <v>3.2206046849402091E-4</v>
+        <v>1.1547939545046859E-3</v>
       </c>
       <c r="U15">
         <f t="shared" si="12"/>
-        <v>1.4986513504731071E-4</v>
+        <v>6.168056024502454E-4</v>
       </c>
       <c r="V15">
         <f t="shared" si="12"/>
-        <v>6.948063275876973E-5</v>
+        <v>3.2835995862759231E-4</v>
       </c>
       <c r="W15">
         <f t="shared" si="12"/>
-        <v>3.2124622987969866E-5</v>
+        <v>1.7436507406295052E-4</v>
       </c>
       <c r="X15">
         <f t="shared" si="12"/>
-        <v>1.4822707042927862E-5</v>
+        <v>9.2415023540416322E-5</v>
       </c>
       <c r="Y15">
         <f t="shared" si="12"/>
-        <v>6.8290107710563044E-6</v>
+        <v>4.8910490769615902E-5</v>
       </c>
       <c r="Z15">
         <f>Y15*EXP(-m-SUMPRODUCT(Y$6:Y$7,$C$6:$C$7))/(1-EXP(-m-SUMPRODUCT(C$6:C$7,Z6:Z7)))</f>
-        <v>5.817607249002134E-6</v>
+        <v>5.481196605646795E-5</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -14393,79 +14357,79 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" ref="H17:Z17" si="14">(H15-H14)/dh</f>
-        <v>-3560.808427235806</v>
+        <v>-1814.8467343203411</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="14"/>
-        <v>-6005.4950901339989</v>
+        <v>-3117.2150710483011</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="14"/>
-        <v>-7296.4422865455726</v>
+        <v>-3883.2848776033488</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="14"/>
-        <v>-7487.5115916825271</v>
+        <v>-4114.9102457724348</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="14"/>
-        <v>-6812.2051150256821</v>
+        <v>-3889.8049901494851</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="14"/>
-        <v>-5638.9025977510137</v>
+        <v>-3359.906901891954</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="14"/>
-        <v>-4331.7711888779431</v>
+        <v>-2698.9234805662445</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="14"/>
-        <v>-3140.3491805170656</v>
+        <v>-2046.0167815883945</v>
       </c>
       <c r="P17" s="3">
         <f t="shared" si="14"/>
-        <v>-2178.322205241629</v>
+        <v>-1481.8751211498161</v>
       </c>
       <c r="Q17" s="3">
         <f t="shared" si="14"/>
-        <v>-1461.5471585824469</v>
+        <v>-1035.5961342244932</v>
       </c>
       <c r="R17" s="3">
         <f t="shared" si="14"/>
-        <v>-956.41909487165321</v>
+        <v>-703.74529714920584</v>
       </c>
       <c r="S17" s="3">
         <f t="shared" si="14"/>
-        <v>-614.23355173323989</v>
+        <v>-467.84238921501617</v>
       </c>
       <c r="T17" s="3">
         <f t="shared" si="14"/>
-        <v>-388.94969601867587</v>
+        <v>-305.67634741760935</v>
       </c>
       <c r="U17" s="3">
         <f t="shared" si="14"/>
-        <v>-243.69361623443763</v>
+        <v>-196.9995694941442</v>
       </c>
       <c r="V17" s="3">
         <f t="shared" si="14"/>
-        <v>-151.46890471030983</v>
+        <v>-125.58097212342756</v>
       </c>
       <c r="W17" s="3">
         <f t="shared" si="14"/>
-        <v>-93.580845637081708</v>
+        <v>-79.356800529583637</v>
       </c>
       <c r="X17" s="3">
         <f t="shared" si="14"/>
-        <v>-57.554430442007266</v>
+        <v>-49.795198792258411</v>
       </c>
       <c r="Y17" s="3">
         <f>(Y15-Y14)/dh</f>
-        <v>-35.276400027663854</v>
+        <v>-31.068252027807894</v>
       </c>
       <c r="Z17" s="3">
         <f t="shared" si="14"/>
-        <v>-55.234621921905088</v>
+        <v>-50.335186041158501</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -15260,11 +15224,11 @@
       </c>
       <c r="Y27">
         <f>(Y15-2*Y14+Y16)/dh^2</f>
-        <v>-3527129.9349776707</v>
+        <v>-3106315.1349920747</v>
       </c>
       <c r="Z27">
         <f>(Z15-2*Z14+Z16)/dh^2</f>
-        <v>-5522528.1094698934</v>
+        <v>-5032584.5213952344</v>
       </c>
     </row>
     <row r="28" spans="1:26">

</xml_diff>

<commit_message>
added documentation and questions to msy.hpp
</commit_message>
<xml_diff>
--- a/examples/MSF.xlsx
+++ b/examples/MSF.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-30540" yWindow="0" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4791,11 +4791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142774472"/>
-        <c:axId val="2142775880"/>
+        <c:axId val="-2094691576"/>
+        <c:axId val="-2094688552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142774472"/>
+        <c:axId val="-2094691576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4804,7 +4804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142775880"/>
+        <c:crossAx val="-2094688552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4812,7 +4812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142775880"/>
+        <c:axId val="-2094688552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4823,14 +4823,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142774472"/>
+        <c:crossAx val="-2094691576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5117,11 +5116,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137736984"/>
-        <c:axId val="-2137734008"/>
+        <c:axId val="-2094662408"/>
+        <c:axId val="-2094659432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137736984"/>
+        <c:axId val="-2094662408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5130,7 +5129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137734008"/>
+        <c:crossAx val="-2094659432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5138,7 +5137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137734008"/>
+        <c:axId val="-2094659432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5149,7 +5148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137736984"/>
+        <c:crossAx val="-2094662408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5355,11 +5354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142859016"/>
-        <c:axId val="2142861992"/>
+        <c:axId val="-2094603672"/>
+        <c:axId val="-2094600696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142859016"/>
+        <c:axId val="-2094603672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5368,7 +5367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142861992"/>
+        <c:crossAx val="-2094600696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5376,7 +5375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142861992"/>
+        <c:axId val="-2094600696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5387,14 +5386,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142859016"/>
+        <c:crossAx val="-2094603672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5687,8 +5685,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142909752"/>
-        <c:axId val="2142912744"/>
+        <c:axId val="-2094553160"/>
+        <c:axId val="-2094550168"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -5951,11 +5949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142919080"/>
-        <c:axId val="2142915784"/>
+        <c:axId val="-2094543832"/>
+        <c:axId val="-2094547128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142909752"/>
+        <c:axId val="-2094553160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5965,12 +5963,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142912744"/>
+        <c:crossAx val="-2094550168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142912744"/>
+        <c:axId val="-2094550168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5981,12 +5979,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142909752"/>
+        <c:crossAx val="-2094553160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142915784"/>
+        <c:axId val="-2094547128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -5998,12 +5996,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142919080"/>
+        <c:crossAx val="-2094543832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142919080"/>
+        <c:axId val="-2094543832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6013,7 +6011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142915784"/>
+        <c:crossAx val="-2094547128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6312,8 +6310,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142971976"/>
-        <c:axId val="2142974968"/>
+        <c:axId val="-2094491704"/>
+        <c:axId val="-2094488712"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -6576,11 +6574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142981304"/>
-        <c:axId val="2142978008"/>
+        <c:axId val="-2094482376"/>
+        <c:axId val="-2094485672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142971976"/>
+        <c:axId val="-2094491704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6590,12 +6588,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142974968"/>
+        <c:crossAx val="-2094488712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142974968"/>
+        <c:axId val="-2094488712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6606,12 +6604,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142971976"/>
+        <c:crossAx val="-2094491704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142978008"/>
+        <c:axId val="-2094485672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -6623,12 +6621,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142981304"/>
+        <c:crossAx val="-2094482376"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142981304"/>
+        <c:axId val="-2094482376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6638,7 +6636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142978008"/>
+        <c:crossAx val="-2094485672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10116,10 +10114,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <selection pane="topRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>